<commit_message>
Code updated 23-04-10 06:33:58
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G111"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>04-08_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>04-09_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>04-09_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,7 +462,13 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -483,7 +499,13 @@
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -514,7 +536,13 @@
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -545,7 +573,13 @@
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="G5" t="n">
+        <v>4956</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>4956</t>
         </is>
@@ -576,7 +610,13 @@
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="G6" t="n">
+        <v>2742</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
         <is>
           <t>2742</t>
         </is>
@@ -607,7 +647,13 @@
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -638,7 +684,13 @@
       <c r="F8" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="G8" t="n">
+        <v>4975</v>
+      </c>
+      <c r="H8" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="I8" t="inlineStr">
         <is>
           <t>4975</t>
         </is>
@@ -669,7 +721,13 @@
       <c r="F9" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" t="n">
+        <v>4769</v>
+      </c>
+      <c r="H9" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>4769</t>
         </is>
@@ -700,7 +758,13 @@
       <c r="F10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -731,7 +795,13 @@
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" t="n">
+        <v>2813</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>2813</t>
         </is>
@@ -762,7 +832,13 @@
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" t="n">
+        <v>1824</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>1824</t>
         </is>
@@ -793,7 +869,13 @@
       <c r="F13" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>4198</v>
+      </c>
+      <c r="H13" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>4198</t>
         </is>
@@ -824,7 +906,13 @@
       <c r="F14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -855,7 +943,13 @@
       <c r="F15" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G15" t="n">
+        <v>4621</v>
+      </c>
+      <c r="H15" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="I15" t="inlineStr">
         <is>
           <t>4621</t>
         </is>
@@ -886,7 +980,13 @@
       <c r="F16" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="G16" t="n">
+        <v>6537</v>
+      </c>
+      <c r="H16" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I16" t="inlineStr">
         <is>
           <t>6537</t>
         </is>
@@ -917,7 +1017,13 @@
       <c r="F17" s="3" t="n">
         <v>37</v>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G17" t="n">
+        <v>5402</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="I17" t="inlineStr">
         <is>
           <t>5402</t>
         </is>
@@ -948,7 +1054,13 @@
       <c r="F18" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="G18" t="n">
+        <v>5602</v>
+      </c>
+      <c r="H18" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="I18" t="inlineStr">
         <is>
           <t>5602</t>
         </is>
@@ -979,7 +1091,13 @@
       <c r="F19" s="5" t="n">
         <v>22</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="n">
+        <v>6503</v>
+      </c>
+      <c r="H19" s="5" t="n">
+        <v>22</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>6503</t>
         </is>
@@ -1010,7 +1128,13 @@
       <c r="F20" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="G20" t="n">
+        <v>5665</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>5665</t>
         </is>
@@ -1041,7 +1165,13 @@
       <c r="F21" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="G21" t="n">
+        <v>6176</v>
+      </c>
+      <c r="H21" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="I21" t="inlineStr">
         <is>
           <t>6176</t>
         </is>
@@ -1072,7 +1202,13 @@
       <c r="F22" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="G22" t="n">
+        <v>5494</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="I22" t="inlineStr">
         <is>
           <t>5494</t>
         </is>
@@ -1103,7 +1239,13 @@
       <c r="F23" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="G23" t="n">
+        <v>4041</v>
+      </c>
+      <c r="H23" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I23" t="inlineStr">
         <is>
           <t>4041</t>
         </is>
@@ -1134,7 +1276,13 @@
       <c r="F24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="G24" t="n">
+        <v>4237</v>
+      </c>
+      <c r="H24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="inlineStr">
         <is>
           <t>4237</t>
         </is>
@@ -1165,7 +1313,13 @@
       <c r="F25" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="G25" t="n">
+        <v>5041</v>
+      </c>
+      <c r="H25" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I25" t="inlineStr">
         <is>
           <t>5041</t>
         </is>
@@ -1196,7 +1350,13 @@
       <c r="F26" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="G26" t="n">
+        <v>5579</v>
+      </c>
+      <c r="H26" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I26" t="inlineStr">
         <is>
           <t>5579</t>
         </is>
@@ -1227,7 +1387,13 @@
       <c r="F27" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" t="n">
+        <v>4934</v>
+      </c>
+      <c r="H27" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>4934</t>
         </is>
@@ -1258,7 +1424,13 @@
       <c r="F28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="G28" t="n">
+        <v>5732</v>
+      </c>
+      <c r="H28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="inlineStr">
         <is>
           <t>5732</t>
         </is>
@@ -1289,7 +1461,13 @@
       <c r="F29" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G29" t="n">
+        <v>5363</v>
+      </c>
+      <c r="H29" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>5363</t>
         </is>
@@ -1320,7 +1498,13 @@
       <c r="F30" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="n">
+        <v>4610</v>
+      </c>
+      <c r="H30" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>4610</t>
         </is>
@@ -1351,7 +1535,13 @@
       <c r="F31" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="G31" t="n">
+        <v>5176</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>5176</t>
         </is>
@@ -1382,7 +1572,13 @@
       <c r="F32" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="G32" t="n">
+        <v>4803</v>
+      </c>
+      <c r="H32" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>4803</t>
         </is>
@@ -1413,7 +1609,13 @@
       <c r="F33" s="5" t="n">
         <v>21</v>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="G33" t="n">
+        <v>6303</v>
+      </c>
+      <c r="H33" s="5" t="n">
+        <v>21</v>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>6303</t>
         </is>
@@ -1444,7 +1646,13 @@
       <c r="F34" s="5" t="n">
         <v>29</v>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" t="n">
+        <v>6095</v>
+      </c>
+      <c r="H34" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>6095</t>
         </is>
@@ -1475,7 +1683,13 @@
       <c r="F35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="G35" t="n">
+        <v>4689</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>4689</t>
         </is>
@@ -1506,7 +1720,13 @@
       <c r="F36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="G36" t="n">
+        <v>3532</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>3532</t>
         </is>
@@ -1537,7 +1757,13 @@
       <c r="F37" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="G37" t="n">
+        <v>5973</v>
+      </c>
+      <c r="H37" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>5973</t>
         </is>
@@ -1568,7 +1794,13 @@
       <c r="F38" s="5" t="n">
         <v>27</v>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="G38" t="n">
+        <v>4244</v>
+      </c>
+      <c r="H38" s="5" t="n">
+        <v>27</v>
+      </c>
+      <c r="I38" t="inlineStr">
         <is>
           <t>4244</t>
         </is>
@@ -1599,7 +1831,13 @@
       <c r="F39" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="G39" t="n">
+        <v>3861</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I39" t="inlineStr">
         <is>
           <t>3861</t>
         </is>
@@ -1630,7 +1868,13 @@
       <c r="F40" s="3" t="n">
         <v>33</v>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G40" t="n">
+        <v>6057</v>
+      </c>
+      <c r="H40" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>6057</t>
         </is>
@@ -1661,7 +1905,13 @@
       <c r="F41" s="5" t="n">
         <v>29</v>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="G41" t="n">
+        <v>5869</v>
+      </c>
+      <c r="H41" s="5" t="n">
+        <v>29</v>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>5869</t>
         </is>
@@ -1692,7 +1942,13 @@
       <c r="F42" s="5" t="n">
         <v>24</v>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="G42" t="n">
+        <v>5264</v>
+      </c>
+      <c r="H42" s="5" t="n">
+        <v>24</v>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>5264</t>
         </is>
@@ -1723,7 +1979,13 @@
       <c r="F43" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="G43" t="n">
+        <v>5532</v>
+      </c>
+      <c r="H43" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I43" t="inlineStr">
         <is>
           <t>5532</t>
         </is>
@@ -1754,7 +2016,13 @@
       <c r="F44" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G44" t="inlineStr">
+      <c r="G44" t="n">
+        <v>5095</v>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" t="inlineStr">
         <is>
           <t>5095</t>
         </is>
@@ -1785,7 +2053,13 @@
       <c r="F45" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G45" t="inlineStr">
+      <c r="G45" t="n">
+        <v>5438</v>
+      </c>
+      <c r="H45" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>5438</t>
         </is>
@@ -1816,7 +2090,13 @@
       <c r="F46" s="5" t="n">
         <v>23</v>
       </c>
-      <c r="G46" t="inlineStr">
+      <c r="G46" t="n">
+        <v>5220</v>
+      </c>
+      <c r="H46" s="5" t="n">
+        <v>23</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>5220</t>
         </is>
@@ -1847,7 +2127,13 @@
       <c r="F47" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G47" t="inlineStr">
+      <c r="G47" t="n">
+        <v>4936</v>
+      </c>
+      <c r="H47" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>4936</t>
         </is>
@@ -1878,7 +2164,13 @@
       <c r="F48" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G48" t="inlineStr">
+      <c r="G48" t="n">
+        <v>5828</v>
+      </c>
+      <c r="H48" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I48" t="inlineStr">
         <is>
           <t>5828</t>
         </is>
@@ -1909,7 +2201,13 @@
       <c r="F49" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="G49" t="inlineStr">
+      <c r="G49" t="n">
+        <v>4556</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="I49" t="inlineStr">
         <is>
           <t>4556</t>
         </is>
@@ -1940,7 +2238,13 @@
       <c r="F50" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G50" t="inlineStr">
+      <c r="G50" t="n">
+        <v>4139</v>
+      </c>
+      <c r="H50" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="I50" t="inlineStr">
         <is>
           <t>4139</t>
         </is>
@@ -1971,7 +2275,13 @@
       <c r="F51" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="G51" t="inlineStr">
+      <c r="G51" t="n">
+        <v>4616</v>
+      </c>
+      <c r="H51" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="I51" t="inlineStr">
         <is>
           <t>4616</t>
         </is>
@@ -2002,7 +2312,13 @@
       <c r="F52" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="G52" t="inlineStr">
+      <c r="G52" t="n">
+        <v>4500</v>
+      </c>
+      <c r="H52" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="I52" t="inlineStr">
         <is>
           <t>4500</t>
         </is>
@@ -2033,7 +2349,13 @@
       <c r="F53" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G53" t="inlineStr">
+      <c r="G53" t="n">
+        <v>4596</v>
+      </c>
+      <c r="H53" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I53" t="inlineStr">
         <is>
           <t>4596</t>
         </is>
@@ -2064,7 +2386,13 @@
       <c r="F54" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G54" t="inlineStr">
+      <c r="G54" t="n">
+        <v>4055</v>
+      </c>
+      <c r="H54" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I54" t="inlineStr">
         <is>
           <t>4055</t>
         </is>
@@ -2095,7 +2423,13 @@
       <c r="F55" s="5" t="n">
         <v>30</v>
       </c>
-      <c r="G55" t="inlineStr">
+      <c r="G55" t="n">
+        <v>4218</v>
+      </c>
+      <c r="H55" s="5" t="n">
+        <v>30</v>
+      </c>
+      <c r="I55" t="inlineStr">
         <is>
           <t>4218</t>
         </is>
@@ -2126,7 +2460,13 @@
       <c r="F56" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G56" t="inlineStr">
+      <c r="G56" t="n">
+        <v>4123</v>
+      </c>
+      <c r="H56" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I56" t="inlineStr">
         <is>
           <t>4123</t>
         </is>
@@ -2157,7 +2497,13 @@
       <c r="F57" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="G57" t="inlineStr">
+      <c r="G57" t="n">
+        <v>4506</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="I57" t="inlineStr">
         <is>
           <t>4506</t>
         </is>
@@ -2188,7 +2534,13 @@
       <c r="F58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G58" t="inlineStr">
+      <c r="G58" t="n">
+        <v>0</v>
+      </c>
+      <c r="H58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2219,7 +2571,13 @@
       <c r="F59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G59" t="inlineStr">
+      <c r="G59" t="n">
+        <v>2944</v>
+      </c>
+      <c r="H59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I59" t="inlineStr">
         <is>
           <t>2944</t>
         </is>
@@ -2250,7 +2608,13 @@
       <c r="F60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G60" t="inlineStr">
+      <c r="G60" t="n">
+        <v>2737</v>
+      </c>
+      <c r="H60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I60" t="inlineStr">
         <is>
           <t>2737</t>
         </is>
@@ -2281,7 +2645,13 @@
       <c r="F61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G61" t="inlineStr">
+      <c r="G61" t="n">
+        <v>3168</v>
+      </c>
+      <c r="H61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I61" t="inlineStr">
         <is>
           <t>3168</t>
         </is>
@@ -2312,7 +2682,13 @@
       <c r="F62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G62" t="inlineStr">
+      <c r="G62" t="n">
+        <v>0</v>
+      </c>
+      <c r="H62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2338,6 +2714,8 @@
       <c r="E63" t="inlineStr"/>
       <c r="F63" s="5" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
+      <c r="H63" s="5" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2364,7 +2742,13 @@
       <c r="F64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G64" t="inlineStr">
+      <c r="G64" t="n">
+        <v>0</v>
+      </c>
+      <c r="H64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2395,7 +2779,13 @@
       <c r="F65" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G65" t="inlineStr">
+      <c r="G65" t="n">
+        <v>5200</v>
+      </c>
+      <c r="H65" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I65" t="inlineStr">
         <is>
           <t>5200</t>
         </is>
@@ -2426,7 +2816,13 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2457,7 +2853,13 @@
       <c r="F67" s="5" t="n">
         <v>28</v>
       </c>
-      <c r="G67" t="inlineStr">
+      <c r="G67" t="n">
+        <v>5509</v>
+      </c>
+      <c r="H67" s="5" t="n">
+        <v>28</v>
+      </c>
+      <c r="I67" t="inlineStr">
         <is>
           <t>5509</t>
         </is>
@@ -2488,7 +2890,13 @@
       <c r="F68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2519,7 +2927,13 @@
       <c r="F69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G69" t="inlineStr">
+      <c r="G69" t="n">
+        <v>2757</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
         <is>
           <t>2757</t>
         </is>
@@ -2550,7 +2964,13 @@
       <c r="F70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2581,7 +3001,13 @@
       <c r="F71" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G71" t="n">
+        <v>4891</v>
+      </c>
+      <c r="H71" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I71" t="inlineStr">
         <is>
           <t>4891</t>
         </is>
@@ -2612,7 +3038,13 @@
       <c r="F72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="G72" t="n">
+        <v>3355</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
         <is>
           <t>3355</t>
         </is>
@@ -2643,7 +3075,13 @@
       <c r="F73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G73" t="inlineStr">
+      <c r="G73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2674,7 +3112,13 @@
       <c r="F74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G74" t="inlineStr">
+      <c r="G74" t="n">
+        <v>1225</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
         <is>
           <t>1225</t>
         </is>
@@ -2705,7 +3149,13 @@
       <c r="F75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="G75" t="n">
+        <v>3440</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
         <is>
           <t>3440</t>
         </is>
@@ -2736,7 +3186,13 @@
       <c r="F76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G76" t="inlineStr">
+      <c r="G76" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2767,7 +3223,13 @@
       <c r="F77" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
+      <c r="G77" t="n">
+        <v>4653</v>
+      </c>
+      <c r="H77" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
         <is>
           <t>4653</t>
         </is>
@@ -2798,7 +3260,13 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2829,7 +3297,13 @@
       <c r="F79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G79" t="inlineStr">
+      <c r="G79" t="n">
+        <v>3187</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr">
         <is>
           <t>3187</t>
         </is>
@@ -2860,7 +3334,13 @@
       <c r="F80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G80" t="inlineStr">
+      <c r="G80" t="n">
+        <v>1455</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr">
         <is>
           <t>1455</t>
         </is>
@@ -2891,7 +3371,13 @@
       <c r="F81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G81" t="inlineStr">
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2922,7 +3408,13 @@
       <c r="F82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2953,7 +3445,13 @@
       <c r="F83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2984,7 +3482,13 @@
       <c r="F84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G84" t="inlineStr">
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3015,7 +3519,13 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3046,7 +3556,13 @@
       <c r="F86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="G86" t="n">
+        <v>999</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>999</t>
         </is>
@@ -3077,7 +3593,13 @@
       <c r="F87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3108,7 +3630,13 @@
       <c r="F88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G88" t="n">
+        <v>3122</v>
+      </c>
+      <c r="H88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>3122</t>
         </is>
@@ -3139,7 +3667,13 @@
       <c r="F89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3170,7 +3704,13 @@
       <c r="F90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3201,7 +3741,13 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="G91" t="n">
+        <v>2899</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>2899</t>
         </is>
@@ -3232,7 +3778,13 @@
       <c r="F92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3263,7 +3815,13 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="G93" t="n">
+        <v>3982</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
         <is>
           <t>3982</t>
         </is>
@@ -3294,7 +3852,13 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3325,7 +3889,13 @@
       <c r="F95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3356,7 +3926,13 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
+      <c r="G96" t="n">
+        <v>2057</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
         <is>
           <t>2057</t>
         </is>
@@ -3387,7 +3963,13 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3418,7 +4000,13 @@
       <c r="F98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3449,7 +4037,13 @@
       <c r="F99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3480,7 +4074,13 @@
       <c r="F100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="G100" t="n">
+        <v>2059</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
         <is>
           <t>2059</t>
         </is>
@@ -3511,7 +4111,13 @@
       <c r="F101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G101" t="inlineStr">
+      <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3542,7 +4148,13 @@
       <c r="F102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G102" t="inlineStr">
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3573,7 +4185,13 @@
       <c r="F103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="inlineStr">
+      <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3604,7 +4222,13 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="inlineStr">
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3635,7 +4259,13 @@
       <c r="F105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3666,7 +4296,13 @@
       <c r="F106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G106" t="inlineStr">
+      <c r="G106" t="n">
+        <v>0</v>
+      </c>
+      <c r="H106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3697,7 +4333,13 @@
       <c r="F107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G107" t="inlineStr">
+      <c r="G107" t="n">
+        <v>0</v>
+      </c>
+      <c r="H107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I107" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3728,7 +4370,13 @@
       <c r="F108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G108" t="inlineStr">
+      <c r="G108" t="n">
+        <v>0</v>
+      </c>
+      <c r="H108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3759,7 +4407,13 @@
       <c r="F109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G109" t="inlineStr">
+      <c r="G109" t="n">
+        <v>0</v>
+      </c>
+      <c r="H109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I109" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3790,7 +4444,13 @@
       <c r="F110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G110" t="inlineStr">
+      <c r="G110" t="n">
+        <v>0</v>
+      </c>
+      <c r="H110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3821,7 +4481,13 @@
       <c r="F111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G111" t="inlineStr">
+      <c r="G111" t="n">
+        <v>3224</v>
+      </c>
+      <c r="H111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I111" t="inlineStr">
         <is>
           <t>3224</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-10 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,10 +468,8 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="I2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -507,7 +505,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -581,7 +579,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>4956</t>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -618,7 +616,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2742</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -655,7 +653,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -690,10 +688,8 @@
       <c r="H8" s="3" t="n">
         <v>40</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>4975</t>
-        </is>
+      <c r="I8" t="n">
+        <v>4975</v>
       </c>
     </row>
     <row r="9">
@@ -715,7 +711,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F9" s="4" t="n">
@@ -725,11 +721,11 @@
         <v>4769</v>
       </c>
       <c r="H9" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>4769</t>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -803,7 +799,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2813</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -840,7 +836,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>1824</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -872,12 +868,12 @@
       <c r="G13" t="n">
         <v>4198</v>
       </c>
-      <c r="H13" s="4" t="n">
-        <v>15</v>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>4198</t>
+          <t>2491</t>
         </is>
       </c>
     </row>
@@ -914,7 +910,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -946,12 +942,12 @@
       <c r="G15" t="n">
         <v>4621</v>
       </c>
-      <c r="H15" s="4" t="n">
-        <v>18</v>
+      <c r="H15" s="5" t="n">
+        <v>29</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>4621</t>
+          <t>2778</t>
         </is>
       </c>
     </row>
@@ -983,12 +979,12 @@
       <c r="G16" t="n">
         <v>6537</v>
       </c>
-      <c r="H16" s="5" t="n">
-        <v>30</v>
+      <c r="H16" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>6537</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1021,11 +1017,11 @@
         <v>5402</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>5402</t>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -1058,11 +1054,11 @@
         <v>5602</v>
       </c>
       <c r="H18" s="5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>5602</t>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -1095,11 +1091,11 @@
         <v>6503</v>
       </c>
       <c r="H19" s="5" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>6503</t>
+          <t>2904</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1132,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>5665</t>
+          <t>3040</t>
         </is>
       </c>
     </row>
@@ -1169,11 +1165,11 @@
         <v>6176</v>
       </c>
       <c r="H21" s="5" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>6176</t>
+          <t>2929</t>
         </is>
       </c>
     </row>
@@ -1205,12 +1201,12 @@
       <c r="G22" t="n">
         <v>5494</v>
       </c>
-      <c r="H22" s="4" t="n">
-        <v>16</v>
+      <c r="H22" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>5494</t>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -1247,7 +1243,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>4041</t>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -1284,7 +1280,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>4237</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1316,12 +1312,12 @@
       <c r="G25" t="n">
         <v>5041</v>
       </c>
-      <c r="H25" s="5" t="n">
-        <v>30</v>
+      <c r="H25" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>5041</t>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -1353,12 +1349,12 @@
       <c r="G26" t="n">
         <v>5579</v>
       </c>
-      <c r="H26" s="5" t="n">
-        <v>30</v>
+      <c r="H26" s="3" t="n">
+        <v>34</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>5579</t>
+          <t>2967</t>
         </is>
       </c>
     </row>
@@ -1390,12 +1386,12 @@
       <c r="G27" t="n">
         <v>4934</v>
       </c>
-      <c r="H27" s="5" t="n">
-        <v>21</v>
+      <c r="H27" s="4" t="n">
+        <v>10</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>4934</t>
+          <t>2672</t>
         </is>
       </c>
     </row>
@@ -1432,7 +1428,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>5732</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1469,7 +1465,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>5363</t>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -1501,12 +1497,12 @@
       <c r="G30" t="n">
         <v>4610</v>
       </c>
-      <c r="H30" s="4" t="n">
-        <v>16</v>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>4610</t>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -1543,7 +1539,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>5176</t>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -1576,11 +1572,11 @@
         <v>4803</v>
       </c>
       <c r="H32" s="5" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>4803</t>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -1613,11 +1609,11 @@
         <v>6303</v>
       </c>
       <c r="H33" s="5" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>3052</t>
         </is>
       </c>
     </row>
@@ -1650,11 +1646,11 @@
         <v>6095</v>
       </c>
       <c r="H34" s="5" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>6095</t>
+          <t>2738</t>
         </is>
       </c>
     </row>
@@ -1686,12 +1682,12 @@
       <c r="G35" t="n">
         <v>4689</v>
       </c>
-      <c r="H35" s="2" t="n">
-        <v>0</v>
+      <c r="H35" s="4" t="n">
+        <v>14</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>4689</t>
+          <t>2767</t>
         </is>
       </c>
     </row>
@@ -1728,7 +1724,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>3532</t>
+          <t>2590</t>
         </is>
       </c>
     </row>
@@ -1765,7 +1761,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>5973</t>
+          <t>2904</t>
         </is>
       </c>
     </row>
@@ -1797,12 +1793,12 @@
       <c r="G38" t="n">
         <v>4244</v>
       </c>
-      <c r="H38" s="5" t="n">
-        <v>27</v>
+      <c r="H38" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>4244</t>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -1835,11 +1831,11 @@
         <v>3861</v>
       </c>
       <c r="H39" s="4" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>3861</t>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -1871,12 +1867,12 @@
       <c r="G40" t="n">
         <v>6057</v>
       </c>
-      <c r="H40" s="3" t="n">
-        <v>33</v>
+      <c r="H40" s="5" t="n">
+        <v>30</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>6057</t>
+          <t>2991</t>
         </is>
       </c>
     </row>
@@ -1909,11 +1905,11 @@
         <v>5869</v>
       </c>
       <c r="H41" s="5" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>5869</t>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -1946,11 +1942,11 @@
         <v>5264</v>
       </c>
       <c r="H42" s="5" t="n">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>5264</t>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -1983,11 +1979,11 @@
         <v>5532</v>
       </c>
       <c r="H43" s="5" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>5532</t>
+          <t>3024</t>
         </is>
       </c>
     </row>
@@ -2020,11 +2016,11 @@
         <v>5095</v>
       </c>
       <c r="H44" s="4" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>5095</t>
+          <t>2710</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2057,7 @@
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>5438</t>
+          <t>2933</t>
         </is>
       </c>
     </row>
@@ -2093,12 +2089,12 @@
       <c r="G46" t="n">
         <v>5220</v>
       </c>
-      <c r="H46" s="5" t="n">
-        <v>23</v>
+      <c r="H46" s="4" t="n">
+        <v>12</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>5220</t>
+          <t>2706</t>
         </is>
       </c>
     </row>
@@ -2130,12 +2126,12 @@
       <c r="G47" t="n">
         <v>4936</v>
       </c>
-      <c r="H47" s="5" t="n">
-        <v>20</v>
+      <c r="H47" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>4936</t>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -2168,11 +2164,11 @@
         <v>5828</v>
       </c>
       <c r="H48" s="5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>5828</t>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -2204,12 +2200,12 @@
       <c r="G49" t="n">
         <v>4556</v>
       </c>
-      <c r="H49" s="4" t="n">
-        <v>15</v>
+      <c r="H49" s="5" t="n">
+        <v>20</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>4556</t>
+          <t>2792</t>
         </is>
       </c>
     </row>
@@ -2244,10 +2240,8 @@
       <c r="H50" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>4139</t>
-        </is>
+      <c r="I50" t="n">
+        <v>4139</v>
       </c>
     </row>
     <row r="51">
@@ -2278,12 +2272,12 @@
       <c r="G51" t="n">
         <v>4616</v>
       </c>
-      <c r="H51" s="4" t="n">
-        <v>9</v>
+      <c r="H51" s="5" t="n">
+        <v>23</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>4616</t>
+          <t>2791</t>
         </is>
       </c>
     </row>
@@ -2315,12 +2309,12 @@
       <c r="G52" t="n">
         <v>4500</v>
       </c>
-      <c r="H52" s="4" t="n">
-        <v>18</v>
+      <c r="H52" s="5" t="n">
+        <v>20</v>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>4500</t>
+          <t>2786</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2351,7 @@
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>4596</t>
+          <t>2941</t>
         </is>
       </c>
     </row>
@@ -2394,7 +2388,7 @@
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>4055</t>
+          <t>2745</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2425,7 @@
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>4218</t>
+          <t>2845</t>
         </is>
       </c>
     </row>
@@ -2463,12 +2457,12 @@
       <c r="G56" t="n">
         <v>4123</v>
       </c>
-      <c r="H56" s="4" t="n">
-        <v>10</v>
+      <c r="H56" s="5" t="n">
+        <v>21</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>4123</t>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -2500,12 +2494,12 @@
       <c r="G57" t="n">
         <v>4506</v>
       </c>
-      <c r="H57" s="4" t="n">
-        <v>17</v>
+      <c r="H57" s="5" t="n">
+        <v>20</v>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>4506</t>
+          <t>2924</t>
         </is>
       </c>
     </row>
@@ -2579,7 +2573,7 @@
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>2944</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2616,7 +2610,7 @@
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>2737</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2653,7 +2647,7 @@
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>3168</t>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -2787,7 +2781,7 @@
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>5200</t>
+          <t>2796</t>
         </is>
       </c>
     </row>
@@ -2824,7 +2818,7 @@
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -2856,12 +2850,12 @@
       <c r="G67" t="n">
         <v>5509</v>
       </c>
-      <c r="H67" s="5" t="n">
-        <v>28</v>
+      <c r="H67" s="3" t="n">
+        <v>38</v>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>5509</t>
+          <t>3051</t>
         </is>
       </c>
     </row>
@@ -2935,7 +2929,7 @@
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>2757</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3004,12 +2998,12 @@
       <c r="G71" t="n">
         <v>4891</v>
       </c>
-      <c r="H71" s="4" t="n">
-        <v>2</v>
+      <c r="H71" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>4891</t>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -3046,7 +3040,7 @@
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>3355</t>
+          <t>2505</t>
         </is>
       </c>
     </row>
@@ -3120,7 +3114,7 @@
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>1225</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3157,7 +3151,7 @@
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>3440</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3188,7 @@
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -3226,12 +3220,12 @@
       <c r="G77" t="n">
         <v>4653</v>
       </c>
-      <c r="H77" s="5" t="n">
-        <v>20</v>
+      <c r="H77" s="4" t="n">
+        <v>4</v>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>4653</t>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -3305,7 +3299,7 @@
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>3187</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3342,7 +3336,7 @@
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>1455</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3564,7 +3558,7 @@
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>999</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3638,7 +3632,7 @@
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>3122</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -3749,7 +3743,7 @@
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>2899</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -3823,7 +3817,7 @@
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>3982</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3934,7 +3928,7 @@
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>2057</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4082,7 +4076,7 @@
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>2059</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4119,7 +4113,7 @@
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1499</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4483,65 @@
       </c>
       <c r="I111" t="inlineStr">
         <is>
-          <t>3224</t>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>27484940</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>"Zephyr zgx"</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr"/>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F112" s="5" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" s="5" t="n">
+        <v>20</v>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>2831</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>41837764</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>好风光会长</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr"/>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>二馆</t>
+        </is>
+      </c>
+      <c r="F113" s="5" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-11 06:39:24
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -82,9 +82,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:K113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>04-09_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>04-10_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>04-10_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -471,6 +481,8 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
+      <c r="J2" s="3" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -503,7 +515,13 @@
       <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="n">
+        <v>2519</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>2519</t>
         </is>
@@ -540,7 +558,13 @@
       <c r="H4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -577,7 +601,13 @@
       <c r="H5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="I5" t="n">
+        <v>2498</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -614,7 +644,13 @@
       <c r="H6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -651,7 +687,13 @@
       <c r="H7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="I7" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -679,18 +721,20 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="4" t="n">
         <v>40</v>
       </c>
       <c r="G8" t="n">
         <v>4975</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="4" t="n">
         <v>40</v>
       </c>
       <c r="I8" t="n">
         <v>4975</v>
       </c>
+      <c r="J8" s="3" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -714,16 +758,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G9" t="n">
         <v>4769</v>
       </c>
-      <c r="H9" s="4" t="n">
+      <c r="H9" s="5" t="n">
         <v>8</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="I9" t="n">
+        <v>2625</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="inlineStr">
         <is>
           <t>2625</t>
         </is>
@@ -760,7 +810,13 @@
       <c r="H10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -797,7 +853,13 @@
       <c r="H11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -834,7 +896,13 @@
       <c r="H12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -862,7 +930,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="5" t="n">
         <v>15</v>
       </c>
       <c r="G13" t="n">
@@ -871,7 +939,13 @@
       <c r="H13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="n">
+        <v>2491</v>
+      </c>
+      <c r="J13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>2491</t>
         </is>
@@ -908,7 +982,13 @@
       <c r="H14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="I14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="J14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -936,16 +1016,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <v>18</v>
       </c>
       <c r="G15" t="n">
         <v>4621</v>
       </c>
-      <c r="H15" s="5" t="n">
+      <c r="H15" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="I15" t="n">
+        <v>2778</v>
+      </c>
+      <c r="J15" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K15" t="inlineStr">
         <is>
           <t>2778</t>
         </is>
@@ -973,7 +1059,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G16" t="n">
@@ -982,7 +1068,13 @@
       <c r="H16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="I16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K16" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1010,16 +1102,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F17" s="3" t="n">
+      <c r="F17" s="4" t="n">
         <v>37</v>
       </c>
       <c r="G17" t="n">
         <v>5402</v>
       </c>
-      <c r="H17" s="3" t="n">
+      <c r="H17" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="I17" t="n">
+        <v>2956</v>
+      </c>
+      <c r="J17" s="4" t="n">
+        <v>40</v>
+      </c>
+      <c r="K17" t="inlineStr">
         <is>
           <t>2956</t>
         </is>
@@ -1047,16 +1145,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G18" t="n">
         <v>5602</v>
       </c>
-      <c r="H18" s="5" t="n">
+      <c r="H18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="I18" t="n">
+        <v>2740</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" t="inlineStr">
         <is>
           <t>2740</t>
         </is>
@@ -1084,16 +1188,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F19" s="5" t="n">
+      <c r="F19" s="3" t="n">
         <v>22</v>
       </c>
       <c r="G19" t="n">
         <v>6503</v>
       </c>
-      <c r="H19" s="5" t="n">
+      <c r="H19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="n">
+        <v>2904</v>
+      </c>
+      <c r="J19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>2904</t>
         </is>
@@ -1121,16 +1231,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F20" s="3" t="n">
+      <c r="F20" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G20" t="n">
         <v>5665</v>
       </c>
-      <c r="H20" s="3" t="n">
+      <c r="H20" s="4" t="n">
         <v>33</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="I20" t="n">
+        <v>3040</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>33</v>
+      </c>
+      <c r="K20" t="inlineStr">
         <is>
           <t>3040</t>
         </is>
@@ -1158,16 +1274,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F21" s="5" t="n">
+      <c r="F21" s="3" t="n">
         <v>27</v>
       </c>
       <c r="G21" t="n">
         <v>6176</v>
       </c>
-      <c r="H21" s="5" t="n">
+      <c r="H21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="n">
+        <v>2929</v>
+      </c>
+      <c r="J21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>2929</t>
         </is>
@@ -1195,7 +1317,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>16</v>
       </c>
       <c r="G22" t="n">
@@ -1204,7 +1326,13 @@
       <c r="H22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="I22" t="n">
+        <v>2498</v>
+      </c>
+      <c r="J22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -1232,16 +1360,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F23" s="5" t="n">
+      <c r="F23" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G23" t="n">
         <v>4041</v>
       </c>
-      <c r="H23" s="5" t="n">
+      <c r="H23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="I23" t="n">
+        <v>2741</v>
+      </c>
+      <c r="J23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>2741</t>
         </is>
@@ -1278,7 +1412,13 @@
       <c r="H24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="I24" t="n">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1306,7 +1446,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G25" t="n">
@@ -1315,7 +1455,13 @@
       <c r="H25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="I25" t="n">
+        <v>2526</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>2526</t>
         </is>
@@ -1343,16 +1489,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="F26" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G26" t="n">
         <v>5579</v>
       </c>
-      <c r="H26" s="3" t="n">
+      <c r="H26" s="4" t="n">
         <v>34</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="I26" t="n">
+        <v>2967</v>
+      </c>
+      <c r="J26" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>2967</t>
         </is>
@@ -1380,16 +1532,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G27" t="n">
         <v>4934</v>
       </c>
-      <c r="H27" s="4" t="n">
+      <c r="H27" s="5" t="n">
         <v>10</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" t="n">
+        <v>2672</v>
+      </c>
+      <c r="J27" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>2672</t>
         </is>
@@ -1426,7 +1584,13 @@
       <c r="H28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="I28" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1454,16 +1618,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F29" s="5" t="n">
+      <c r="F29" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G29" t="n">
         <v>5363</v>
       </c>
-      <c r="H29" s="5" t="n">
+      <c r="H29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="I29" t="n">
+        <v>2830</v>
+      </c>
+      <c r="J29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K29" t="inlineStr">
         <is>
           <t>2830</t>
         </is>
@@ -1491,7 +1661,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F30" s="4" t="n">
+      <c r="F30" s="5" t="n">
         <v>16</v>
       </c>
       <c r="G30" t="n">
@@ -1500,7 +1670,13 @@
       <c r="H30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="I30" t="n">
+        <v>2524</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>2524</t>
         </is>
@@ -1528,16 +1704,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F31" s="5" t="n">
+      <c r="F31" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G31" t="n">
         <v>5176</v>
       </c>
-      <c r="H31" s="5" t="n">
+      <c r="H31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I31" t="inlineStr">
+      <c r="I31" t="n">
+        <v>2906</v>
+      </c>
+      <c r="J31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>2906</t>
         </is>
@@ -1565,16 +1747,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F32" s="5" t="n">
+      <c r="F32" s="3" t="n">
         <v>28</v>
       </c>
       <c r="G32" t="n">
         <v>4803</v>
       </c>
-      <c r="H32" s="5" t="n">
+      <c r="H32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="I32" t="n">
+        <v>2856</v>
+      </c>
+      <c r="J32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>2856</t>
         </is>
@@ -1602,16 +1790,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F33" s="5" t="n">
+      <c r="F33" s="3" t="n">
         <v>21</v>
       </c>
       <c r="G33" t="n">
         <v>6303</v>
       </c>
-      <c r="H33" s="5" t="n">
+      <c r="H33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" t="n">
+        <v>3052</v>
+      </c>
+      <c r="J33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>3052</t>
         </is>
@@ -1639,16 +1833,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F34" s="5" t="n">
+      <c r="F34" s="3" t="n">
         <v>29</v>
       </c>
       <c r="G34" t="n">
         <v>6095</v>
       </c>
-      <c r="H34" s="5" t="n">
+      <c r="H34" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>2738</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>2738</t>
         </is>
@@ -1682,10 +1882,16 @@
       <c r="G35" t="n">
         <v>4689</v>
       </c>
-      <c r="H35" s="4" t="n">
+      <c r="H35" s="5" t="n">
         <v>14</v>
       </c>
-      <c r="I35" t="inlineStr">
+      <c r="I35" t="n">
+        <v>2767</v>
+      </c>
+      <c r="J35" s="5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>2767</t>
         </is>
@@ -1722,7 +1928,13 @@
       <c r="H36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="I36" t="n">
+        <v>2590</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>2590</t>
         </is>
@@ -1750,16 +1962,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F37" s="5" t="n">
+      <c r="F37" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G37" t="n">
         <v>5973</v>
       </c>
-      <c r="H37" s="5" t="n">
+      <c r="H37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="I37" t="n">
+        <v>2904</v>
+      </c>
+      <c r="J37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>2904</t>
         </is>
@@ -1787,16 +2005,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F38" s="5" t="n">
+      <c r="F38" s="3" t="n">
         <v>27</v>
       </c>
       <c r="G38" t="n">
         <v>4244</v>
       </c>
-      <c r="H38" s="4" t="n">
+      <c r="H38" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I38" t="inlineStr">
+      <c r="I38" t="n">
+        <v>2528</v>
+      </c>
+      <c r="J38" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>2528</t>
         </is>
@@ -1824,16 +2048,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F39" s="4" t="n">
+      <c r="F39" s="5" t="n">
         <v>15</v>
       </c>
       <c r="G39" t="n">
         <v>3861</v>
       </c>
-      <c r="H39" s="4" t="n">
+      <c r="H39" s="5" t="n">
         <v>5</v>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="I39" t="n">
+        <v>2575</v>
+      </c>
+      <c r="J39" s="5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K39" t="inlineStr">
         <is>
           <t>2575</t>
         </is>
@@ -1861,16 +2091,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F40" s="3" t="n">
+      <c r="F40" s="4" t="n">
         <v>33</v>
       </c>
       <c r="G40" t="n">
         <v>6057</v>
       </c>
-      <c r="H40" s="5" t="n">
+      <c r="H40" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="I40" t="n">
+        <v>2991</v>
+      </c>
+      <c r="J40" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>2991</t>
         </is>
@@ -1898,16 +2134,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F41" s="5" t="n">
+      <c r="F41" s="3" t="n">
         <v>29</v>
       </c>
       <c r="G41" t="n">
         <v>5869</v>
       </c>
-      <c r="H41" s="5" t="n">
+      <c r="H41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="I41" t="n">
+        <v>2997</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>2997</t>
         </is>
@@ -1935,16 +2177,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F42" s="5" t="n">
+      <c r="F42" s="3" t="n">
         <v>24</v>
       </c>
       <c r="G42" t="n">
         <v>5264</v>
       </c>
-      <c r="H42" s="5" t="n">
+      <c r="H42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="I42" t="n">
+        <v>2990</v>
+      </c>
+      <c r="J42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>2990</t>
         </is>
@@ -1972,16 +2220,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F43" s="5" t="n">
+      <c r="F43" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G43" t="n">
         <v>5532</v>
       </c>
-      <c r="H43" s="5" t="n">
+      <c r="H43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="I43" t="n">
+        <v>3024</v>
+      </c>
+      <c r="J43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>3024</t>
         </is>
@@ -2009,16 +2263,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F44" s="4" t="n">
+      <c r="F44" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G44" t="n">
         <v>5095</v>
       </c>
-      <c r="H44" s="4" t="n">
+      <c r="H44" s="5" t="n">
         <v>13</v>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="I44" t="n">
+        <v>2710</v>
+      </c>
+      <c r="J44" s="5" t="n">
+        <v>13</v>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>2710</t>
         </is>
@@ -2046,16 +2306,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F45" s="5" t="n">
+      <c r="F45" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G45" t="n">
         <v>5438</v>
       </c>
-      <c r="H45" s="5" t="n">
+      <c r="H45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I45" t="inlineStr">
+      <c r="I45" t="n">
+        <v>2933</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>2933</t>
         </is>
@@ -2083,16 +2349,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F46" s="5" t="n">
+      <c r="F46" s="3" t="n">
         <v>23</v>
       </c>
       <c r="G46" t="n">
         <v>5220</v>
       </c>
-      <c r="H46" s="4" t="n">
+      <c r="H46" s="5" t="n">
         <v>12</v>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="I46" t="n">
+        <v>2706</v>
+      </c>
+      <c r="J46" s="5" t="n">
+        <v>12</v>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>2706</t>
         </is>
@@ -2120,7 +2392,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F47" s="5" t="n">
+      <c r="F47" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G47" t="n">
@@ -2129,7 +2401,13 @@
       <c r="H47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="I47" t="n">
+        <v>2567</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>2567</t>
         </is>
@@ -2157,16 +2435,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F48" s="5" t="n">
+      <c r="F48" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G48" t="n">
         <v>5828</v>
       </c>
-      <c r="H48" s="5" t="n">
+      <c r="H48" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="I48" t="n">
+        <v>2915</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K48" t="inlineStr">
         <is>
           <t>2915</t>
         </is>
@@ -2194,16 +2478,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F49" s="4" t="n">
+      <c r="F49" s="5" t="n">
         <v>15</v>
       </c>
       <c r="G49" t="n">
         <v>4556</v>
       </c>
-      <c r="H49" s="5" t="n">
+      <c r="H49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="I49" t="n">
+        <v>2792</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K49" t="inlineStr">
         <is>
           <t>2792</t>
         </is>
@@ -2231,18 +2521,20 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F50" s="4" t="n">
+      <c r="F50" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G50" t="n">
         <v>4139</v>
       </c>
-      <c r="H50" s="4" t="n">
+      <c r="H50" s="5" t="n">
         <v>5</v>
       </c>
       <c r="I50" t="n">
         <v>4139</v>
       </c>
+      <c r="J50" s="3" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2266,16 +2558,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F51" s="4" t="n">
+      <c r="F51" s="5" t="n">
         <v>9</v>
       </c>
       <c r="G51" t="n">
         <v>4616</v>
       </c>
-      <c r="H51" s="5" t="n">
+      <c r="H51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I51" t="inlineStr">
+      <c r="I51" t="n">
+        <v>2791</v>
+      </c>
+      <c r="J51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K51" t="inlineStr">
         <is>
           <t>2791</t>
         </is>
@@ -2303,16 +2601,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F52" s="4" t="n">
+      <c r="F52" s="5" t="n">
         <v>18</v>
       </c>
       <c r="G52" t="n">
         <v>4500</v>
       </c>
-      <c r="H52" s="5" t="n">
+      <c r="H52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="I52" t="n">
+        <v>2786</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K52" t="inlineStr">
         <is>
           <t>2786</t>
         </is>
@@ -2340,16 +2644,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F53" s="5" t="n">
+      <c r="F53" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G53" t="n">
         <v>4596</v>
       </c>
-      <c r="H53" s="5" t="n">
+      <c r="H53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="I53" t="n">
+        <v>2941</v>
+      </c>
+      <c r="J53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K53" t="inlineStr">
         <is>
           <t>2941</t>
         </is>
@@ -2377,16 +2687,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F54" s="5" t="n">
+      <c r="F54" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G54" t="n">
         <v>4055</v>
       </c>
-      <c r="H54" s="5" t="n">
+      <c r="H54" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I54" t="inlineStr">
+      <c r="I54" t="n">
+        <v>2745</v>
+      </c>
+      <c r="J54" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>2745</t>
         </is>
@@ -2414,16 +2730,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="5" t="n">
+      <c r="F55" s="3" t="n">
         <v>30</v>
       </c>
       <c r="G55" t="n">
         <v>4218</v>
       </c>
-      <c r="H55" s="5" t="n">
+      <c r="H55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="I55" t="n">
+        <v>2845</v>
+      </c>
+      <c r="J55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K55" t="inlineStr">
         <is>
           <t>2845</t>
         </is>
@@ -2451,16 +2773,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F56" s="4" t="n">
+      <c r="F56" s="5" t="n">
         <v>10</v>
       </c>
       <c r="G56" t="n">
         <v>4123</v>
       </c>
-      <c r="H56" s="5" t="n">
+      <c r="H56" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I56" t="inlineStr">
+      <c r="I56" t="n">
+        <v>2794</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K56" t="inlineStr">
         <is>
           <t>2794</t>
         </is>
@@ -2488,16 +2816,22 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F57" s="5" t="n">
         <v>17</v>
       </c>
       <c r="G57" t="n">
         <v>4506</v>
       </c>
-      <c r="H57" s="5" t="n">
+      <c r="H57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
+      <c r="I57" t="n">
+        <v>2924</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
         <is>
           <t>2924</t>
         </is>
@@ -2534,7 +2868,13 @@
       <c r="H58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I58" t="inlineStr">
+      <c r="I58" t="n">
+        <v>0</v>
+      </c>
+      <c r="J58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2571,7 +2911,13 @@
       <c r="H59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I59" t="inlineStr">
+      <c r="I59" t="n">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2608,7 +2954,13 @@
       <c r="H60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I60" t="inlineStr">
+      <c r="I60" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K60" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2645,7 +2997,13 @@
       <c r="H61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I61" t="inlineStr">
+      <c r="I61" t="n">
+        <v>2513</v>
+      </c>
+      <c r="J61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K61" t="inlineStr">
         <is>
           <t>2513</t>
         </is>
@@ -2682,7 +3040,13 @@
       <c r="H62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I62" t="inlineStr">
+      <c r="I62" t="n">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2706,10 +3070,12 @@
         <v>5241</v>
       </c>
       <c r="E63" t="inlineStr"/>
-      <c r="F63" s="5" t="inlineStr"/>
+      <c r="F63" s="3" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
-      <c r="H63" s="5" t="inlineStr"/>
+      <c r="H63" s="3" t="inlineStr"/>
       <c r="I63" t="inlineStr"/>
+      <c r="J63" s="3" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2742,7 +3108,13 @@
       <c r="H64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I64" t="inlineStr">
+      <c r="I64" t="n">
+        <v>0</v>
+      </c>
+      <c r="J64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2770,16 +3142,22 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F65" s="5" t="n">
+      <c r="F65" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G65" t="n">
         <v>5200</v>
       </c>
-      <c r="H65" s="5" t="n">
+      <c r="H65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I65" t="inlineStr">
+      <c r="I65" t="n">
+        <v>2796</v>
+      </c>
+      <c r="J65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K65" t="inlineStr">
         <is>
           <t>2796</t>
         </is>
@@ -2816,7 +3194,13 @@
       <c r="H66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
+      <c r="I66" t="n">
+        <v>2498</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -2844,16 +3228,22 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F67" s="5" t="n">
+      <c r="F67" s="3" t="n">
         <v>28</v>
       </c>
       <c r="G67" t="n">
         <v>5509</v>
       </c>
-      <c r="H67" s="3" t="n">
+      <c r="H67" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="I67" t="inlineStr">
+      <c r="I67" t="n">
+        <v>3051</v>
+      </c>
+      <c r="J67" s="4" t="n">
+        <v>38</v>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t>3051</t>
         </is>
@@ -2890,7 +3280,13 @@
       <c r="H68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2927,7 +3323,13 @@
       <c r="H69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I69" t="inlineStr">
+      <c r="I69" t="n">
+        <v>0</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2964,7 +3366,13 @@
       <c r="H70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I70" t="inlineStr">
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2992,7 +3400,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F71" s="4" t="n">
+      <c r="F71" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G71" t="n">
@@ -3001,7 +3409,13 @@
       <c r="H71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I71" t="inlineStr">
+      <c r="I71" t="n">
+        <v>2539</v>
+      </c>
+      <c r="J71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t>2539</t>
         </is>
@@ -3038,7 +3452,13 @@
       <c r="H72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I72" t="inlineStr">
+      <c r="I72" t="n">
+        <v>2505</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
         <is>
           <t>2505</t>
         </is>
@@ -3075,7 +3495,13 @@
       <c r="H73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I73" t="inlineStr">
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3112,7 +3538,13 @@
       <c r="H74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3149,7 +3581,13 @@
       <c r="H75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3186,7 +3624,13 @@
       <c r="H76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I76" t="inlineStr">
+      <c r="I76" t="n">
+        <v>1500</v>
+      </c>
+      <c r="J76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="inlineStr">
         <is>
           <t>1500</t>
         </is>
@@ -3214,16 +3658,22 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F77" s="5" t="n">
+      <c r="F77" s="3" t="n">
         <v>20</v>
       </c>
       <c r="G77" t="n">
         <v>4653</v>
       </c>
-      <c r="H77" s="4" t="n">
+      <c r="H77" s="5" t="n">
         <v>4</v>
       </c>
-      <c r="I77" t="inlineStr">
+      <c r="I77" t="n">
+        <v>2574</v>
+      </c>
+      <c r="J77" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K77" t="inlineStr">
         <is>
           <t>2574</t>
         </is>
@@ -3260,7 +3710,13 @@
       <c r="H78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3297,7 +3753,13 @@
       <c r="H79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I79" t="inlineStr">
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3334,7 +3796,13 @@
       <c r="H80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I80" t="inlineStr">
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3371,7 +3839,13 @@
       <c r="H81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I81" t="inlineStr">
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3408,7 +3882,13 @@
       <c r="H82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I82" t="inlineStr">
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3445,7 +3925,13 @@
       <c r="H83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I83" t="inlineStr">
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3482,7 +3968,13 @@
       <c r="H84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I84" t="inlineStr">
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3519,7 +4011,13 @@
       <c r="H85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I85" t="inlineStr">
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3556,7 +4054,13 @@
       <c r="H86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I86" t="inlineStr">
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3593,7 +4097,13 @@
       <c r="H87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I87" t="inlineStr">
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3630,7 +4140,13 @@
       <c r="H88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I88" t="inlineStr">
+      <c r="I88" t="n">
+        <v>2499</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -3667,7 +4183,13 @@
       <c r="H89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I89" t="inlineStr">
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3704,7 +4226,13 @@
       <c r="H90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I90" t="inlineStr">
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3741,7 +4269,13 @@
       <c r="H91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="I91" t="n">
+        <v>2499</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -3778,7 +4312,13 @@
       <c r="H92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3815,7 +4355,13 @@
       <c r="H93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I93" t="inlineStr">
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3852,7 +4398,13 @@
       <c r="H94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3889,7 +4441,13 @@
       <c r="H95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I95" t="inlineStr">
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3926,7 +4484,13 @@
       <c r="H96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
+      <c r="I96" t="n">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3963,7 +4527,13 @@
       <c r="H97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4000,7 +4570,13 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4037,7 +4613,13 @@
       <c r="H99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I99" t="inlineStr">
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4074,7 +4656,13 @@
       <c r="H100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I100" t="inlineStr">
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4111,7 +4699,13 @@
       <c r="H101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I101" t="inlineStr">
+      <c r="I101" t="n">
+        <v>1499</v>
+      </c>
+      <c r="J101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr">
         <is>
           <t>1499</t>
         </is>
@@ -4148,7 +4742,13 @@
       <c r="H102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I102" t="inlineStr">
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4185,7 +4785,13 @@
       <c r="H103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I103" t="inlineStr">
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4222,7 +4828,13 @@
       <c r="H104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I104" t="inlineStr">
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4259,7 +4871,13 @@
       <c r="H105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4296,7 +4914,13 @@
       <c r="H106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I106" t="inlineStr">
+      <c r="I106" t="n">
+        <v>0</v>
+      </c>
+      <c r="J106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4333,7 +4957,13 @@
       <c r="H107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I107" t="inlineStr">
+      <c r="I107" t="n">
+        <v>0</v>
+      </c>
+      <c r="J107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K107" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4370,7 +5000,13 @@
       <c r="H108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I108" t="inlineStr">
+      <c r="I108" t="n">
+        <v>0</v>
+      </c>
+      <c r="J108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4407,7 +5043,13 @@
       <c r="H109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I109" t="inlineStr">
+      <c r="I109" t="n">
+        <v>0</v>
+      </c>
+      <c r="J109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K109" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4444,7 +5086,13 @@
       <c r="H110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I110" t="inlineStr">
+      <c r="I110" t="n">
+        <v>0</v>
+      </c>
+      <c r="J110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4481,17 +5129,21 @@
       <c r="H111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I111" t="inlineStr">
+      <c r="I111" t="n">
+        <v>0</v>
+      </c>
+      <c r="J111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K111" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr">
-        <is>
-          <t>27484940</t>
-        </is>
+      <c r="A112" t="n">
+        <v>27484940</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -4505,22 +5157,26 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F112" s="5" t="inlineStr"/>
+      <c r="F112" s="3" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
-      <c r="H112" s="5" t="n">
+      <c r="H112" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I112" t="inlineStr">
+      <c r="I112" t="n">
+        <v>2831</v>
+      </c>
+      <c r="J112" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K112" t="inlineStr">
         <is>
           <t>2831</t>
         </is>
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr">
-        <is>
-          <t>41837764</t>
-        </is>
+      <c r="A113" t="n">
+        <v>41837764</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -4534,12 +5190,18 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F113" s="5" t="inlineStr"/>
+      <c r="F113" s="3" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
       <c r="H113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I113" t="inlineStr">
+      <c r="I113" t="n">
+        <v>2519</v>
+      </c>
+      <c r="J113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K113" t="inlineStr">
         <is>
           <t>2519</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-11 11:30:49
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -83,8 +83,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K113"/>
+  <dimension ref="A1:K116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -604,12 +604,12 @@
       <c r="I5" t="n">
         <v>2498</v>
       </c>
-      <c r="J5" s="2" t="n">
-        <v>0</v>
+      <c r="J5" s="4" t="n">
+        <v>17</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2498</t>
+          <t>2906</t>
         </is>
       </c>
     </row>
@@ -690,12 +690,12 @@
       <c r="I7" t="n">
         <v>2500</v>
       </c>
-      <c r="J7" s="2" t="n">
-        <v>0</v>
+      <c r="J7" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2827</t>
         </is>
       </c>
     </row>
@@ -721,13 +721,13 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="5" t="n">
         <v>40</v>
       </c>
       <c r="G8" t="n">
         <v>4975</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I8" t="n">
@@ -758,24 +758,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G9" t="n">
         <v>4769</v>
       </c>
-      <c r="H9" s="5" t="n">
+      <c r="H9" s="4" t="n">
         <v>8</v>
       </c>
       <c r="I9" t="n">
         <v>2625</v>
       </c>
-      <c r="J9" s="5" t="n">
-        <v>8</v>
+      <c r="J9" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2625</t>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -930,7 +930,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G13" t="n">
@@ -942,12 +942,12 @@
       <c r="I13" t="n">
         <v>2491</v>
       </c>
-      <c r="J13" s="2" t="n">
-        <v>0</v>
+      <c r="J13" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2491</t>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="4" t="n">
         <v>18</v>
       </c>
       <c r="G15" t="n">
@@ -1029,11 +1029,11 @@
         <v>2778</v>
       </c>
       <c r="J15" s="3" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2778</t>
+          <t>2980</t>
         </is>
       </c>
     </row>
@@ -1102,24 +1102,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <v>37</v>
       </c>
       <c r="G17" t="n">
         <v>5402</v>
       </c>
-      <c r="H17" s="4" t="n">
+      <c r="H17" s="5" t="n">
         <v>40</v>
       </c>
       <c r="I17" t="n">
         <v>2956</v>
       </c>
-      <c r="J17" s="4" t="n">
+      <c r="J17" s="5" t="n">
         <v>40</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>2956</t>
+          <t>3345</t>
         </is>
       </c>
     </row>
@@ -1162,7 +1162,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>2740</t>
+          <t>3029</t>
         </is>
       </c>
     </row>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>2904</t>
+          <t>3323</t>
         </is>
       </c>
     </row>
@@ -1231,24 +1231,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G20" t="n">
         <v>5665</v>
       </c>
-      <c r="H20" s="4" t="n">
+      <c r="H20" s="5" t="n">
         <v>33</v>
       </c>
       <c r="I20" t="n">
         <v>3040</v>
       </c>
-      <c r="J20" s="4" t="n">
-        <v>33</v>
+      <c r="J20" s="5" t="n">
+        <v>36</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>3040</t>
+          <t>3395</t>
         </is>
       </c>
     </row>
@@ -1286,12 +1286,12 @@
       <c r="I21" t="n">
         <v>2929</v>
       </c>
-      <c r="J21" s="3" t="n">
-        <v>30</v>
+      <c r="J21" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2929</t>
+          <t>2977</t>
         </is>
       </c>
     </row>
@@ -1317,7 +1317,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="4" t="n">
         <v>16</v>
       </c>
       <c r="G22" t="n">
@@ -1334,7 +1334,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>2498</t>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -1377,7 +1377,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2741</t>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>2526</t>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -1495,18 +1495,18 @@
       <c r="G26" t="n">
         <v>5579</v>
       </c>
-      <c r="H26" s="4" t="n">
+      <c r="H26" s="5" t="n">
         <v>34</v>
       </c>
       <c r="I26" t="n">
         <v>2967</v>
       </c>
-      <c r="J26" s="4" t="n">
-        <v>34</v>
+      <c r="J26" s="5" t="n">
+        <v>35</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>2967</t>
+          <t>3418</t>
         </is>
       </c>
     </row>
@@ -1538,18 +1538,18 @@
       <c r="G27" t="n">
         <v>4934</v>
       </c>
-      <c r="H27" s="5" t="n">
+      <c r="H27" s="4" t="n">
         <v>10</v>
       </c>
       <c r="I27" t="n">
         <v>2672</v>
       </c>
-      <c r="J27" s="5" t="n">
-        <v>10</v>
+      <c r="J27" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>2672</t>
+          <t>2746</t>
         </is>
       </c>
     </row>
@@ -1592,7 +1592,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2523</t>
         </is>
       </c>
     </row>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>2830</t>
+          <t>3086</t>
         </is>
       </c>
     </row>
@@ -1661,7 +1661,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F30" s="5" t="n">
+      <c r="F30" s="4" t="n">
         <v>16</v>
       </c>
       <c r="G30" t="n">
@@ -1678,7 +1678,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>2524</t>
+          <t>2538</t>
         </is>
       </c>
     </row>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>2906</t>
+          <t>3287</t>
         </is>
       </c>
     </row>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2856</t>
+          <t>3161</t>
         </is>
       </c>
     </row>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>3052</t>
+          <t>3589</t>
         </is>
       </c>
     </row>
@@ -1845,12 +1845,12 @@
       <c r="I34" t="n">
         <v>2738</v>
       </c>
-      <c r="J34" s="3" t="n">
-        <v>21</v>
+      <c r="J34" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>2738</t>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -1882,18 +1882,18 @@
       <c r="G35" t="n">
         <v>4689</v>
       </c>
-      <c r="H35" s="5" t="n">
+      <c r="H35" s="4" t="n">
         <v>14</v>
       </c>
       <c r="I35" t="n">
         <v>2767</v>
       </c>
-      <c r="J35" s="5" t="n">
-        <v>14</v>
+      <c r="J35" s="4" t="n">
+        <v>6</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>2767</t>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>2590</t>
+          <t>2671</t>
         </is>
       </c>
     </row>
@@ -1979,7 +1979,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>2904</t>
+          <t>3414</t>
         </is>
       </c>
     </row>
@@ -2011,18 +2011,18 @@
       <c r="G38" t="n">
         <v>4244</v>
       </c>
-      <c r="H38" s="5" t="n">
+      <c r="H38" s="4" t="n">
         <v>5</v>
       </c>
       <c r="I38" t="n">
         <v>2528</v>
       </c>
-      <c r="J38" s="5" t="n">
-        <v>5</v>
+      <c r="J38" s="3" t="n">
+        <v>30</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>2872</t>
         </is>
       </c>
     </row>
@@ -2048,24 +2048,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F39" s="5" t="n">
+      <c r="F39" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G39" t="n">
         <v>3861</v>
       </c>
-      <c r="H39" s="5" t="n">
+      <c r="H39" s="4" t="n">
         <v>5</v>
       </c>
       <c r="I39" t="n">
         <v>2575</v>
       </c>
-      <c r="J39" s="5" t="n">
+      <c r="J39" s="4" t="n">
         <v>5</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>2575</t>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -2091,7 +2091,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F40" s="4" t="n">
+      <c r="F40" s="5" t="n">
         <v>33</v>
       </c>
       <c r="G40" t="n">
@@ -2103,12 +2103,12 @@
       <c r="I40" t="n">
         <v>2991</v>
       </c>
-      <c r="J40" s="3" t="n">
-        <v>30</v>
+      <c r="J40" s="5" t="n">
+        <v>31</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>2991</t>
+          <t>3525</t>
         </is>
       </c>
     </row>
@@ -2151,7 +2151,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>2997</t>
+          <t>3461</t>
         </is>
       </c>
     </row>
@@ -2194,7 +2194,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>2990</t>
+          <t>3474</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>3024</t>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -2263,24 +2263,24 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F44" s="5" t="n">
+      <c r="F44" s="4" t="n">
         <v>2</v>
       </c>
       <c r="G44" t="n">
         <v>5095</v>
       </c>
-      <c r="H44" s="5" t="n">
+      <c r="H44" s="4" t="n">
         <v>13</v>
       </c>
       <c r="I44" t="n">
         <v>2710</v>
       </c>
-      <c r="J44" s="5" t="n">
-        <v>13</v>
+      <c r="J44" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>2710</t>
+          <t>3074</t>
         </is>
       </c>
     </row>
@@ -2323,7 +2323,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>2933</t>
+          <t>3332</t>
         </is>
       </c>
     </row>
@@ -2355,18 +2355,18 @@
       <c r="G46" t="n">
         <v>5220</v>
       </c>
-      <c r="H46" s="5" t="n">
+      <c r="H46" s="4" t="n">
         <v>12</v>
       </c>
       <c r="I46" t="n">
         <v>2706</v>
       </c>
-      <c r="J46" s="5" t="n">
-        <v>12</v>
+      <c r="J46" s="4" t="n">
+        <v>10</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>2706</t>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -2404,12 +2404,12 @@
       <c r="I47" t="n">
         <v>2567</v>
       </c>
-      <c r="J47" s="2" t="n">
-        <v>0</v>
+      <c r="J47" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>2567</t>
+          <t>2626</t>
         </is>
       </c>
     </row>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>2915</t>
+          <t>3317</t>
         </is>
       </c>
     </row>
@@ -2478,7 +2478,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F49" s="5" t="n">
+      <c r="F49" s="4" t="n">
         <v>15</v>
       </c>
       <c r="G49" t="n">
@@ -2495,7 +2495,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>2792</t>
+          <t>3059</t>
         </is>
       </c>
     </row>
@@ -2521,13 +2521,13 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F50" s="5" t="n">
+      <c r="F50" s="4" t="n">
         <v>5</v>
       </c>
       <c r="G50" t="n">
         <v>4139</v>
       </c>
-      <c r="H50" s="5" t="n">
+      <c r="H50" s="4" t="n">
         <v>5</v>
       </c>
       <c r="I50" t="n">
@@ -2558,7 +2558,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F51" s="5" t="n">
+      <c r="F51" s="4" t="n">
         <v>9</v>
       </c>
       <c r="G51" t="n">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>2791</t>
+          <t>3091</t>
         </is>
       </c>
     </row>
@@ -2601,7 +2601,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F52" s="5" t="n">
+      <c r="F52" s="4" t="n">
         <v>18</v>
       </c>
       <c r="G52" t="n">
@@ -2618,7 +2618,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>2786</t>
+          <t>3006</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>2941</t>
+          <t>3206</t>
         </is>
       </c>
     </row>
@@ -2704,7 +2704,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>2745</t>
+          <t>2936</t>
         </is>
       </c>
     </row>
@@ -2747,7 +2747,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>2845</t>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -2773,7 +2773,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F56" s="5" t="n">
+      <c r="F56" s="4" t="n">
         <v>10</v>
       </c>
       <c r="G56" t="n">
@@ -2786,11 +2786,11 @@
         <v>2794</v>
       </c>
       <c r="J56" s="3" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>2794</t>
+          <t>2997</t>
         </is>
       </c>
     </row>
@@ -2816,7 +2816,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F57" s="5" t="n">
+      <c r="F57" s="4" t="n">
         <v>17</v>
       </c>
       <c r="G57" t="n">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="K57" t="inlineStr">
         <is>
-          <t>2924</t>
+          <t>3126</t>
         </is>
       </c>
     </row>
@@ -2919,7 +2919,7 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -3000,12 +3000,12 @@
       <c r="I61" t="n">
         <v>2513</v>
       </c>
-      <c r="J61" s="2" t="n">
-        <v>0</v>
+      <c r="J61" s="4" t="n">
+        <v>5</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>2513</t>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>2796</t>
+          <t>3073</t>
         </is>
       </c>
     </row>
@@ -3202,7 +3202,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>2498</t>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -3225,7 +3225,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F67" s="3" t="n">
@@ -3234,18 +3234,18 @@
       <c r="G67" t="n">
         <v>5509</v>
       </c>
-      <c r="H67" s="4" t="n">
+      <c r="H67" s="5" t="n">
         <v>38</v>
       </c>
       <c r="I67" t="n">
         <v>3051</v>
       </c>
-      <c r="J67" s="4" t="n">
-        <v>38</v>
+      <c r="J67" s="5" t="n">
+        <v>33</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>3051</t>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -3400,7 +3400,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F71" s="5" t="n">
+      <c r="F71" s="4" t="n">
         <v>2</v>
       </c>
       <c r="G71" t="n">
@@ -3412,12 +3412,12 @@
       <c r="I71" t="n">
         <v>2539</v>
       </c>
-      <c r="J71" s="2" t="n">
-        <v>0</v>
+      <c r="J71" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>2539</t>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>2505</t>
+          <t>2520</t>
         </is>
       </c>
     </row>
@@ -3587,10 +3587,8 @@
       <c r="J75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K75" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="K75" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -3664,18 +3662,18 @@
       <c r="G77" t="n">
         <v>4653</v>
       </c>
-      <c r="H77" s="5" t="n">
+      <c r="H77" s="4" t="n">
         <v>4</v>
       </c>
       <c r="I77" t="n">
         <v>2574</v>
       </c>
-      <c r="J77" s="5" t="n">
-        <v>4</v>
+      <c r="J77" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>2574</t>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -4148,7 +4146,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>2499</t>
+          <t>2549</t>
         </is>
       </c>
     </row>
@@ -4277,7 +4275,7 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>2499</t>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -4358,12 +4356,12 @@
       <c r="I93" t="n">
         <v>0</v>
       </c>
-      <c r="J93" s="2" t="n">
-        <v>0</v>
+      <c r="J93" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="K93" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -5166,11 +5164,11 @@
         <v>2831</v>
       </c>
       <c r="J112" s="3" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="K112" t="inlineStr">
         <is>
-          <t>2831</t>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -5203,7 +5201,100 @@
       </c>
       <c r="K113" t="inlineStr">
         <is>
-          <t>2519</t>
+          <t>2602</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>44437839</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>strangetamer828</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr"/>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F114" s="3" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" s="3" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>1595</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>49043337</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>FanXiFang1976</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F115" s="3" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" s="3" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>3166</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>59020292</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Player-59020292</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F116" s="3" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" s="3" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>2761</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-12 11:30:49
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K116"/>
+  <dimension ref="A1:M116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>04-10_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>04-11_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>04-11_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -483,6 +493,8 @@
       </c>
       <c r="J2" s="3" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
+      <c r="L2" s="3" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -521,7 +533,13 @@
       <c r="J3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" t="n">
+        <v>2519</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>2519</t>
         </is>
@@ -564,7 +582,13 @@
       <c r="J4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -607,9 +631,15 @@
       <c r="J5" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2906</t>
+      <c r="K5" t="n">
+        <v>2906</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>3006</t>
         </is>
       </c>
     </row>
@@ -650,7 +680,13 @@
       <c r="J6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -693,9 +729,15 @@
       <c r="J7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>2827</t>
+      <c r="K7" t="n">
+        <v>2827</v>
+      </c>
+      <c r="L7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>3147</t>
         </is>
       </c>
     </row>
@@ -735,6 +777,8 @@
       </c>
       <c r="J8" s="3" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" s="3" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -773,9 +817,15 @@
       <c r="J9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>2740</t>
+      <c r="K9" t="n">
+        <v>2740</v>
+      </c>
+      <c r="L9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -816,7 +866,13 @@
       <c r="J10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -859,7 +915,13 @@
       <c r="J11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K11" t="inlineStr">
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -902,7 +964,13 @@
       <c r="J12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -945,9 +1013,15 @@
       <c r="J13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="K13" t="n">
+        <v>2752</v>
+      </c>
+      <c r="L13" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>3016</t>
         </is>
       </c>
     </row>
@@ -988,7 +1062,13 @@
       <c r="J14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="K14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="L14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -1031,9 +1111,15 @@
       <c r="J15" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>2980</t>
+      <c r="K15" t="n">
+        <v>2980</v>
+      </c>
+      <c r="L15" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>3284</t>
         </is>
       </c>
     </row>
@@ -1074,7 +1160,13 @@
       <c r="J16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K16" t="inlineStr">
+      <c r="K16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M16" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1117,9 +1209,15 @@
       <c r="J17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>3345</t>
+      <c r="K17" t="n">
+        <v>3345</v>
+      </c>
+      <c r="L17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>3703</t>
         </is>
       </c>
     </row>
@@ -1160,9 +1258,15 @@
       <c r="J18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3029</t>
+      <c r="K18" t="n">
+        <v>3029</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>3373</t>
         </is>
       </c>
     </row>
@@ -1203,9 +1307,15 @@
       <c r="J19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>3323</t>
+      <c r="K19" t="n">
+        <v>3323</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>3719</t>
         </is>
       </c>
     </row>
@@ -1246,9 +1356,15 @@
       <c r="J20" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3395</t>
+      <c r="K20" t="n">
+        <v>3395</v>
+      </c>
+      <c r="L20" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>3841</t>
         </is>
       </c>
     </row>
@@ -1289,9 +1405,15 @@
       <c r="J21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>2977</t>
+      <c r="K21" t="n">
+        <v>2977</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>3455</t>
         </is>
       </c>
     </row>
@@ -1332,9 +1454,15 @@
       <c r="J22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="K22" t="n">
+        <v>2539</v>
+      </c>
+      <c r="L22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>2553</t>
         </is>
       </c>
     </row>
@@ -1375,9 +1503,15 @@
       <c r="J23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="K23" t="n">
+        <v>2996</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>3216</t>
         </is>
       </c>
     </row>
@@ -1418,7 +1552,13 @@
       <c r="J24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="K24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1461,9 +1601,15 @@
       <c r="J25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="K25" t="n">
+        <v>2521</v>
+      </c>
+      <c r="L25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>2541</t>
         </is>
       </c>
     </row>
@@ -1504,9 +1650,15 @@
       <c r="J26" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="K26" t="inlineStr">
-        <is>
-          <t>3418</t>
+      <c r="K26" t="n">
+        <v>3418</v>
+      </c>
+      <c r="L26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>3786</t>
         </is>
       </c>
     </row>
@@ -1547,9 +1699,15 @@
       <c r="J27" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>2746</t>
+      <c r="K27" t="n">
+        <v>2746</v>
+      </c>
+      <c r="L27" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1748,13 @@
       <c r="J28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K28" t="inlineStr">
+      <c r="K28" t="n">
+        <v>2523</v>
+      </c>
+      <c r="L28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M28" t="inlineStr">
         <is>
           <t>2523</t>
         </is>
@@ -1633,9 +1797,15 @@
       <c r="J29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>3086</t>
+      <c r="K29" t="n">
+        <v>3086</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>3378</t>
         </is>
       </c>
     </row>
@@ -1676,9 +1846,15 @@
       <c r="J30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>2538</t>
+      <c r="K30" t="n">
+        <v>2538</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>2590</t>
         </is>
       </c>
     </row>
@@ -1719,9 +1895,15 @@
       <c r="J31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>3287</t>
+      <c r="K31" t="n">
+        <v>3287</v>
+      </c>
+      <c r="L31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>3639</t>
         </is>
       </c>
     </row>
@@ -1762,9 +1944,15 @@
       <c r="J32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>3161</t>
+      <c r="K32" t="n">
+        <v>3161</v>
+      </c>
+      <c r="L32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>3528</t>
         </is>
       </c>
     </row>
@@ -1805,9 +1993,15 @@
       <c r="J33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K33" t="inlineStr">
-        <is>
-          <t>3589</t>
+      <c r="K33" t="n">
+        <v>3589</v>
+      </c>
+      <c r="L33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>4012</t>
         </is>
       </c>
     </row>
@@ -1848,9 +2042,15 @@
       <c r="J34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="K34" t="n">
+        <v>2729</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>2717</t>
         </is>
       </c>
     </row>
@@ -1891,9 +2091,15 @@
       <c r="J35" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="K35" t="n">
+        <v>3018</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>3391</t>
         </is>
       </c>
     </row>
@@ -1934,9 +2140,15 @@
       <c r="J36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>2671</t>
+      <c r="K36" t="n">
+        <v>2671</v>
+      </c>
+      <c r="L36" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -1977,9 +2189,15 @@
       <c r="J37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>3414</t>
+      <c r="K37" t="n">
+        <v>3414</v>
+      </c>
+      <c r="L37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>3787</t>
         </is>
       </c>
     </row>
@@ -2020,9 +2238,15 @@
       <c r="J38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>2872</t>
+      <c r="K38" t="n">
+        <v>2872</v>
+      </c>
+      <c r="L38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>3146</t>
         </is>
       </c>
     </row>
@@ -2063,9 +2287,15 @@
       <c r="J39" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="K39" t="n">
+        <v>2685</v>
+      </c>
+      <c r="L39" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>2842</t>
         </is>
       </c>
     </row>
@@ -2106,9 +2336,15 @@
       <c r="J40" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="K40" t="inlineStr">
-        <is>
-          <t>3525</t>
+      <c r="K40" t="n">
+        <v>3525</v>
+      </c>
+      <c r="L40" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>3979</t>
         </is>
       </c>
     </row>
@@ -2149,9 +2385,15 @@
       <c r="J41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>3461</t>
+      <c r="K41" t="n">
+        <v>3461</v>
+      </c>
+      <c r="L41" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>3699</t>
         </is>
       </c>
     </row>
@@ -2192,9 +2434,15 @@
       <c r="J42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3474</t>
+      <c r="K42" t="n">
+        <v>3474</v>
+      </c>
+      <c r="L42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>3834</t>
         </is>
       </c>
     </row>
@@ -2235,9 +2483,15 @@
       <c r="J43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K43" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="K43" t="n">
+        <v>3465</v>
+      </c>
+      <c r="L43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>3873</t>
         </is>
       </c>
     </row>
@@ -2278,9 +2532,15 @@
       <c r="J44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>3074</t>
+      <c r="K44" t="n">
+        <v>3074</v>
+      </c>
+      <c r="L44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>3442</t>
         </is>
       </c>
     </row>
@@ -2321,9 +2581,15 @@
       <c r="J45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3332</t>
+      <c r="K45" t="n">
+        <v>3332</v>
+      </c>
+      <c r="L45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3699</t>
         </is>
       </c>
     </row>
@@ -2364,9 +2630,15 @@
       <c r="J46" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="K46" t="n">
+        <v>2860</v>
+      </c>
+      <c r="L46" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>3151</t>
         </is>
       </c>
     </row>
@@ -2407,9 +2679,15 @@
       <c r="J47" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>2626</t>
+      <c r="K47" t="n">
+        <v>2626</v>
+      </c>
+      <c r="L47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>2954</t>
         </is>
       </c>
     </row>
@@ -2450,9 +2728,15 @@
       <c r="J48" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>3317</t>
+      <c r="K48" t="n">
+        <v>3317</v>
+      </c>
+      <c r="L48" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>3751</t>
         </is>
       </c>
     </row>
@@ -2493,9 +2777,15 @@
       <c r="J49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3059</t>
+      <c r="K49" t="n">
+        <v>3059</v>
+      </c>
+      <c r="L49" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>3297</t>
         </is>
       </c>
     </row>
@@ -2535,6 +2825,8 @@
       </c>
       <c r="J50" s="3" t="inlineStr"/>
       <c r="K50" t="inlineStr"/>
+      <c r="L50" s="3" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2573,9 +2865,15 @@
       <c r="J51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>3091</t>
+      <c r="K51" t="n">
+        <v>3091</v>
+      </c>
+      <c r="L51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -2616,9 +2914,15 @@
       <c r="J52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>3006</t>
+      <c r="K52" t="n">
+        <v>3006</v>
+      </c>
+      <c r="L52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>3256</t>
         </is>
       </c>
     </row>
@@ -2659,9 +2963,15 @@
       <c r="J53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>3206</t>
+      <c r="K53" t="n">
+        <v>3206</v>
+      </c>
+      <c r="L53" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>3416</t>
         </is>
       </c>
     </row>
@@ -2702,9 +3012,15 @@
       <c r="J54" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>2936</t>
+      <c r="K54" t="n">
+        <v>2936</v>
+      </c>
+      <c r="L54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>3149</t>
         </is>
       </c>
     </row>
@@ -2745,9 +3061,15 @@
       <c r="J55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="K55" t="n">
+        <v>2996</v>
+      </c>
+      <c r="L55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3160</t>
         </is>
       </c>
     </row>
@@ -2788,9 +3110,15 @@
       <c r="J56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>2997</t>
+      <c r="K56" t="n">
+        <v>2997</v>
+      </c>
+      <c r="L56" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>3248</t>
         </is>
       </c>
     </row>
@@ -2831,9 +3159,15 @@
       <c r="J57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>3126</t>
+      <c r="K57" t="n">
+        <v>3126</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>3394</t>
         </is>
       </c>
     </row>
@@ -2874,7 +3208,13 @@
       <c r="J58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K58" t="inlineStr">
+      <c r="K58" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2917,9 +3257,15 @@
       <c r="J59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="K59" t="n">
+        <v>2518</v>
+      </c>
+      <c r="L59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>2539</t>
         </is>
       </c>
     </row>
@@ -2960,9 +3306,15 @@
       <c r="J60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="K60" t="n">
+        <v>2493</v>
+      </c>
+      <c r="L60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>2485</t>
         </is>
       </c>
     </row>
@@ -3003,7 +3355,13 @@
       <c r="J61" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K61" t="inlineStr">
+      <c r="K61" t="n">
+        <v>2597</v>
+      </c>
+      <c r="L61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M61" t="inlineStr">
         <is>
           <t>2597</t>
         </is>
@@ -3046,7 +3404,13 @@
       <c r="J62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K62" t="inlineStr">
+      <c r="K62" t="n">
+        <v>0</v>
+      </c>
+      <c r="L62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3076,6 +3440,8 @@
       <c r="I63" t="inlineStr"/>
       <c r="J63" s="3" t="inlineStr"/>
       <c r="K63" t="inlineStr"/>
+      <c r="L63" s="3" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3114,7 +3480,13 @@
       <c r="J64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K64" t="inlineStr">
+      <c r="K64" t="n">
+        <v>0</v>
+      </c>
+      <c r="L64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3157,9 +3529,15 @@
       <c r="J65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>3073</t>
+      <c r="K65" t="n">
+        <v>3073</v>
+      </c>
+      <c r="L65" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>3376</t>
         </is>
       </c>
     </row>
@@ -3200,9 +3578,15 @@
       <c r="J66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K66" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="K66" t="n">
+        <v>2493</v>
+      </c>
+      <c r="L66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>2492</t>
         </is>
       </c>
     </row>
@@ -3243,9 +3627,15 @@
       <c r="J67" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K67" t="inlineStr">
-        <is>
-          <t>3498</t>
+      <c r="K67" t="n">
+        <v>3498</v>
+      </c>
+      <c r="L67" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>3796</t>
         </is>
       </c>
     </row>
@@ -3286,7 +3676,13 @@
       <c r="J68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3329,7 +3725,13 @@
       <c r="J69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K69" t="inlineStr">
+      <c r="K69" t="n">
+        <v>0</v>
+      </c>
+      <c r="L69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3372,7 +3774,13 @@
       <c r="J70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K70" t="inlineStr">
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3415,9 +3823,15 @@
       <c r="J71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>2918</t>
+      <c r="K71" t="n">
+        <v>2918</v>
+      </c>
+      <c r="L71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -3458,9 +3872,15 @@
       <c r="J72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>2520</t>
+      <c r="K72" t="n">
+        <v>2520</v>
+      </c>
+      <c r="L72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -3501,7 +3921,13 @@
       <c r="J73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K73" t="inlineStr">
+      <c r="K73" t="n">
+        <v>0</v>
+      </c>
+      <c r="L73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3544,7 +3970,13 @@
       <c r="J74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="inlineStr">
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3590,6 +4022,8 @@
       <c r="K75" t="n">
         <v>0</v>
       </c>
+      <c r="L75" s="3" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -3628,9 +4062,15 @@
       <c r="J76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="K76" t="n">
+        <v>1500</v>
+      </c>
+      <c r="L76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>1499</t>
         </is>
       </c>
     </row>
@@ -3671,9 +4111,15 @@
       <c r="J77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="K77" t="n">
+        <v>2857</v>
+      </c>
+      <c r="L77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -3714,7 +4160,13 @@
       <c r="J78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K78" t="inlineStr">
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3757,7 +4209,13 @@
       <c r="J79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K79" t="inlineStr">
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3800,7 +4258,13 @@
       <c r="J80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K80" t="inlineStr">
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3843,7 +4307,13 @@
       <c r="J81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K81" t="inlineStr">
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3886,7 +4356,13 @@
       <c r="J82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K82" t="inlineStr">
+      <c r="K82" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3929,7 +4405,13 @@
       <c r="J83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K83" t="inlineStr">
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
+      <c r="L83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3972,7 +4454,13 @@
       <c r="J84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K84" t="inlineStr">
+      <c r="K84" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4015,7 +4503,13 @@
       <c r="J85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K85" t="inlineStr">
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4058,7 +4552,13 @@
       <c r="J86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K86" t="inlineStr">
+      <c r="K86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4101,7 +4601,13 @@
       <c r="J87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K87" t="inlineStr">
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4144,9 +4650,15 @@
       <c r="J88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K88" t="inlineStr">
-        <is>
-          <t>2549</t>
+      <c r="K88" t="n">
+        <v>2549</v>
+      </c>
+      <c r="L88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>2590</t>
         </is>
       </c>
     </row>
@@ -4187,7 +4699,13 @@
       <c r="J89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K89" t="inlineStr">
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4230,7 +4748,13 @@
       <c r="J90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr">
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4273,9 +4797,15 @@
       <c r="J91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>2490</t>
+      <c r="K91" t="n">
+        <v>2490</v>
+      </c>
+      <c r="L91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -4316,7 +4846,13 @@
       <c r="J92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K92" t="inlineStr">
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4359,9 +4895,15 @@
       <c r="J93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K93" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="K93" t="n">
+        <v>2758</v>
+      </c>
+      <c r="L93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -4402,7 +4944,13 @@
       <c r="J94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K94" t="inlineStr">
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4445,7 +4993,13 @@
       <c r="J95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K95" t="inlineStr">
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
+      <c r="L95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4488,7 +5042,13 @@
       <c r="J96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
+      <c r="K96" t="n">
+        <v>0</v>
+      </c>
+      <c r="L96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4531,7 +5091,13 @@
       <c r="J97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr">
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
+      <c r="L97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4574,7 +5140,13 @@
       <c r="J98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4617,7 +5189,13 @@
       <c r="J99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K99" t="inlineStr">
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+      <c r="L99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4660,7 +5238,13 @@
       <c r="J100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K100" t="inlineStr">
+      <c r="K100" t="n">
+        <v>0</v>
+      </c>
+      <c r="L100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4703,7 +5287,13 @@
       <c r="J101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K101" t="inlineStr">
+      <c r="K101" t="n">
+        <v>1499</v>
+      </c>
+      <c r="L101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" t="inlineStr">
         <is>
           <t>1499</t>
         </is>
@@ -4746,7 +5336,13 @@
       <c r="J102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K102" t="inlineStr">
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4789,7 +5385,13 @@
       <c r="J103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K103" t="inlineStr">
+      <c r="K103" t="n">
+        <v>0</v>
+      </c>
+      <c r="L103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4832,7 +5434,13 @@
       <c r="J104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K104" t="inlineStr">
+      <c r="K104" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4875,7 +5483,13 @@
       <c r="J105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K105" t="inlineStr">
+      <c r="K105" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4918,7 +5532,13 @@
       <c r="J106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K106" t="inlineStr">
+      <c r="K106" t="n">
+        <v>0</v>
+      </c>
+      <c r="L106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4961,7 +5581,13 @@
       <c r="J107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K107" t="inlineStr">
+      <c r="K107" t="n">
+        <v>0</v>
+      </c>
+      <c r="L107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M107" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5004,7 +5630,13 @@
       <c r="J108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K108" t="inlineStr">
+      <c r="K108" t="n">
+        <v>0</v>
+      </c>
+      <c r="L108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5047,7 +5679,13 @@
       <c r="J109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K109" t="inlineStr">
+      <c r="K109" t="n">
+        <v>0</v>
+      </c>
+      <c r="L109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M109" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5090,7 +5728,13 @@
       <c r="J110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K110" t="inlineStr">
+      <c r="K110" t="n">
+        <v>0</v>
+      </c>
+      <c r="L110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5133,7 +5777,13 @@
       <c r="J111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K111" t="inlineStr">
+      <c r="K111" t="n">
+        <v>0</v>
+      </c>
+      <c r="L111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M111" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5166,9 +5816,15 @@
       <c r="J112" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="K112" t="inlineStr">
-        <is>
-          <t>3237</t>
+      <c r="K112" t="n">
+        <v>3237</v>
+      </c>
+      <c r="L112" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M112" t="inlineStr">
+        <is>
+          <t>3471</t>
         </is>
       </c>
     </row>
@@ -5199,17 +5855,21 @@
       <c r="J113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K113" t="inlineStr">
-        <is>
-          <t>2602</t>
+      <c r="K113" t="n">
+        <v>2602</v>
+      </c>
+      <c r="L113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M113" t="inlineStr">
+        <is>
+          <t>2620</t>
         </is>
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>44437839</t>
-        </is>
+      <c r="A114" t="n">
+        <v>44437839</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -5230,17 +5890,21 @@
       <c r="J114" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="K114" t="inlineStr">
-        <is>
-          <t>1595</t>
+      <c r="K114" t="n">
+        <v>1595</v>
+      </c>
+      <c r="L114" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="M114" t="inlineStr">
+        <is>
+          <t>1588</t>
         </is>
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>49043337</t>
-        </is>
+      <c r="A115" t="n">
+        <v>49043337</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -5261,21 +5925,25 @@
       <c r="J115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>3166</t>
+      <c r="K115" t="n">
+        <v>3166</v>
+      </c>
+      <c r="L115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>3541</t>
         </is>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>59020292</t>
-        </is>
+      <c r="A116" t="n">
+        <v>59020292</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Player-59020292</t>
+          <t>Sharnoth</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -5292,9 +5960,15 @@
       <c r="J116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>2761</t>
+      <c r="K116" t="n">
+        <v>2761</v>
+      </c>
+      <c r="L116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>2865</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-13 11:31:07
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M116"/>
+  <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>04-11_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>04-12_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>04-12_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -495,6 +505,8 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" s="3" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
+      <c r="N2" s="3" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -539,9 +551,15 @@
       <c r="L3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="M3" t="n">
+        <v>2519</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -588,7 +606,13 @@
       <c r="L4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -613,7 +637,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F5" s="2" t="n">
@@ -637,9 +661,15 @@
       <c r="L5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>3006</t>
+      <c r="M5" t="n">
+        <v>3006</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>3550</t>
         </is>
       </c>
     </row>
@@ -686,7 +716,13 @@
       <c r="L6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -735,9 +771,15 @@
       <c r="L7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>3147</t>
+      <c r="M7" t="n">
+        <v>3147</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>3544</t>
         </is>
       </c>
     </row>
@@ -779,6 +821,8 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" s="3" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" s="3" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -823,9 +867,15 @@
       <c r="L9" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="M9" t="n">
+        <v>2887</v>
+      </c>
+      <c r="N9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>2920</t>
         </is>
       </c>
     </row>
@@ -872,7 +922,13 @@
       <c r="L10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M10" t="inlineStr">
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -921,7 +977,13 @@
       <c r="L11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -970,7 +1032,13 @@
       <c r="L12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M12" t="inlineStr">
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1019,9 +1087,15 @@
       <c r="L13" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>3016</t>
+      <c r="M13" t="n">
+        <v>3016</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>3289</t>
         </is>
       </c>
     </row>
@@ -1068,7 +1142,13 @@
       <c r="L14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M14" t="inlineStr">
+      <c r="M14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="N14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -1117,9 +1197,15 @@
       <c r="L15" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>3284</t>
+      <c r="M15" t="n">
+        <v>3284</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1252,13 @@
       <c r="L16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="M16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1215,9 +1307,15 @@
       <c r="L17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>3703</t>
+      <c r="M17" t="n">
+        <v>3703</v>
+      </c>
+      <c r="N17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -1264,9 +1362,15 @@
       <c r="L18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>3373</t>
+      <c r="M18" t="n">
+        <v>3373</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>3718</t>
         </is>
       </c>
     </row>
@@ -1313,9 +1417,15 @@
       <c r="L19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>3719</t>
+      <c r="M19" t="n">
+        <v>3719</v>
+      </c>
+      <c r="N19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -1362,9 +1472,15 @@
       <c r="L20" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>3841</t>
+      <c r="M20" t="n">
+        <v>3841</v>
+      </c>
+      <c r="N20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -1411,9 +1527,15 @@
       <c r="L21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>3455</t>
+      <c r="M21" t="n">
+        <v>3455</v>
+      </c>
+      <c r="N21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>3870</t>
         </is>
       </c>
     </row>
@@ -1460,7 +1582,13 @@
       <c r="L22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="M22" t="n">
+        <v>2553</v>
+      </c>
+      <c r="N22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O22" t="inlineStr">
         <is>
           <t>2553</t>
         </is>
@@ -1509,9 +1637,15 @@
       <c r="L23" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>3216</t>
+      <c r="M23" t="n">
+        <v>3216</v>
+      </c>
+      <c r="N23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>3536</t>
         </is>
       </c>
     </row>
@@ -1558,7 +1692,13 @@
       <c r="L24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="M24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1607,9 +1747,15 @@
       <c r="L25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>2541</t>
+      <c r="M25" t="n">
+        <v>2541</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -1656,9 +1802,15 @@
       <c r="L26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>3786</t>
+      <c r="M26" t="n">
+        <v>3786</v>
+      </c>
+      <c r="N26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -1705,7 +1857,13 @@
       <c r="L27" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M27" t="n">
+        <v>2804</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr">
         <is>
           <t>2804</t>
         </is>
@@ -1754,7 +1912,13 @@
       <c r="L28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="M28" t="n">
+        <v>2523</v>
+      </c>
+      <c r="N28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O28" t="inlineStr">
         <is>
           <t>2523</t>
         </is>
@@ -1803,9 +1967,15 @@
       <c r="L29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M29" t="inlineStr">
-        <is>
-          <t>3378</t>
+      <c r="M29" t="n">
+        <v>3378</v>
+      </c>
+      <c r="N29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>3755</t>
         </is>
       </c>
     </row>
@@ -1852,7 +2022,13 @@
       <c r="L30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="M30" t="n">
+        <v>2590</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>2590</t>
         </is>
@@ -1901,9 +2077,15 @@
       <c r="L31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>3639</t>
+      <c r="M31" t="n">
+        <v>3639</v>
+      </c>
+      <c r="N31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>3959</t>
         </is>
       </c>
     </row>
@@ -1950,9 +2132,15 @@
       <c r="L32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>3528</t>
+      <c r="M32" t="n">
+        <v>3528</v>
+      </c>
+      <c r="N32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>3802</t>
         </is>
       </c>
     </row>
@@ -1999,9 +2187,15 @@
       <c r="L33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>4012</t>
+      <c r="M33" t="n">
+        <v>4012</v>
+      </c>
+      <c r="N33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>4303</t>
         </is>
       </c>
     </row>
@@ -2048,9 +2242,15 @@
       <c r="L34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M34" t="inlineStr">
-        <is>
-          <t>2717</t>
+      <c r="M34" t="n">
+        <v>2717</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>2726</t>
         </is>
       </c>
     </row>
@@ -2097,9 +2297,15 @@
       <c r="L35" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>3391</t>
+      <c r="M35" t="n">
+        <v>3391</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>3711</t>
         </is>
       </c>
     </row>
@@ -2146,9 +2352,15 @@
       <c r="L36" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="M36" t="n">
+        <v>2804</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>2896</t>
         </is>
       </c>
     </row>
@@ -2195,9 +2407,15 @@
       <c r="L37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>3787</t>
+      <c r="M37" t="n">
+        <v>3787</v>
+      </c>
+      <c r="N37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -2244,9 +2462,15 @@
       <c r="L38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>3146</t>
+      <c r="M38" t="n">
+        <v>3146</v>
+      </c>
+      <c r="N38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>3393</t>
         </is>
       </c>
     </row>
@@ -2293,9 +2517,15 @@
       <c r="L39" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>2842</t>
+      <c r="M39" t="n">
+        <v>2842</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>2904</t>
         </is>
       </c>
     </row>
@@ -2342,9 +2572,15 @@
       <c r="L40" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>3979</t>
+      <c r="M40" t="n">
+        <v>3979</v>
+      </c>
+      <c r="N40" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>4197</t>
         </is>
       </c>
     </row>
@@ -2391,9 +2627,15 @@
       <c r="L41" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>3699</t>
+      <c r="M41" t="n">
+        <v>3699</v>
+      </c>
+      <c r="N41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>4141</t>
         </is>
       </c>
     </row>
@@ -2440,9 +2682,15 @@
       <c r="L42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>3834</t>
+      <c r="M42" t="n">
+        <v>3834</v>
+      </c>
+      <c r="N42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -2489,9 +2737,15 @@
       <c r="L43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M43" t="inlineStr">
-        <is>
-          <t>3873</t>
+      <c r="M43" t="n">
+        <v>3873</v>
+      </c>
+      <c r="N43" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -2538,9 +2792,15 @@
       <c r="L44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>3442</t>
+      <c r="M44" t="n">
+        <v>3442</v>
+      </c>
+      <c r="N44" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>3577</t>
         </is>
       </c>
     </row>
@@ -2587,9 +2847,15 @@
       <c r="L45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3699</t>
+      <c r="M45" t="n">
+        <v>3699</v>
+      </c>
+      <c r="N45" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -2636,9 +2902,15 @@
       <c r="L46" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>3151</t>
+      <c r="M46" t="n">
+        <v>3151</v>
+      </c>
+      <c r="N46" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>3425</t>
         </is>
       </c>
     </row>
@@ -2685,9 +2957,15 @@
       <c r="L47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>2954</t>
+      <c r="M47" t="n">
+        <v>2954</v>
+      </c>
+      <c r="N47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -2734,9 +3012,15 @@
       <c r="L48" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>3751</t>
+      <c r="M48" t="n">
+        <v>3751</v>
+      </c>
+      <c r="N48" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>4070</t>
         </is>
       </c>
     </row>
@@ -2783,9 +3067,15 @@
       <c r="L49" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>3297</t>
+      <c r="M49" t="n">
+        <v>3297</v>
+      </c>
+      <c r="N49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>3571</t>
         </is>
       </c>
     </row>
@@ -2827,6 +3117,8 @@
       <c r="K50" t="inlineStr"/>
       <c r="L50" s="3" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
+      <c r="N50" s="3" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -2871,9 +3163,15 @@
       <c r="L51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="M51" t="n">
+        <v>3316</v>
+      </c>
+      <c r="N51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>3539</t>
         </is>
       </c>
     </row>
@@ -2920,9 +3218,15 @@
       <c r="L52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>3256</t>
+      <c r="M52" t="n">
+        <v>3256</v>
+      </c>
+      <c r="N52" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>3506</t>
         </is>
       </c>
     </row>
@@ -2969,9 +3273,15 @@
       <c r="L53" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>3416</t>
+      <c r="M53" t="n">
+        <v>3416</v>
+      </c>
+      <c r="N53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>3653</t>
         </is>
       </c>
     </row>
@@ -3018,9 +3328,15 @@
       <c r="L54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>3149</t>
+      <c r="M54" t="n">
+        <v>3149</v>
+      </c>
+      <c r="N54" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>3339</t>
         </is>
       </c>
     </row>
@@ -3067,9 +3383,15 @@
       <c r="L55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3160</t>
+      <c r="M55" t="n">
+        <v>3160</v>
+      </c>
+      <c r="N55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>3303</t>
         </is>
       </c>
     </row>
@@ -3116,9 +3438,15 @@
       <c r="L56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>3248</t>
+      <c r="M56" t="n">
+        <v>3248</v>
+      </c>
+      <c r="N56" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>3380</t>
         </is>
       </c>
     </row>
@@ -3165,9 +3493,15 @@
       <c r="L57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>3394</t>
+      <c r="M57" t="n">
+        <v>3394</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>3668</t>
         </is>
       </c>
     </row>
@@ -3214,7 +3548,13 @@
       <c r="L58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M58" t="inlineStr">
+      <c r="M58" t="n">
+        <v>0</v>
+      </c>
+      <c r="N58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3263,9 +3603,15 @@
       <c r="L59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>2539</t>
+      <c r="M59" t="n">
+        <v>2539</v>
+      </c>
+      <c r="N59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -3312,9 +3658,15 @@
       <c r="L60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>2485</t>
+      <c r="M60" t="n">
+        <v>2485</v>
+      </c>
+      <c r="N60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -3361,9 +3713,15 @@
       <c r="L61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M61" t="inlineStr">
-        <is>
-          <t>2597</t>
+      <c r="M61" t="n">
+        <v>2597</v>
+      </c>
+      <c r="N61" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>2942</t>
         </is>
       </c>
     </row>
@@ -3410,7 +3768,13 @@
       <c r="L62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M62" t="inlineStr">
+      <c r="M62" t="n">
+        <v>0</v>
+      </c>
+      <c r="N62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O62" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3442,6 +3806,8 @@
       <c r="K63" t="inlineStr"/>
       <c r="L63" s="3" t="inlineStr"/>
       <c r="M63" t="inlineStr"/>
+      <c r="N63" s="3" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3486,7 +3852,13 @@
       <c r="L64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M64" t="inlineStr">
+      <c r="M64" t="n">
+        <v>0</v>
+      </c>
+      <c r="N64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3535,11 +3907,11 @@
       <c r="L65" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>3376</t>
-        </is>
-      </c>
+      <c r="M65" t="n">
+        <v>3376</v>
+      </c>
+      <c r="N65" s="3" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3584,9 +3956,15 @@
       <c r="L66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M66" t="inlineStr">
-        <is>
-          <t>2492</t>
+      <c r="M66" t="n">
+        <v>2492</v>
+      </c>
+      <c r="N66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>2491</t>
         </is>
       </c>
     </row>
@@ -3633,9 +4011,15 @@
       <c r="L67" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M67" t="inlineStr">
-        <is>
-          <t>3796</t>
+      <c r="M67" t="n">
+        <v>3796</v>
+      </c>
+      <c r="N67" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>4031</t>
         </is>
       </c>
     </row>
@@ -3682,7 +4066,13 @@
       <c r="L68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M68" t="inlineStr">
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3731,7 +4121,13 @@
       <c r="L69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M69" t="inlineStr">
+      <c r="M69" t="n">
+        <v>0</v>
+      </c>
+      <c r="N69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3780,7 +4176,13 @@
       <c r="L70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M70" t="inlineStr">
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3829,9 +4231,15 @@
       <c r="L71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M71" t="inlineStr">
-        <is>
-          <t>2962</t>
+      <c r="M71" t="n">
+        <v>2962</v>
+      </c>
+      <c r="N71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>2993</t>
         </is>
       </c>
     </row>
@@ -3878,9 +4286,15 @@
       <c r="L72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M72" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="M72" t="n">
+        <v>2555</v>
+      </c>
+      <c r="N72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>2588</t>
         </is>
       </c>
     </row>
@@ -3927,7 +4341,13 @@
       <c r="L73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M73" t="inlineStr">
+      <c r="M73" t="n">
+        <v>0</v>
+      </c>
+      <c r="N73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3976,7 +4396,13 @@
       <c r="L74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M74" t="inlineStr">
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4024,6 +4450,8 @@
       </c>
       <c r="L75" s="3" t="inlineStr"/>
       <c r="M75" t="inlineStr"/>
+      <c r="N75" s="3" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4068,7 +4496,13 @@
       <c r="L76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M76" t="inlineStr">
+      <c r="M76" t="n">
+        <v>1499</v>
+      </c>
+      <c r="N76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O76" t="inlineStr">
         <is>
           <t>1499</t>
         </is>
@@ -4117,9 +4551,15 @@
       <c r="L77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="M77" t="n">
+        <v>2875</v>
+      </c>
+      <c r="N77" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>2942</t>
         </is>
       </c>
     </row>
@@ -4166,7 +4606,13 @@
       <c r="L78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4215,7 +4661,13 @@
       <c r="L79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M79" t="inlineStr">
+      <c r="M79" t="n">
+        <v>0</v>
+      </c>
+      <c r="N79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4264,7 +4716,13 @@
       <c r="L80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M80" t="inlineStr">
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4313,7 +4771,13 @@
       <c r="L81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M81" t="inlineStr">
+      <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4362,7 +4826,13 @@
       <c r="L82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M82" t="inlineStr">
+      <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4411,7 +4881,13 @@
       <c r="L83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M83" t="inlineStr">
+      <c r="M83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4460,7 +4936,13 @@
       <c r="L84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M84" t="inlineStr">
+      <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4509,7 +4991,13 @@
       <c r="L85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M85" t="inlineStr">
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4558,7 +5046,13 @@
       <c r="L86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M86" t="inlineStr">
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4607,7 +5101,13 @@
       <c r="L87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M87" t="inlineStr">
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4656,9 +5156,15 @@
       <c r="L88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M88" t="inlineStr">
-        <is>
-          <t>2590</t>
+      <c r="M88" t="n">
+        <v>2590</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr">
+        <is>
+          <t>2583</t>
         </is>
       </c>
     </row>
@@ -4705,7 +5211,13 @@
       <c r="L89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M89" t="inlineStr">
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4754,7 +5266,13 @@
       <c r="L90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4803,9 +5321,15 @@
       <c r="L91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="M91" t="n">
+        <v>2475</v>
+      </c>
+      <c r="N91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -4852,7 +5376,13 @@
       <c r="L92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M92" t="inlineStr">
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4901,9 +5431,15 @@
       <c r="L93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M93" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="M93" t="n">
+        <v>2998</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -4950,7 +5486,13 @@
       <c r="L94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M94" t="inlineStr">
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4999,7 +5541,13 @@
       <c r="L95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M95" t="inlineStr">
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5048,7 +5596,13 @@
       <c r="L96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
+      <c r="M96" t="n">
+        <v>0</v>
+      </c>
+      <c r="N96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5097,7 +5651,13 @@
       <c r="L97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5146,7 +5706,13 @@
       <c r="L98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M98" t="inlineStr">
+      <c r="M98" t="n">
+        <v>0</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5195,7 +5761,13 @@
       <c r="L99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M99" t="inlineStr">
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5244,7 +5816,13 @@
       <c r="L100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M100" t="inlineStr">
+      <c r="M100" t="n">
+        <v>0</v>
+      </c>
+      <c r="N100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5293,7 +5871,13 @@
       <c r="L101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M101" t="inlineStr">
+      <c r="M101" t="n">
+        <v>1499</v>
+      </c>
+      <c r="N101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="inlineStr">
         <is>
           <t>1499</t>
         </is>
@@ -5342,7 +5926,13 @@
       <c r="L102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M102" t="inlineStr">
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5391,7 +5981,13 @@
       <c r="L103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M103" t="inlineStr">
+      <c r="M103" t="n">
+        <v>0</v>
+      </c>
+      <c r="N103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5440,7 +6036,13 @@
       <c r="L104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M104" t="inlineStr">
+      <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5489,7 +6091,13 @@
       <c r="L105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M105" t="inlineStr">
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
+      <c r="N105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5538,7 +6146,13 @@
       <c r="L106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M106" t="inlineStr">
+      <c r="M106" t="n">
+        <v>0</v>
+      </c>
+      <c r="N106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5587,7 +6201,13 @@
       <c r="L107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M107" t="inlineStr">
+      <c r="M107" t="n">
+        <v>0</v>
+      </c>
+      <c r="N107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O107" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5636,7 +6256,13 @@
       <c r="L108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M108" t="inlineStr">
+      <c r="M108" t="n">
+        <v>0</v>
+      </c>
+      <c r="N108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5685,7 +6311,13 @@
       <c r="L109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M109" t="inlineStr">
+      <c r="M109" t="n">
+        <v>0</v>
+      </c>
+      <c r="N109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O109" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5734,7 +6366,13 @@
       <c r="L110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M110" t="inlineStr">
+      <c r="M110" t="n">
+        <v>0</v>
+      </c>
+      <c r="N110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5783,7 +6421,13 @@
       <c r="L111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M111" t="inlineStr">
+      <c r="M111" t="n">
+        <v>0</v>
+      </c>
+      <c r="N111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O111" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5822,9 +6466,15 @@
       <c r="L112" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>3471</t>
+      <c r="M112" t="n">
+        <v>3471</v>
+      </c>
+      <c r="N112" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O112" t="inlineStr">
+        <is>
+          <t>3815</t>
         </is>
       </c>
     </row>
@@ -5861,9 +6511,15 @@
       <c r="L113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>2620</t>
+      <c r="M113" t="n">
+        <v>2620</v>
+      </c>
+      <c r="N113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O113" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -5896,7 +6552,13 @@
       <c r="L114" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="M114" t="inlineStr">
+      <c r="M114" t="n">
+        <v>1588</v>
+      </c>
+      <c r="N114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O114" t="inlineStr">
         <is>
           <t>1588</t>
         </is>
@@ -5931,9 +6593,15 @@
       <c r="L115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>3541</t>
+      <c r="M115" t="n">
+        <v>3541</v>
+      </c>
+      <c r="N115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -5966,9 +6634,120 @@
       <c r="L116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>2865</t>
+      <c r="M116" t="n">
+        <v>2865</v>
+      </c>
+      <c r="N116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>2963</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>46422609</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>㊥林天大大神</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F117" s="3" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" s="3" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" s="3" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" s="3" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>4455</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>56100131</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>♪iran†★</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F118" s="3" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" s="3" t="inlineStr"/>
+      <c r="I118" t="inlineStr"/>
+      <c r="J118" s="3" t="inlineStr"/>
+      <c r="K118" t="inlineStr"/>
+      <c r="L118" s="3" t="inlineStr"/>
+      <c r="M118" t="inlineStr"/>
+      <c r="N118" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>2224</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>57531381</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>㊥蝦雞霸丸</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F119" s="3" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" s="3" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" s="3" t="inlineStr"/>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" s="3" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>4020</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-15 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:Q121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>04-12_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>04-14_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>04-14_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -507,6 +517,8 @@
       <c r="M2" t="inlineStr"/>
       <c r="N2" s="3" t="inlineStr"/>
       <c r="O2" t="inlineStr"/>
+      <c r="P2" s="3" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -557,7 +569,13 @@
       <c r="N3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" t="n">
+        <v>2535</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>2535</t>
         </is>
@@ -612,7 +630,13 @@
       <c r="N4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -667,9 +691,15 @@
       <c r="N5" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>3550</t>
+      <c r="O5" t="n">
+        <v>3550</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>3909</t>
         </is>
       </c>
     </row>
@@ -722,7 +752,13 @@
       <c r="N6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -777,9 +813,15 @@
       <c r="N7" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>3544</t>
+      <c r="O7" t="n">
+        <v>3544</v>
+      </c>
+      <c r="P7" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>4293</t>
         </is>
       </c>
     </row>
@@ -823,6 +865,8 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" s="3" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" s="3" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -873,9 +917,15 @@
       <c r="N9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>2920</t>
+      <c r="O9" t="n">
+        <v>2920</v>
+      </c>
+      <c r="P9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>3063</t>
         </is>
       </c>
     </row>
@@ -928,7 +978,13 @@
       <c r="N10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O10" t="inlineStr">
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -983,7 +1039,13 @@
       <c r="N11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1038,7 +1100,13 @@
       <c r="N12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1093,9 +1161,15 @@
       <c r="N13" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>3289</t>
+      <c r="O13" t="n">
+        <v>3289</v>
+      </c>
+      <c r="P13" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>3768</t>
         </is>
       </c>
     </row>
@@ -1148,9 +1222,15 @@
       <c r="N14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="O14" t="n">
+        <v>2499</v>
+      </c>
+      <c r="P14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -1203,9 +1283,15 @@
       <c r="N15" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>3536</t>
+      <c r="O15" t="n">
+        <v>3536</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -1258,7 +1344,13 @@
       <c r="N16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O16" t="inlineStr">
+      <c r="O16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q16" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1313,9 +1405,15 @@
       <c r="N17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="O17" t="n">
+        <v>3995</v>
+      </c>
+      <c r="P17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>4231</t>
         </is>
       </c>
     </row>
@@ -1368,9 +1466,15 @@
       <c r="N18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>3718</t>
+      <c r="O18" t="n">
+        <v>3718</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>4263</t>
         </is>
       </c>
     </row>
@@ -1423,9 +1527,15 @@
       <c r="N19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="O19" t="n">
+        <v>4068</v>
+      </c>
+      <c r="P19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -1478,9 +1588,15 @@
       <c r="N20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="O20" t="n">
+        <v>3995</v>
+      </c>
+      <c r="P20" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>4266</t>
         </is>
       </c>
     </row>
@@ -1533,9 +1649,15 @@
       <c r="N21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>3870</t>
+      <c r="O21" t="n">
+        <v>3870</v>
+      </c>
+      <c r="P21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>4305</t>
         </is>
       </c>
     </row>
@@ -1588,9 +1710,15 @@
       <c r="N22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>2553</t>
+      <c r="O22" t="n">
+        <v>2553</v>
+      </c>
+      <c r="P22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -1643,9 +1771,15 @@
       <c r="N23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>3536</t>
+      <c r="O23" t="n">
+        <v>3536</v>
+      </c>
+      <c r="P23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>3534</t>
         </is>
       </c>
     </row>
@@ -1698,7 +1832,13 @@
       <c r="N24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O24" t="inlineStr">
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1753,9 +1893,15 @@
       <c r="N25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="O25" t="n">
+        <v>2536</v>
+      </c>
+      <c r="P25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -1808,9 +1954,15 @@
       <c r="N26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="O26" t="n">
+        <v>3989</v>
+      </c>
+      <c r="P26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>4323</t>
         </is>
       </c>
     </row>
@@ -1863,9 +2015,15 @@
       <c r="N27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="O27" t="n">
+        <v>2804</v>
+      </c>
+      <c r="P27" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>2822</t>
         </is>
       </c>
     </row>
@@ -1918,9 +2076,15 @@
       <c r="N28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>2523</t>
+      <c r="O28" t="n">
+        <v>2523</v>
+      </c>
+      <c r="P28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -1973,9 +2137,15 @@
       <c r="N29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>3755</t>
+      <c r="O29" t="n">
+        <v>3755</v>
+      </c>
+      <c r="P29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>4205</t>
         </is>
       </c>
     </row>
@@ -2028,9 +2198,15 @@
       <c r="N30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>2590</t>
+      <c r="O30" t="n">
+        <v>2590</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>2629</t>
         </is>
       </c>
     </row>
@@ -2083,9 +2259,15 @@
       <c r="N31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>3959</t>
+      <c r="O31" t="n">
+        <v>3959</v>
+      </c>
+      <c r="P31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -2138,9 +2320,15 @@
       <c r="N32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>3802</t>
+      <c r="O32" t="n">
+        <v>3802</v>
+      </c>
+      <c r="P32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>4094</t>
         </is>
       </c>
     </row>
@@ -2193,9 +2381,15 @@
       <c r="N33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>4303</t>
+      <c r="O33" t="n">
+        <v>4303</v>
+      </c>
+      <c r="P33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>4687</t>
         </is>
       </c>
     </row>
@@ -2248,9 +2442,15 @@
       <c r="N34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>2726</t>
+      <c r="O34" t="n">
+        <v>2726</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>2711</t>
         </is>
       </c>
     </row>
@@ -2303,9 +2503,15 @@
       <c r="N35" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>3711</t>
+      <c r="O35" t="n">
+        <v>3711</v>
+      </c>
+      <c r="P35" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -2358,9 +2564,15 @@
       <c r="N36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="O36" t="n">
+        <v>2896</v>
+      </c>
+      <c r="P36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>2962</t>
         </is>
       </c>
     </row>
@@ -2413,9 +2625,15 @@
       <c r="N37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="O37" t="n">
+        <v>3994</v>
+      </c>
+      <c r="P37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>4491</t>
         </is>
       </c>
     </row>
@@ -2468,9 +2686,15 @@
       <c r="N38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>3393</t>
+      <c r="O38" t="n">
+        <v>3393</v>
+      </c>
+      <c r="P38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>3771</t>
         </is>
       </c>
     </row>
@@ -2523,9 +2747,15 @@
       <c r="N39" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>2904</t>
+      <c r="O39" t="n">
+        <v>2904</v>
+      </c>
+      <c r="P39" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -2578,9 +2808,15 @@
       <c r="N40" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>4197</t>
+      <c r="O40" t="n">
+        <v>4197</v>
+      </c>
+      <c r="P40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>4595</t>
         </is>
       </c>
     </row>
@@ -2633,9 +2869,15 @@
       <c r="N41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>4141</t>
+      <c r="O41" t="n">
+        <v>4141</v>
+      </c>
+      <c r="P41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>4494</t>
         </is>
       </c>
     </row>
@@ -2688,9 +2930,15 @@
       <c r="N42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>3985</t>
+      <c r="O42" t="n">
+        <v>3985</v>
+      </c>
+      <c r="P42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>4126</t>
         </is>
       </c>
     </row>
@@ -2743,9 +2991,15 @@
       <c r="N43" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="O43" t="n">
+        <v>3998</v>
+      </c>
+      <c r="P43" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>4298</t>
         </is>
       </c>
     </row>
@@ -2798,9 +3052,15 @@
       <c r="N44" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>3577</t>
+      <c r="O44" t="n">
+        <v>3577</v>
+      </c>
+      <c r="P44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -2853,9 +3113,15 @@
       <c r="N45" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="O45" t="n">
+        <v>3988</v>
+      </c>
+      <c r="P45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>4258</t>
         </is>
       </c>
     </row>
@@ -2908,9 +3174,15 @@
       <c r="N46" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>3425</t>
+      <c r="O46" t="n">
+        <v>3425</v>
+      </c>
+      <c r="P46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>4054</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3235,15 @@
       <c r="N47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="O47" t="n">
+        <v>2952</v>
+      </c>
+      <c r="P47" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -3018,9 +3296,15 @@
       <c r="N48" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>4070</t>
+      <c r="O48" t="n">
+        <v>4070</v>
+      </c>
+      <c r="P48" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>4404</t>
         </is>
       </c>
     </row>
@@ -3030,7 +3314,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Globalking1001</t>
+          <t>Globalking</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -3073,9 +3357,15 @@
       <c r="N49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>3571</t>
+      <c r="O49" t="n">
+        <v>3571</v>
+      </c>
+      <c r="P49" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>3937</t>
         </is>
       </c>
     </row>
@@ -3119,6 +3409,8 @@
       <c r="M50" t="inlineStr"/>
       <c r="N50" s="3" t="inlineStr"/>
       <c r="O50" t="inlineStr"/>
+      <c r="P50" s="3" t="inlineStr"/>
+      <c r="Q50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3169,9 +3461,15 @@
       <c r="N51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>3539</t>
+      <c r="O51" t="n">
+        <v>3539</v>
+      </c>
+      <c r="P51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>4006</t>
         </is>
       </c>
     </row>
@@ -3224,9 +3522,15 @@
       <c r="N52" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>3506</t>
+      <c r="O52" t="n">
+        <v>3506</v>
+      </c>
+      <c r="P52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>3898</t>
         </is>
       </c>
     </row>
@@ -3279,9 +3583,15 @@
       <c r="N53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>3653</t>
+      <c r="O53" t="n">
+        <v>3653</v>
+      </c>
+      <c r="P53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -3334,9 +3644,15 @@
       <c r="N54" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="O54" t="n">
+        <v>3339</v>
+      </c>
+      <c r="P54" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>3621</t>
         </is>
       </c>
     </row>
@@ -3389,9 +3705,15 @@
       <c r="N55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>3303</t>
+      <c r="O55" t="n">
+        <v>3303</v>
+      </c>
+      <c r="P55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>3837</t>
         </is>
       </c>
     </row>
@@ -3444,9 +3766,15 @@
       <c r="N56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>3380</t>
+      <c r="O56" t="n">
+        <v>3380</v>
+      </c>
+      <c r="P56" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>3865</t>
         </is>
       </c>
     </row>
@@ -3499,9 +3827,15 @@
       <c r="N57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>3668</t>
+      <c r="O57" t="n">
+        <v>3668</v>
+      </c>
+      <c r="P57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>3979</t>
         </is>
       </c>
     </row>
@@ -3554,7 +3888,13 @@
       <c r="N58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O58" t="inlineStr">
+      <c r="O58" t="n">
+        <v>0</v>
+      </c>
+      <c r="P58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3609,9 +3949,15 @@
       <c r="N59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>2536</t>
+      <c r="O59" t="n">
+        <v>2536</v>
+      </c>
+      <c r="P59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>2615</t>
         </is>
       </c>
     </row>
@@ -3664,9 +4010,15 @@
       <c r="N60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="O60" t="n">
+        <v>2489</v>
+      </c>
+      <c r="P60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>2481</t>
         </is>
       </c>
     </row>
@@ -3719,9 +4071,15 @@
       <c r="N61" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>2942</t>
+      <c r="O61" t="n">
+        <v>2942</v>
+      </c>
+      <c r="P61" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>3371</t>
         </is>
       </c>
     </row>
@@ -3774,9 +4132,15 @@
       <c r="N62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O62" t="n">
+        <v>0</v>
+      </c>
+      <c r="P62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>1991</t>
         </is>
       </c>
     </row>
@@ -3808,6 +4172,8 @@
       <c r="M63" t="inlineStr"/>
       <c r="N63" s="3" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
+      <c r="P63" s="3" t="inlineStr"/>
+      <c r="Q63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -3858,7 +4224,13 @@
       <c r="N64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O64" t="inlineStr">
+      <c r="O64" t="n">
+        <v>0</v>
+      </c>
+      <c r="P64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3912,6 +4284,8 @@
       </c>
       <c r="N65" s="3" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
+      <c r="P65" s="3" t="inlineStr"/>
+      <c r="Q65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -3962,9 +4336,15 @@
       <c r="N66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>2491</t>
+      <c r="O66" t="n">
+        <v>2491</v>
+      </c>
+      <c r="P66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -4017,9 +4397,15 @@
       <c r="N67" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>4031</t>
+      <c r="O67" t="n">
+        <v>4031</v>
+      </c>
+      <c r="P67" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>4526</t>
         </is>
       </c>
     </row>
@@ -4072,7 +4458,13 @@
       <c r="N68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O68" t="inlineStr">
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4127,7 +4519,13 @@
       <c r="N69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O69" t="inlineStr">
+      <c r="O69" t="n">
+        <v>0</v>
+      </c>
+      <c r="P69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q69" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4182,7 +4580,13 @@
       <c r="N70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O70" t="inlineStr">
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4237,9 +4641,15 @@
       <c r="N71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="O71" t="n">
+        <v>2993</v>
+      </c>
+      <c r="P71" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>3357</t>
         </is>
       </c>
     </row>
@@ -4292,9 +4702,15 @@
       <c r="N72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>2588</t>
+      <c r="O72" t="n">
+        <v>2588</v>
+      </c>
+      <c r="P72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>2603</t>
         </is>
       </c>
     </row>
@@ -4347,7 +4763,13 @@
       <c r="N73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O73" t="inlineStr">
+      <c r="O73" t="n">
+        <v>0</v>
+      </c>
+      <c r="P73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4402,7 +4824,13 @@
       <c r="N74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="inlineStr">
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4452,6 +4880,8 @@
       <c r="M75" t="inlineStr"/>
       <c r="N75" s="3" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
+      <c r="P75" s="3" t="inlineStr"/>
+      <c r="Q75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4502,9 +4932,15 @@
       <c r="N76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>1499</t>
+      <c r="O76" t="n">
+        <v>1499</v>
+      </c>
+      <c r="P76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>1497</t>
         </is>
       </c>
     </row>
@@ -4557,9 +4993,15 @@
       <c r="N77" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>2942</t>
+      <c r="O77" t="n">
+        <v>2942</v>
+      </c>
+      <c r="P77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>2998</t>
         </is>
       </c>
     </row>
@@ -4612,7 +5054,13 @@
       <c r="N78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O78" t="inlineStr">
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4667,7 +5115,13 @@
       <c r="N79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O79" t="inlineStr">
+      <c r="O79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4722,9 +5176,15 @@
       <c r="N80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>1424</t>
         </is>
       </c>
     </row>
@@ -4777,7 +5237,13 @@
       <c r="N81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O81" t="inlineStr">
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4832,7 +5298,13 @@
       <c r="N82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O82" t="inlineStr">
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4887,7 +5359,13 @@
       <c r="N83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O83" t="inlineStr">
+      <c r="O83" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4942,7 +5420,13 @@
       <c r="N84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O84" t="inlineStr">
+      <c r="O84" t="n">
+        <v>0</v>
+      </c>
+      <c r="P84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4997,7 +5481,13 @@
       <c r="N85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O85" t="inlineStr">
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5052,7 +5542,13 @@
       <c r="N86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O86" t="inlineStr">
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5107,7 +5603,13 @@
       <c r="N87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O87" t="inlineStr">
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5162,9 +5664,15 @@
       <c r="N88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="O88" t="n">
+        <v>2583</v>
+      </c>
+      <c r="P88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>2616</t>
         </is>
       </c>
     </row>
@@ -5217,7 +5725,13 @@
       <c r="N89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O89" t="inlineStr">
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5272,7 +5786,13 @@
       <c r="N90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O90" t="inlineStr">
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5327,9 +5847,15 @@
       <c r="N91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="O91" t="n">
+        <v>2515</v>
+      </c>
+      <c r="P91" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>2581</t>
         </is>
       </c>
     </row>
@@ -5382,7 +5908,13 @@
       <c r="N92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5437,9 +5969,15 @@
       <c r="N93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="O93" t="n">
+        <v>2985</v>
+      </c>
+      <c r="P93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>3510</t>
         </is>
       </c>
     </row>
@@ -5492,7 +6030,13 @@
       <c r="N94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O94" t="inlineStr">
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5547,7 +6091,13 @@
       <c r="N95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O95" t="inlineStr">
+      <c r="O95" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5602,7 +6152,13 @@
       <c r="N96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O96" t="inlineStr">
+      <c r="O96" t="n">
+        <v>0</v>
+      </c>
+      <c r="P96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5657,7 +6213,13 @@
       <c r="N97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O97" t="inlineStr">
+      <c r="O97" t="n">
+        <v>0</v>
+      </c>
+      <c r="P97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5712,7 +6274,13 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
+      <c r="O98" t="n">
+        <v>0</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5767,7 +6335,13 @@
       <c r="N99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O99" t="inlineStr">
+      <c r="O99" t="n">
+        <v>0</v>
+      </c>
+      <c r="P99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5822,7 +6396,13 @@
       <c r="N100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O100" t="inlineStr">
+      <c r="O100" t="n">
+        <v>0</v>
+      </c>
+      <c r="P100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5877,7 +6457,13 @@
       <c r="N101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O101" t="inlineStr">
+      <c r="O101" t="n">
+        <v>1499</v>
+      </c>
+      <c r="P101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="inlineStr">
         <is>
           <t>1499</t>
         </is>
@@ -5932,7 +6518,13 @@
       <c r="N102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O102" t="inlineStr">
+      <c r="O102" t="n">
+        <v>0</v>
+      </c>
+      <c r="P102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5987,7 +6579,13 @@
       <c r="N103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O103" t="inlineStr">
+      <c r="O103" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6042,7 +6640,13 @@
       <c r="N104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O104" t="inlineStr">
+      <c r="O104" t="n">
+        <v>0</v>
+      </c>
+      <c r="P104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6097,7 +6701,13 @@
       <c r="N105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O105" t="inlineStr">
+      <c r="O105" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6152,7 +6762,13 @@
       <c r="N106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O106" t="inlineStr">
+      <c r="O106" t="n">
+        <v>0</v>
+      </c>
+      <c r="P106" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q106" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6207,7 +6823,13 @@
       <c r="N107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O107" t="inlineStr">
+      <c r="O107" t="n">
+        <v>0</v>
+      </c>
+      <c r="P107" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q107" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6262,7 +6884,13 @@
       <c r="N108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O108" t="inlineStr">
+      <c r="O108" t="n">
+        <v>0</v>
+      </c>
+      <c r="P108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q108" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6317,7 +6945,13 @@
       <c r="N109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O109" t="inlineStr">
+      <c r="O109" t="n">
+        <v>0</v>
+      </c>
+      <c r="P109" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q109" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6372,7 +7006,13 @@
       <c r="N110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O110" t="inlineStr">
+      <c r="O110" t="n">
+        <v>0</v>
+      </c>
+      <c r="P110" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q110" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6427,7 +7067,13 @@
       <c r="N111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O111" t="inlineStr">
+      <c r="O111" t="n">
+        <v>0</v>
+      </c>
+      <c r="P111" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q111" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6472,9 +7118,15 @@
       <c r="N112" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O112" t="inlineStr">
-        <is>
-          <t>3815</t>
+      <c r="O112" t="n">
+        <v>3815</v>
+      </c>
+      <c r="P112" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>4330</t>
         </is>
       </c>
     </row>
@@ -6517,9 +7169,15 @@
       <c r="N113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O113" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="O113" t="n">
+        <v>2692</v>
+      </c>
+      <c r="P113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -6558,9 +7216,15 @@
       <c r="N114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O114" t="inlineStr">
-        <is>
-          <t>1588</t>
+      <c r="O114" t="n">
+        <v>1588</v>
+      </c>
+      <c r="P114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>1587</t>
         </is>
       </c>
     </row>
@@ -6599,9 +7263,15 @@
       <c r="N115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>3779</t>
+      <c r="O115" t="n">
+        <v>3779</v>
+      </c>
+      <c r="P115" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>4427</t>
         </is>
       </c>
     </row>
@@ -6640,17 +7310,21 @@
       <c r="N116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="O116" t="n">
+        <v>2963</v>
+      </c>
+      <c r="P116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>3366</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>46422609</t>
-        </is>
+      <c r="A117" t="n">
+        <v>46422609</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -6675,17 +7349,15 @@
       <c r="N117" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>4455</t>
-        </is>
-      </c>
+      <c r="O117" t="n">
+        <v>4455</v>
+      </c>
+      <c r="P117" s="3" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>56100131</t>
-        </is>
+      <c r="A118" t="n">
+        <v>56100131</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -6710,17 +7382,21 @@
       <c r="N118" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>2224</t>
+      <c r="O118" t="n">
+        <v>2224</v>
+      </c>
+      <c r="P118" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>57531381</t>
-        </is>
+      <c r="A119" t="n">
+        <v>57531381</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -6745,9 +7421,83 @@
       <c r="N119" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>4020</t>
+      <c r="O119" t="n">
+        <v>4020</v>
+      </c>
+      <c r="P119" s="3" t="inlineStr"/>
+      <c r="Q119" t="inlineStr"/>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>59166269</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Player-59166269</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F120" s="3" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" s="3" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" s="3" t="inlineStr"/>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" s="3" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" s="3" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>1375</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>15695258</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Player-15695258</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F121" s="3" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" s="3" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" s="3" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
+      <c r="L121" s="3" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" s="3" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-16 11:30:59
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q121"/>
+  <dimension ref="A1:S123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>04-14_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>04-15_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>04-15_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -519,6 +529,8 @@
       <c r="O2" t="inlineStr"/>
       <c r="P2" s="3" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
+      <c r="R2" s="3" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -575,7 +587,13 @@
       <c r="P3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" t="n">
+        <v>2535</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>2535</t>
         </is>
@@ -636,7 +654,13 @@
       <c r="P4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -697,9 +721,15 @@
       <c r="P5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>3909</t>
+      <c r="Q5" t="n">
+        <v>3909</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>3979</t>
         </is>
       </c>
     </row>
@@ -758,9 +788,15 @@
       <c r="P6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -819,9 +855,15 @@
       <c r="P7" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>4293</t>
+      <c r="Q7" t="n">
+        <v>4293</v>
+      </c>
+      <c r="R7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -867,6 +909,8 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" s="3" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
+      <c r="R8" s="3" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -923,9 +967,15 @@
       <c r="P9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>3063</t>
+      <c r="Q9" t="n">
+        <v>3063</v>
+      </c>
+      <c r="R9" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>3163</t>
         </is>
       </c>
     </row>
@@ -984,7 +1034,13 @@
       <c r="P10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1045,7 +1101,13 @@
       <c r="P11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q11" t="inlineStr">
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1106,7 +1168,13 @@
       <c r="P12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q12" t="inlineStr">
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1167,9 +1235,15 @@
       <c r="P13" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>3768</t>
+      <c r="Q13" t="n">
+        <v>3768</v>
+      </c>
+      <c r="R13" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>3911</t>
         </is>
       </c>
     </row>
@@ -1228,9 +1302,15 @@
       <c r="P14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="Q14" t="n">
+        <v>2686</v>
+      </c>
+      <c r="R14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -1289,9 +1369,15 @@
       <c r="P15" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="Q15" t="n">
+        <v>3993</v>
+      </c>
+      <c r="R15" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>4082</t>
         </is>
       </c>
     </row>
@@ -1350,7 +1436,13 @@
       <c r="P16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" t="inlineStr">
+      <c r="Q16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S16" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1411,9 +1503,15 @@
       <c r="P17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>4231</t>
+      <c r="Q17" t="n">
+        <v>4231</v>
+      </c>
+      <c r="R17" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>4462</t>
         </is>
       </c>
     </row>
@@ -1472,9 +1570,15 @@
       <c r="P18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>4263</t>
+      <c r="Q18" t="n">
+        <v>4263</v>
+      </c>
+      <c r="R18" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>4499</t>
         </is>
       </c>
     </row>
@@ -1533,9 +1637,15 @@
       <c r="P19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>4725</t>
+      <c r="Q19" t="n">
+        <v>4725</v>
+      </c>
+      <c r="R19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>4897</t>
         </is>
       </c>
     </row>
@@ -1594,9 +1704,15 @@
       <c r="P20" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>4266</t>
+      <c r="Q20" t="n">
+        <v>4266</v>
+      </c>
+      <c r="R20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>4395</t>
         </is>
       </c>
     </row>
@@ -1655,9 +1771,15 @@
       <c r="P21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>4305</t>
+      <c r="Q21" t="n">
+        <v>4305</v>
+      </c>
+      <c r="R21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>4652</t>
         </is>
       </c>
     </row>
@@ -1716,9 +1838,15 @@
       <c r="P22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="Q22" t="n">
+        <v>2567</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -1777,9 +1905,15 @@
       <c r="P23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>3534</t>
+      <c r="Q23" t="n">
+        <v>3534</v>
+      </c>
+      <c r="R23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>3828</t>
         </is>
       </c>
     </row>
@@ -1838,7 +1972,13 @@
       <c r="P24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q24" t="inlineStr">
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1899,9 +2039,15 @@
       <c r="P25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="Q25" t="n">
+        <v>2548</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>2577</t>
         </is>
       </c>
     </row>
@@ -1960,9 +2106,15 @@
       <c r="P26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>4323</t>
+      <c r="Q26" t="n">
+        <v>4323</v>
+      </c>
+      <c r="R26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>4538</t>
         </is>
       </c>
     </row>
@@ -2021,7 +2173,13 @@
       <c r="P27" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="Q27" t="n">
+        <v>2822</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>2822</t>
         </is>
@@ -2082,7 +2240,13 @@
       <c r="P28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q28" t="inlineStr">
+      <c r="Q28" t="n">
+        <v>2570</v>
+      </c>
+      <c r="R28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S28" t="inlineStr">
         <is>
           <t>2570</t>
         </is>
@@ -2143,9 +2307,15 @@
       <c r="P29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>4205</t>
+      <c r="Q29" t="n">
+        <v>4205</v>
+      </c>
+      <c r="R29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>4365</t>
         </is>
       </c>
     </row>
@@ -2204,9 +2374,15 @@
       <c r="P30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>2629</t>
+      <c r="Q30" t="n">
+        <v>2629</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -2265,9 +2441,15 @@
       <c r="P31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="Q31" t="n">
+        <v>4135</v>
+      </c>
+      <c r="R31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>4314</t>
         </is>
       </c>
     </row>
@@ -2326,9 +2508,15 @@
       <c r="P32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>4094</t>
+      <c r="Q32" t="n">
+        <v>4094</v>
+      </c>
+      <c r="R32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>4302</t>
         </is>
       </c>
     </row>
@@ -2387,9 +2575,15 @@
       <c r="P33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>4687</t>
+      <c r="Q33" t="n">
+        <v>4687</v>
+      </c>
+      <c r="R33" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>4831</t>
         </is>
       </c>
     </row>
@@ -2448,9 +2642,15 @@
       <c r="P34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>2711</t>
+      <c r="Q34" t="n">
+        <v>2711</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>2721</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2709,15 @@
       <c r="P35" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="Q35" t="n">
+        <v>3989</v>
+      </c>
+      <c r="R35" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>4170</t>
         </is>
       </c>
     </row>
@@ -2570,9 +2776,15 @@
       <c r="P36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>2962</t>
+      <c r="Q36" t="n">
+        <v>2962</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>3042</t>
         </is>
       </c>
     </row>
@@ -2631,9 +2843,15 @@
       <c r="P37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>4491</t>
+      <c r="Q37" t="n">
+        <v>4491</v>
+      </c>
+      <c r="R37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>4687</t>
         </is>
       </c>
     </row>
@@ -2692,9 +2910,15 @@
       <c r="P38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>3771</t>
+      <c r="Q38" t="n">
+        <v>3771</v>
+      </c>
+      <c r="R38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -2753,9 +2977,15 @@
       <c r="P39" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="Q39" t="n">
+        <v>3123</v>
+      </c>
+      <c r="R39" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>3174</t>
         </is>
       </c>
     </row>
@@ -2814,9 +3044,15 @@
       <c r="P40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>4595</t>
+      <c r="Q40" t="n">
+        <v>4595</v>
+      </c>
+      <c r="R40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>4806</t>
         </is>
       </c>
     </row>
@@ -2875,9 +3111,15 @@
       <c r="P41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>4494</t>
+      <c r="Q41" t="n">
+        <v>4494</v>
+      </c>
+      <c r="R41" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>4781</t>
         </is>
       </c>
     </row>
@@ -2936,9 +3178,15 @@
       <c r="P42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>4126</t>
+      <c r="Q42" t="n">
+        <v>4126</v>
+      </c>
+      <c r="R42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>4370</t>
         </is>
       </c>
     </row>
@@ -2997,9 +3245,15 @@
       <c r="P43" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>4298</t>
+      <c r="Q43" t="n">
+        <v>4298</v>
+      </c>
+      <c r="R43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>4457</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3312,15 @@
       <c r="P44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="Q44" t="n">
+        <v>3982</v>
+      </c>
+      <c r="R44" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>4187</t>
         </is>
       </c>
     </row>
@@ -3119,9 +3379,15 @@
       <c r="P45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>4258</t>
+      <c r="Q45" t="n">
+        <v>4258</v>
+      </c>
+      <c r="R45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -3180,9 +3446,15 @@
       <c r="P46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>4054</t>
+      <c r="Q46" t="n">
+        <v>4054</v>
+      </c>
+      <c r="R46" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>4254</t>
         </is>
       </c>
     </row>
@@ -3241,9 +3513,15 @@
       <c r="P47" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="Q47" t="n">
+        <v>3047</v>
+      </c>
+      <c r="R47" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>3252</t>
         </is>
       </c>
     </row>
@@ -3302,9 +3580,15 @@
       <c r="P48" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>4404</t>
+      <c r="Q48" t="n">
+        <v>4404</v>
+      </c>
+      <c r="R48" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>4703</t>
         </is>
       </c>
     </row>
@@ -3363,9 +3647,15 @@
       <c r="P49" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>3937</t>
+      <c r="Q49" t="n">
+        <v>3937</v>
+      </c>
+      <c r="R49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>4029</t>
         </is>
       </c>
     </row>
@@ -3411,6 +3701,8 @@
       <c r="O50" t="inlineStr"/>
       <c r="P50" s="3" t="inlineStr"/>
       <c r="Q50" t="inlineStr"/>
+      <c r="R50" s="3" t="inlineStr"/>
+      <c r="S50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3467,9 +3759,15 @@
       <c r="P51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>4006</t>
+      <c r="Q51" t="n">
+        <v>4006</v>
+      </c>
+      <c r="R51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>4042</t>
         </is>
       </c>
     </row>
@@ -3528,9 +3826,15 @@
       <c r="P52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>3898</t>
+      <c r="Q52" t="n">
+        <v>3898</v>
+      </c>
+      <c r="R52" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>4004</t>
         </is>
       </c>
     </row>
@@ -3589,9 +3893,15 @@
       <c r="P53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="Q53" t="n">
+        <v>3995</v>
+      </c>
+      <c r="R53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -3650,9 +3960,15 @@
       <c r="P54" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="Q54" t="n">
+        <v>3621</v>
+      </c>
+      <c r="R54" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>3590</t>
         </is>
       </c>
     </row>
@@ -3711,9 +4027,15 @@
       <c r="P55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>3837</t>
+      <c r="Q55" t="n">
+        <v>3837</v>
+      </c>
+      <c r="R55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>3913</t>
         </is>
       </c>
     </row>
@@ -3772,9 +4094,15 @@
       <c r="P56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>3865</t>
+      <c r="Q56" t="n">
+        <v>3865</v>
+      </c>
+      <c r="R56" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -3833,9 +4161,15 @@
       <c r="P57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>3979</t>
+      <c r="Q57" t="n">
+        <v>3979</v>
+      </c>
+      <c r="R57" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -3894,7 +4228,13 @@
       <c r="P58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q58" t="inlineStr">
+      <c r="Q58" t="n">
+        <v>0</v>
+      </c>
+      <c r="R58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3955,9 +4295,15 @@
       <c r="P59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>2615</t>
+      <c r="Q59" t="n">
+        <v>2615</v>
+      </c>
+      <c r="R59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -4016,9 +4362,15 @@
       <c r="P60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="Q60" t="n">
+        <v>2481</v>
+      </c>
+      <c r="R60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -4077,9 +4429,15 @@
       <c r="P61" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>3371</t>
+      <c r="Q61" t="n">
+        <v>3371</v>
+      </c>
+      <c r="R61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>3369</t>
         </is>
       </c>
     </row>
@@ -4138,9 +4496,15 @@
       <c r="P62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>1991</t>
+      <c r="Q62" t="n">
+        <v>1991</v>
+      </c>
+      <c r="R62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>1986</t>
         </is>
       </c>
     </row>
@@ -4174,6 +4538,8 @@
       <c r="O63" t="inlineStr"/>
       <c r="P63" s="3" t="inlineStr"/>
       <c r="Q63" t="inlineStr"/>
+      <c r="R63" s="3" t="inlineStr"/>
+      <c r="S63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4230,7 +4596,13 @@
       <c r="P64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q64" t="inlineStr">
+      <c r="Q64" t="n">
+        <v>0</v>
+      </c>
+      <c r="R64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4286,6 +4658,8 @@
       <c r="O65" t="inlineStr"/>
       <c r="P65" s="3" t="inlineStr"/>
       <c r="Q65" t="inlineStr"/>
+      <c r="R65" s="3" t="inlineStr"/>
+      <c r="S65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4342,9 +4716,15 @@
       <c r="P66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="Q66" t="n">
+        <v>2487</v>
+      </c>
+      <c r="R66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>2486</t>
         </is>
       </c>
     </row>
@@ -4403,9 +4783,15 @@
       <c r="P67" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>4526</t>
+      <c r="Q67" t="n">
+        <v>4526</v>
+      </c>
+      <c r="R67" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>4697</t>
         </is>
       </c>
     </row>
@@ -4464,7 +4850,13 @@
       <c r="P68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q68" t="inlineStr">
+      <c r="Q68" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4525,9 +4917,15 @@
       <c r="P69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q69" t="n">
+        <v>0</v>
+      </c>
+      <c r="R69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -4586,7 +4984,13 @@
       <c r="P70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q70" t="inlineStr">
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4647,9 +5051,15 @@
       <c r="P71" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>3357</t>
+      <c r="Q71" t="n">
+        <v>3357</v>
+      </c>
+      <c r="R71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>3375</t>
         </is>
       </c>
     </row>
@@ -4708,9 +5118,15 @@
       <c r="P72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>2603</t>
+      <c r="Q72" t="n">
+        <v>2603</v>
+      </c>
+      <c r="R72" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>2851</t>
         </is>
       </c>
     </row>
@@ -4769,7 +5185,13 @@
       <c r="P73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q73" t="inlineStr">
+      <c r="Q73" t="n">
+        <v>0</v>
+      </c>
+      <c r="R73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4830,7 +5252,13 @@
       <c r="P74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q74" t="inlineStr">
+      <c r="Q74" t="n">
+        <v>0</v>
+      </c>
+      <c r="R74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4882,6 +5310,8 @@
       <c r="O75" t="inlineStr"/>
       <c r="P75" s="3" t="inlineStr"/>
       <c r="Q75" t="inlineStr"/>
+      <c r="R75" s="3" t="inlineStr"/>
+      <c r="S75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -4938,9 +5368,15 @@
       <c r="P76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>1497</t>
+      <c r="Q76" t="n">
+        <v>1497</v>
+      </c>
+      <c r="R76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4999,9 +5435,15 @@
       <c r="P77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>2998</t>
+      <c r="Q77" t="n">
+        <v>2998</v>
+      </c>
+      <c r="R77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>2990</t>
         </is>
       </c>
     </row>
@@ -5060,7 +5502,13 @@
       <c r="P78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q78" t="inlineStr">
+      <c r="Q78" t="n">
+        <v>0</v>
+      </c>
+      <c r="R78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5121,7 +5569,13 @@
       <c r="P79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q79" t="inlineStr">
+      <c r="Q79" t="n">
+        <v>0</v>
+      </c>
+      <c r="R79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5182,9 +5636,15 @@
       <c r="P80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>1424</t>
+      <c r="Q80" t="n">
+        <v>1424</v>
+      </c>
+      <c r="R80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>1454</t>
         </is>
       </c>
     </row>
@@ -5243,7 +5703,13 @@
       <c r="P81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q81" t="inlineStr">
+      <c r="Q81" t="n">
+        <v>0</v>
+      </c>
+      <c r="R81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5304,7 +5770,13 @@
       <c r="P82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q82" t="inlineStr">
+      <c r="Q82" t="n">
+        <v>0</v>
+      </c>
+      <c r="R82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5365,7 +5837,13 @@
       <c r="P83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q83" t="inlineStr">
+      <c r="Q83" t="n">
+        <v>0</v>
+      </c>
+      <c r="R83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5426,7 +5904,13 @@
       <c r="P84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q84" t="inlineStr">
+      <c r="Q84" t="n">
+        <v>0</v>
+      </c>
+      <c r="R84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5487,7 +5971,13 @@
       <c r="P85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q85" t="inlineStr">
+      <c r="Q85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5548,7 +6038,13 @@
       <c r="P86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q86" t="inlineStr">
+      <c r="Q86" t="n">
+        <v>0</v>
+      </c>
+      <c r="R86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5609,7 +6105,13 @@
       <c r="P87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q87" t="inlineStr">
+      <c r="Q87" t="n">
+        <v>0</v>
+      </c>
+      <c r="R87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5634,7 +6136,7 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>三馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F88" s="2" t="n">
@@ -5670,9 +6172,15 @@
       <c r="P88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>2616</t>
+      <c r="Q88" t="n">
+        <v>2616</v>
+      </c>
+      <c r="R88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>2626</t>
         </is>
       </c>
     </row>
@@ -5731,7 +6239,13 @@
       <c r="P89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q89" t="inlineStr">
+      <c r="Q89" t="n">
+        <v>0</v>
+      </c>
+      <c r="R89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5792,7 +6306,13 @@
       <c r="P90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q90" t="inlineStr">
+      <c r="Q90" t="n">
+        <v>0</v>
+      </c>
+      <c r="R90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5853,11 +6373,11 @@
       <c r="P91" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>2581</t>
-        </is>
-      </c>
+      <c r="Q91" t="n">
+        <v>2581</v>
+      </c>
+      <c r="R91" s="3" t="inlineStr"/>
+      <c r="S91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -5914,7 +6434,13 @@
       <c r="P92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr">
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5975,9 +6501,15 @@
       <c r="P93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>3510</t>
+      <c r="Q93" t="n">
+        <v>3510</v>
+      </c>
+      <c r="R93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>3485</t>
         </is>
       </c>
     </row>
@@ -6036,7 +6568,13 @@
       <c r="P94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q94" t="inlineStr">
+      <c r="Q94" t="n">
+        <v>0</v>
+      </c>
+      <c r="R94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6097,7 +6635,13 @@
       <c r="P95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q95" t="inlineStr">
+      <c r="Q95" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6158,7 +6702,13 @@
       <c r="P96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q96" t="inlineStr">
+      <c r="Q96" t="n">
+        <v>0</v>
+      </c>
+      <c r="R96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6219,7 +6769,13 @@
       <c r="P97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr">
+      <c r="Q97" t="n">
+        <v>0</v>
+      </c>
+      <c r="R97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6280,7 +6836,13 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
+      <c r="Q98" t="n">
+        <v>0</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6341,7 +6903,13 @@
       <c r="P99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q99" t="inlineStr">
+      <c r="Q99" t="n">
+        <v>0</v>
+      </c>
+      <c r="R99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6402,7 +6970,13 @@
       <c r="P100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q100" t="inlineStr">
+      <c r="Q100" t="n">
+        <v>0</v>
+      </c>
+      <c r="R100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6463,9 +7037,15 @@
       <c r="P101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q101" t="inlineStr">
-        <is>
-          <t>1499</t>
+      <c r="Q101" t="n">
+        <v>1499</v>
+      </c>
+      <c r="R101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -6524,7 +7104,13 @@
       <c r="P102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q102" t="inlineStr">
+      <c r="Q102" t="n">
+        <v>0</v>
+      </c>
+      <c r="R102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6585,11 +7171,11 @@
       <c r="P103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q103" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q103" t="n">
+        <v>0</v>
+      </c>
+      <c r="R103" s="3" t="inlineStr"/>
+      <c r="S103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -6646,11 +7232,11 @@
       <c r="P104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q104" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q104" t="n">
+        <v>0</v>
+      </c>
+      <c r="R104" s="3" t="inlineStr"/>
+      <c r="S104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -6707,11 +7293,11 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q105" t="n">
+        <v>0</v>
+      </c>
+      <c r="R105" s="3" t="inlineStr"/>
+      <c r="S105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -6768,11 +7354,11 @@
       <c r="P106" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q106" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q106" t="n">
+        <v>0</v>
+      </c>
+      <c r="R106" s="3" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6829,11 +7415,11 @@
       <c r="P107" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q107" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q107" t="n">
+        <v>0</v>
+      </c>
+      <c r="R107" s="3" t="inlineStr"/>
+      <c r="S107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6890,11 +7476,11 @@
       <c r="P108" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q108" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q108" t="n">
+        <v>0</v>
+      </c>
+      <c r="R108" s="3" t="inlineStr"/>
+      <c r="S108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6951,11 +7537,11 @@
       <c r="P109" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q109" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q109" t="n">
+        <v>0</v>
+      </c>
+      <c r="R109" s="3" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -7012,11 +7598,11 @@
       <c r="P110" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q110" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q110" t="n">
+        <v>0</v>
+      </c>
+      <c r="R110" s="3" t="inlineStr"/>
+      <c r="S110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7073,11 +7659,11 @@
       <c r="P111" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q111" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="Q111" t="n">
+        <v>0</v>
+      </c>
+      <c r="R111" s="3" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7124,7 +7710,13 @@
       <c r="P112" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q112" t="inlineStr">
+      <c r="Q112" t="n">
+        <v>4330</v>
+      </c>
+      <c r="R112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S112" t="inlineStr">
         <is>
           <t>4330</t>
         </is>
@@ -7175,9 +7767,15 @@
       <c r="P113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q113" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="Q113" t="n">
+        <v>2722</v>
+      </c>
+      <c r="R113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>2727</t>
         </is>
       </c>
     </row>
@@ -7222,7 +7820,13 @@
       <c r="P114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q114" t="inlineStr">
+      <c r="Q114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="R114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S114" t="inlineStr">
         <is>
           <t>1587</t>
         </is>
@@ -7269,9 +7873,15 @@
       <c r="P115" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Q115" t="inlineStr">
-        <is>
-          <t>4427</t>
+      <c r="Q115" t="n">
+        <v>4427</v>
+      </c>
+      <c r="R115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>4599</t>
         </is>
       </c>
     </row>
@@ -7316,9 +7926,15 @@
       <c r="P116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q116" t="inlineStr">
-        <is>
-          <t>3366</t>
+      <c r="Q116" t="n">
+        <v>3366</v>
+      </c>
+      <c r="R116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>3466</t>
         </is>
       </c>
     </row>
@@ -7354,6 +7970,8 @@
       </c>
       <c r="P117" s="3" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
+      <c r="R117" s="3" t="inlineStr"/>
+      <c r="S117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7388,9 +8006,15 @@
       <c r="P118" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Q118" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="Q118" t="n">
+        <v>2496</v>
+      </c>
+      <c r="R118" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>2583</t>
         </is>
       </c>
     </row>
@@ -7426,12 +8050,12 @@
       </c>
       <c r="P119" s="3" t="inlineStr"/>
       <c r="Q119" t="inlineStr"/>
+      <c r="R119" s="3" t="inlineStr"/>
+      <c r="S119" t="inlineStr"/>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>59166269</t>
-        </is>
+      <c r="A120" t="n">
+        <v>59166269</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -7458,17 +8082,21 @@
       <c r="P120" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>1375</t>
+      <c r="Q120" t="n">
+        <v>1375</v>
+      </c>
+      <c r="R120" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>1451</t>
         </is>
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>15695258</t>
-        </is>
+      <c r="A121" t="n">
+        <v>15695258</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -7495,9 +8123,93 @@
       <c r="P121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q121" t="inlineStr">
+      <c r="Q121" t="n">
+        <v>0</v>
+      </c>
+      <c r="R121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>42558469</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>palyer25524836</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F122" s="3" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" s="3" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" s="3" t="inlineStr"/>
+      <c r="K122" t="inlineStr"/>
+      <c r="L122" s="3" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" s="3" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" s="3" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+      <c r="R122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>2499</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>43834954</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>wuhugouyun</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F123" s="3" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" s="3" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" s="3" t="inlineStr"/>
+      <c r="K123" t="inlineStr"/>
+      <c r="L123" s="3" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" s="3" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" s="3" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+      <c r="R123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-17 11:30:53
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S123"/>
+  <dimension ref="A1:U124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,6 +484,16 @@
       <c r="S1" s="1" t="inlineStr">
         <is>
           <t>04-15_0</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>04-16_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>04-16_0</t>
         </is>
       </c>
     </row>
@@ -531,6 +541,8 @@
       <c r="Q2" t="inlineStr"/>
       <c r="R2" s="3" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
+      <c r="T2" s="3" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -593,7 +605,13 @@
       <c r="R3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="S3" t="n">
+        <v>2535</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="inlineStr">
         <is>
           <t>2535</t>
         </is>
@@ -660,7 +678,13 @@
       <c r="R4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -727,9 +751,15 @@
       <c r="R5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>3979</t>
+      <c r="S5" t="n">
+        <v>3979</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>4033</t>
         </is>
       </c>
     </row>
@@ -794,9 +824,15 @@
       <c r="R6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="S6" t="n">
+        <v>2499</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -861,9 +897,15 @@
       <c r="R7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="S7" t="n">
+        <v>4608</v>
+      </c>
+      <c r="T7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>4823</t>
         </is>
       </c>
     </row>
@@ -911,6 +953,8 @@
       <c r="Q8" t="inlineStr"/>
       <c r="R8" s="3" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
+      <c r="T8" s="3" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -973,9 +1017,15 @@
       <c r="R9" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>3163</t>
+      <c r="S9" t="n">
+        <v>3163</v>
+      </c>
+      <c r="T9" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>3320</t>
         </is>
       </c>
     </row>
@@ -1040,7 +1090,13 @@
       <c r="R10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S10" t="inlineStr">
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1107,7 +1163,13 @@
       <c r="R11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S11" t="inlineStr">
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1174,7 +1236,13 @@
       <c r="R12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S12" t="inlineStr">
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1241,9 +1309,15 @@
       <c r="R13" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>3911</t>
+      <c r="S13" t="n">
+        <v>3911</v>
+      </c>
+      <c r="T13" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -1308,7 +1382,13 @@
       <c r="R14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S14" t="inlineStr">
+      <c r="S14" t="n">
+        <v>2685</v>
+      </c>
+      <c r="T14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" t="inlineStr">
         <is>
           <t>2685</t>
         </is>
@@ -1375,9 +1455,15 @@
       <c r="R15" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>4082</t>
+      <c r="S15" t="n">
+        <v>4082</v>
+      </c>
+      <c r="T15" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -1442,7 +1528,13 @@
       <c r="R16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S16" t="inlineStr">
+      <c r="S16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U16" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1509,9 +1601,15 @@
       <c r="R17" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="S17" t="inlineStr">
-        <is>
-          <t>4462</t>
+      <c r="S17" t="n">
+        <v>4462</v>
+      </c>
+      <c r="T17" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="U17" t="inlineStr">
+        <is>
+          <t>4558</t>
         </is>
       </c>
     </row>
@@ -1576,9 +1674,15 @@
       <c r="R18" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>4499</t>
+      <c r="S18" t="n">
+        <v>4499</v>
+      </c>
+      <c r="T18" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>4651</t>
         </is>
       </c>
     </row>
@@ -1643,9 +1747,15 @@
       <c r="R19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>4897</t>
+      <c r="S19" t="n">
+        <v>4897</v>
+      </c>
+      <c r="T19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>5084</t>
         </is>
       </c>
     </row>
@@ -1710,9 +1820,15 @@
       <c r="R20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>4395</t>
+      <c r="S20" t="n">
+        <v>4395</v>
+      </c>
+      <c r="T20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -1777,9 +1893,15 @@
       <c r="R21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>4652</t>
+      <c r="S21" t="n">
+        <v>4652</v>
+      </c>
+      <c r="T21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>4881</t>
         </is>
       </c>
     </row>
@@ -1844,7 +1966,13 @@
       <c r="R22" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="S22" t="inlineStr">
+      <c r="S22" t="n">
+        <v>2830</v>
+      </c>
+      <c r="T22" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U22" t="inlineStr">
         <is>
           <t>2830</t>
         </is>
@@ -1911,9 +2039,15 @@
       <c r="R23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>3828</t>
+      <c r="S23" t="n">
+        <v>3828</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>3919</t>
         </is>
       </c>
     </row>
@@ -1978,7 +2112,13 @@
       <c r="R24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S24" t="inlineStr">
+      <c r="S24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2045,9 +2185,15 @@
       <c r="R25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>2577</t>
+      <c r="S25" t="n">
+        <v>2577</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -2112,9 +2258,15 @@
       <c r="R26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>4538</t>
+      <c r="S26" t="n">
+        <v>4538</v>
+      </c>
+      <c r="T26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>4665</t>
         </is>
       </c>
     </row>
@@ -2179,9 +2331,15 @@
       <c r="R27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>2822</t>
+      <c r="S27" t="n">
+        <v>2822</v>
+      </c>
+      <c r="T27" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>3180</t>
         </is>
       </c>
     </row>
@@ -2246,9 +2404,15 @@
       <c r="R28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="S28" t="n">
+        <v>2570</v>
+      </c>
+      <c r="T28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>2569</t>
         </is>
       </c>
     </row>
@@ -2313,9 +2477,15 @@
       <c r="R29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>4365</t>
+      <c r="S29" t="n">
+        <v>4365</v>
+      </c>
+      <c r="T29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>4495</t>
         </is>
       </c>
     </row>
@@ -2380,9 +2550,15 @@
       <c r="R30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="S30" t="n">
+        <v>2641</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -2447,9 +2623,15 @@
       <c r="R31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>4314</t>
+      <c r="S31" t="n">
+        <v>4314</v>
+      </c>
+      <c r="T31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>4466</t>
         </is>
       </c>
     </row>
@@ -2514,9 +2696,15 @@
       <c r="R32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>4302</t>
+      <c r="S32" t="n">
+        <v>4302</v>
+      </c>
+      <c r="T32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>4394</t>
         </is>
       </c>
     </row>
@@ -2581,9 +2769,15 @@
       <c r="R33" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="S33" t="inlineStr">
-        <is>
-          <t>4831</t>
+      <c r="S33" t="n">
+        <v>4831</v>
+      </c>
+      <c r="T33" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>5084</t>
         </is>
       </c>
     </row>
@@ -2648,9 +2842,15 @@
       <c r="R34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S34" t="inlineStr">
-        <is>
-          <t>2721</t>
+      <c r="S34" t="n">
+        <v>2721</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>2734</t>
         </is>
       </c>
     </row>
@@ -2715,9 +2915,15 @@
       <c r="R35" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>4170</t>
+      <c r="S35" t="n">
+        <v>4170</v>
+      </c>
+      <c r="T35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>4265</t>
         </is>
       </c>
     </row>
@@ -2782,9 +2988,15 @@
       <c r="R36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>3042</t>
+      <c r="S36" t="n">
+        <v>3042</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>3054</t>
         </is>
       </c>
     </row>
@@ -2849,9 +3061,15 @@
       <c r="R37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>4687</t>
+      <c r="S37" t="n">
+        <v>4687</v>
+      </c>
+      <c r="T37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>4888</t>
         </is>
       </c>
     </row>
@@ -2916,9 +3134,15 @@
       <c r="R38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="S38" t="n">
+        <v>3984</v>
+      </c>
+      <c r="T38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -2983,9 +3207,15 @@
       <c r="R39" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>3174</t>
+      <c r="S39" t="n">
+        <v>3174</v>
+      </c>
+      <c r="T39" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>3244</t>
         </is>
       </c>
     </row>
@@ -3050,9 +3280,15 @@
       <c r="R40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S40" t="inlineStr">
-        <is>
-          <t>4806</t>
+      <c r="S40" t="n">
+        <v>4806</v>
+      </c>
+      <c r="T40" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>4998</t>
         </is>
       </c>
     </row>
@@ -3117,9 +3353,15 @@
       <c r="R41" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>4781</t>
+      <c r="S41" t="n">
+        <v>4781</v>
+      </c>
+      <c r="T41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>4818</t>
         </is>
       </c>
     </row>
@@ -3184,9 +3426,15 @@
       <c r="R42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>4370</t>
+      <c r="S42" t="n">
+        <v>4370</v>
+      </c>
+      <c r="T42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>4437</t>
         </is>
       </c>
     </row>
@@ -3251,9 +3499,15 @@
       <c r="R43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S43" t="inlineStr">
-        <is>
-          <t>4457</t>
+      <c r="S43" t="n">
+        <v>4457</v>
+      </c>
+      <c r="T43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>4592</t>
         </is>
       </c>
     </row>
@@ -3318,9 +3572,15 @@
       <c r="R44" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>4187</t>
+      <c r="S44" t="n">
+        <v>4187</v>
+      </c>
+      <c r="T44" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>4205</t>
         </is>
       </c>
     </row>
@@ -3385,9 +3645,15 @@
       <c r="R45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>4465</t>
+      <c r="S45" t="n">
+        <v>4465</v>
+      </c>
+      <c r="T45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>4599</t>
         </is>
       </c>
     </row>
@@ -3452,9 +3718,15 @@
       <c r="R46" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>4254</t>
+      <c r="S46" t="n">
+        <v>4254</v>
+      </c>
+      <c r="T46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>4396</t>
         </is>
       </c>
     </row>
@@ -3519,9 +3791,15 @@
       <c r="R47" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>3252</t>
+      <c r="S47" t="n">
+        <v>3252</v>
+      </c>
+      <c r="T47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>3708</t>
         </is>
       </c>
     </row>
@@ -3586,9 +3864,15 @@
       <c r="R48" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>4703</t>
+      <c r="S48" t="n">
+        <v>4703</v>
+      </c>
+      <c r="T48" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -3653,9 +3937,15 @@
       <c r="R49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="S49" t="n">
+        <v>4029</v>
+      </c>
+      <c r="T49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>4124</t>
         </is>
       </c>
     </row>
@@ -3703,6 +3993,8 @@
       <c r="Q50" t="inlineStr"/>
       <c r="R50" s="3" t="inlineStr"/>
       <c r="S50" t="inlineStr"/>
+      <c r="T50" s="3" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3765,9 +4057,15 @@
       <c r="R51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>4042</t>
+      <c r="S51" t="n">
+        <v>4042</v>
+      </c>
+      <c r="T51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>4145</t>
         </is>
       </c>
     </row>
@@ -3832,9 +4130,15 @@
       <c r="R52" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>4004</t>
+      <c r="S52" t="n">
+        <v>4004</v>
+      </c>
+      <c r="T52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>4093</t>
         </is>
       </c>
     </row>
@@ -3899,9 +4203,15 @@
       <c r="R53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="S53" t="n">
+        <v>3998</v>
+      </c>
+      <c r="T53" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>4142</t>
         </is>
       </c>
     </row>
@@ -3966,9 +4276,15 @@
       <c r="R54" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>3590</t>
+      <c r="S54" t="n">
+        <v>3590</v>
+      </c>
+      <c r="T54" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>3866</t>
         </is>
       </c>
     </row>
@@ -4033,9 +4349,15 @@
       <c r="R55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>3913</t>
+      <c r="S55" t="n">
+        <v>3913</v>
+      </c>
+      <c r="T55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -4100,9 +4422,15 @@
       <c r="R56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="S56" t="n">
+        <v>3990</v>
+      </c>
+      <c r="T56" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -4167,9 +4495,15 @@
       <c r="R57" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="S57" t="n">
+        <v>4027</v>
+      </c>
+      <c r="T57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -4234,7 +4568,13 @@
       <c r="R58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S58" t="inlineStr">
+      <c r="S58" t="n">
+        <v>0</v>
+      </c>
+      <c r="T58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4301,9 +4641,15 @@
       <c r="R59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="S59" t="n">
+        <v>2692</v>
+      </c>
+      <c r="T59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -4368,9 +4714,15 @@
       <c r="R60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="S60" t="n">
+        <v>2475</v>
+      </c>
+      <c r="T60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -4435,9 +4787,15 @@
       <c r="R61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S61" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="S61" t="n">
+        <v>3369</v>
+      </c>
+      <c r="T61" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="U61" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -4502,9 +4860,15 @@
       <c r="R62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>1986</t>
+      <c r="S62" t="n">
+        <v>1986</v>
+      </c>
+      <c r="T62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>1983</t>
         </is>
       </c>
     </row>
@@ -4540,6 +4904,8 @@
       <c r="Q63" t="inlineStr"/>
       <c r="R63" s="3" t="inlineStr"/>
       <c r="S63" t="inlineStr"/>
+      <c r="T63" s="3" t="inlineStr"/>
+      <c r="U63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4602,7 +4968,13 @@
       <c r="R64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S64" t="inlineStr">
+      <c r="S64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4660,6 +5032,8 @@
       <c r="Q65" t="inlineStr"/>
       <c r="R65" s="3" t="inlineStr"/>
       <c r="S65" t="inlineStr"/>
+      <c r="T65" s="3" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4722,9 +5096,15 @@
       <c r="R66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S66" t="inlineStr">
-        <is>
-          <t>2486</t>
+      <c r="S66" t="n">
+        <v>2486</v>
+      </c>
+      <c r="T66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>2483</t>
         </is>
       </c>
     </row>
@@ -4789,9 +5169,15 @@
       <c r="R67" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>4697</t>
+      <c r="S67" t="n">
+        <v>4697</v>
+      </c>
+      <c r="T67" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>4888</t>
         </is>
       </c>
     </row>
@@ -4856,7 +5242,13 @@
       <c r="R68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S68" t="inlineStr">
+      <c r="S68" t="n">
+        <v>0</v>
+      </c>
+      <c r="T68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4923,9 +5315,15 @@
       <c r="R69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="S69" t="n">
+        <v>2497</v>
+      </c>
+      <c r="T69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>2550</t>
         </is>
       </c>
     </row>
@@ -4990,7 +5388,13 @@
       <c r="R70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S70" t="inlineStr">
+      <c r="S70" t="n">
+        <v>0</v>
+      </c>
+      <c r="T70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5057,9 +5461,15 @@
       <c r="R71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S71" t="inlineStr">
-        <is>
-          <t>3375</t>
+      <c r="S71" t="n">
+        <v>3375</v>
+      </c>
+      <c r="T71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>3438</t>
         </is>
       </c>
     </row>
@@ -5124,9 +5534,15 @@
       <c r="R72" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S72" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="S72" t="n">
+        <v>2851</v>
+      </c>
+      <c r="T72" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U72" t="inlineStr">
+        <is>
+          <t>3215</t>
         </is>
       </c>
     </row>
@@ -5191,7 +5607,13 @@
       <c r="R73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S73" t="inlineStr">
+      <c r="S73" t="n">
+        <v>0</v>
+      </c>
+      <c r="T73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5258,7 +5680,13 @@
       <c r="R74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S74" t="inlineStr">
+      <c r="S74" t="n">
+        <v>0</v>
+      </c>
+      <c r="T74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5312,6 +5740,8 @@
       <c r="Q75" t="inlineStr"/>
       <c r="R75" s="3" t="inlineStr"/>
       <c r="S75" t="inlineStr"/>
+      <c r="T75" s="3" t="inlineStr"/>
+      <c r="U75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5374,9 +5804,15 @@
       <c r="R76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="S76" t="n">
+        <v>0</v>
+      </c>
+      <c r="T76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>1496</t>
         </is>
       </c>
     </row>
@@ -5441,9 +5877,15 @@
       <c r="R77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S77" t="inlineStr">
-        <is>
-          <t>2990</t>
+      <c r="S77" t="n">
+        <v>2990</v>
+      </c>
+      <c r="T77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>2999</t>
         </is>
       </c>
     </row>
@@ -5508,7 +5950,13 @@
       <c r="R78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S78" t="inlineStr">
+      <c r="S78" t="n">
+        <v>0</v>
+      </c>
+      <c r="T78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5575,7 +6023,13 @@
       <c r="R79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S79" t="inlineStr">
+      <c r="S79" t="n">
+        <v>0</v>
+      </c>
+      <c r="T79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5642,9 +6096,15 @@
       <c r="R80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S80" t="inlineStr">
-        <is>
-          <t>1454</t>
+      <c r="S80" t="n">
+        <v>1454</v>
+      </c>
+      <c r="T80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U80" t="inlineStr">
+        <is>
+          <t>1450</t>
         </is>
       </c>
     </row>
@@ -5709,7 +6169,13 @@
       <c r="R81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S81" t="inlineStr">
+      <c r="S81" t="n">
+        <v>0</v>
+      </c>
+      <c r="T81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5776,7 +6242,13 @@
       <c r="R82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S82" t="inlineStr">
+      <c r="S82" t="n">
+        <v>0</v>
+      </c>
+      <c r="T82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5843,7 +6315,13 @@
       <c r="R83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S83" t="inlineStr">
+      <c r="S83" t="n">
+        <v>0</v>
+      </c>
+      <c r="T83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5910,7 +6388,13 @@
       <c r="R84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S84" t="inlineStr">
+      <c r="S84" t="n">
+        <v>0</v>
+      </c>
+      <c r="T84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5977,7 +6461,13 @@
       <c r="R85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S85" t="inlineStr">
+      <c r="S85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6044,7 +6534,13 @@
       <c r="R86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S86" t="inlineStr">
+      <c r="S86" t="n">
+        <v>0</v>
+      </c>
+      <c r="T86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6111,7 +6607,13 @@
       <c r="R87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S87" t="inlineStr">
+      <c r="S87" t="n">
+        <v>0</v>
+      </c>
+      <c r="T87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6178,9 +6680,15 @@
       <c r="R88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S88" t="inlineStr">
-        <is>
-          <t>2626</t>
+      <c r="S88" t="n">
+        <v>2626</v>
+      </c>
+      <c r="T88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U88" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -6245,7 +6753,13 @@
       <c r="R89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S89" t="inlineStr">
+      <c r="S89" t="n">
+        <v>0</v>
+      </c>
+      <c r="T89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6312,7 +6826,13 @@
       <c r="R90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S90" t="inlineStr">
+      <c r="S90" t="n">
+        <v>0</v>
+      </c>
+      <c r="T90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6378,6 +6898,8 @@
       </c>
       <c r="R91" s="3" t="inlineStr"/>
       <c r="S91" t="inlineStr"/>
+      <c r="T91" s="3" t="inlineStr"/>
+      <c r="U91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -6440,7 +6962,13 @@
       <c r="R92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6507,9 +7035,15 @@
       <c r="R93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S93" t="inlineStr">
-        <is>
-          <t>3485</t>
+      <c r="S93" t="n">
+        <v>3485</v>
+      </c>
+      <c r="T93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="inlineStr">
+        <is>
+          <t>3471</t>
         </is>
       </c>
     </row>
@@ -6574,7 +7108,13 @@
       <c r="R94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S94" t="inlineStr">
+      <c r="S94" t="n">
+        <v>0</v>
+      </c>
+      <c r="T94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6641,7 +7181,13 @@
       <c r="R95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S95" t="inlineStr">
+      <c r="S95" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6708,7 +7254,13 @@
       <c r="R96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S96" t="inlineStr">
+      <c r="S96" t="n">
+        <v>0</v>
+      </c>
+      <c r="T96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6775,7 +7327,13 @@
       <c r="R97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S97" t="inlineStr">
+      <c r="S97" t="n">
+        <v>0</v>
+      </c>
+      <c r="T97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6842,7 +7400,13 @@
       <c r="R98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
+      <c r="S98" t="n">
+        <v>0</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6909,7 +7473,13 @@
       <c r="R99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S99" t="inlineStr">
+      <c r="S99" t="n">
+        <v>0</v>
+      </c>
+      <c r="T99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6976,7 +7546,13 @@
       <c r="R100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S100" t="inlineStr">
+      <c r="S100" t="n">
+        <v>0</v>
+      </c>
+      <c r="T100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7043,9 +7619,15 @@
       <c r="R101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S101" t="inlineStr">
-        <is>
-          <t>1498</t>
+      <c r="S101" t="n">
+        <v>1498</v>
+      </c>
+      <c r="T101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U101" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7110,7 +7692,13 @@
       <c r="R102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S102" t="inlineStr">
+      <c r="S102" t="n">
+        <v>0</v>
+      </c>
+      <c r="T102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7176,6 +7764,8 @@
       </c>
       <c r="R103" s="3" t="inlineStr"/>
       <c r="S103" t="inlineStr"/>
+      <c r="T103" s="3" t="inlineStr"/>
+      <c r="U103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -7237,6 +7827,8 @@
       </c>
       <c r="R104" s="3" t="inlineStr"/>
       <c r="S104" t="inlineStr"/>
+      <c r="T104" s="3" t="inlineStr"/>
+      <c r="U104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -7298,6 +7890,8 @@
       </c>
       <c r="R105" s="3" t="inlineStr"/>
       <c r="S105" t="inlineStr"/>
+      <c r="T105" s="3" t="inlineStr"/>
+      <c r="U105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -7359,6 +7953,8 @@
       </c>
       <c r="R106" s="3" t="inlineStr"/>
       <c r="S106" t="inlineStr"/>
+      <c r="T106" s="3" t="inlineStr"/>
+      <c r="U106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -7420,6 +8016,8 @@
       </c>
       <c r="R107" s="3" t="inlineStr"/>
       <c r="S107" t="inlineStr"/>
+      <c r="T107" s="3" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -7481,6 +8079,8 @@
       </c>
       <c r="R108" s="3" t="inlineStr"/>
       <c r="S108" t="inlineStr"/>
+      <c r="T108" s="3" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -7542,6 +8142,8 @@
       </c>
       <c r="R109" s="3" t="inlineStr"/>
       <c r="S109" t="inlineStr"/>
+      <c r="T109" s="3" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -7603,6 +8205,8 @@
       </c>
       <c r="R110" s="3" t="inlineStr"/>
       <c r="S110" t="inlineStr"/>
+      <c r="T110" s="3" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7664,6 +8268,8 @@
       </c>
       <c r="R111" s="3" t="inlineStr"/>
       <c r="S111" t="inlineStr"/>
+      <c r="T111" s="3" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7716,9 +8322,15 @@
       <c r="R112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S112" t="inlineStr">
-        <is>
-          <t>4330</t>
+      <c r="S112" t="n">
+        <v>4330</v>
+      </c>
+      <c r="T112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U112" t="inlineStr">
+        <is>
+          <t>4342</t>
         </is>
       </c>
     </row>
@@ -7773,9 +8385,15 @@
       <c r="R113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S113" t="inlineStr">
-        <is>
-          <t>2727</t>
+      <c r="S113" t="n">
+        <v>2727</v>
+      </c>
+      <c r="T113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U113" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -7826,7 +8444,13 @@
       <c r="R114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S114" t="inlineStr">
+      <c r="S114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="T114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U114" t="inlineStr">
         <is>
           <t>1587</t>
         </is>
@@ -7879,9 +8503,15 @@
       <c r="R115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>4599</t>
+      <c r="S115" t="n">
+        <v>4599</v>
+      </c>
+      <c r="T115" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>4802</t>
         </is>
       </c>
     </row>
@@ -7932,9 +8562,15 @@
       <c r="R116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="S116" t="inlineStr">
-        <is>
-          <t>3466</t>
+      <c r="S116" t="n">
+        <v>3466</v>
+      </c>
+      <c r="T116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>3498</t>
         </is>
       </c>
     </row>
@@ -7972,6 +8608,8 @@
       <c r="Q117" t="inlineStr"/>
       <c r="R117" s="3" t="inlineStr"/>
       <c r="S117" t="inlineStr"/>
+      <c r="T117" s="3" t="inlineStr"/>
+      <c r="U117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8012,9 +8650,15 @@
       <c r="R118" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="S118" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="S118" t="n">
+        <v>2583</v>
+      </c>
+      <c r="T118" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -8052,6 +8696,8 @@
       <c r="Q119" t="inlineStr"/>
       <c r="R119" s="3" t="inlineStr"/>
       <c r="S119" t="inlineStr"/>
+      <c r="T119" s="3" t="inlineStr"/>
+      <c r="U119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -8088,9 +8734,15 @@
       <c r="R120" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="S120" t="inlineStr">
-        <is>
-          <t>1451</t>
+      <c r="S120" t="n">
+        <v>1451</v>
+      </c>
+      <c r="T120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>1468</t>
         </is>
       </c>
     </row>
@@ -8129,17 +8781,21 @@
       <c r="R121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S121" t="inlineStr">
+      <c r="S121" t="n">
+        <v>0</v>
+      </c>
+      <c r="T121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>42558469</t>
-        </is>
+      <c r="A122" t="n">
+        <v>42558469</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -8168,17 +8824,21 @@
       <c r="R122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S122" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="S122" t="n">
+        <v>2499</v>
+      </c>
+      <c r="T122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>43834954</t>
-        </is>
+      <c r="A123" t="n">
+        <v>43834954</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -8207,9 +8867,56 @@
       <c r="R123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S123" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="S123" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>2538</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>59206405</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>pro-59206405</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F124" s="3" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" s="3" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" s="3" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" s="3" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" s="3" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" s="3" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+      <c r="R124" s="3" t="inlineStr"/>
+      <c r="S124" t="inlineStr"/>
+      <c r="T124" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>1421</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-18 11:31:07
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U124"/>
+  <dimension ref="A1:W127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,16 @@
       <c r="U1" s="1" t="inlineStr">
         <is>
           <t>04-16_0</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>04-17_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>04-17_0</t>
         </is>
       </c>
     </row>
@@ -543,6 +553,8 @@
       <c r="S2" t="inlineStr"/>
       <c r="T2" s="3" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
+      <c r="V2" s="3" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -611,9 +623,15 @@
       <c r="T3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="U3" t="n">
+        <v>2535</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -684,7 +702,13 @@
       <c r="T4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -757,9 +781,15 @@
       <c r="T5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>4033</t>
+      <c r="U5" t="n">
+        <v>4033</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>4108</t>
         </is>
       </c>
     </row>
@@ -830,9 +860,15 @@
       <c r="T6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="U6" t="n">
+        <v>2535</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -855,7 +891,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>总馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
@@ -903,9 +939,15 @@
       <c r="T7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>4823</t>
+      <c r="U7" t="n">
+        <v>4823</v>
+      </c>
+      <c r="V7" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>5028</t>
         </is>
       </c>
     </row>
@@ -955,6 +997,8 @@
       <c r="S8" t="inlineStr"/>
       <c r="T8" s="3" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
+      <c r="V8" s="3" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1023,9 +1067,15 @@
       <c r="T9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>3320</t>
+      <c r="U9" t="n">
+        <v>3320</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="inlineStr">
+        <is>
+          <t>3361</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1146,13 @@
       <c r="T10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U10" t="inlineStr">
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1169,7 +1225,13 @@
       <c r="T11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U11" t="inlineStr">
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1242,7 +1304,13 @@
       <c r="T12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U12" t="inlineStr">
+      <c r="U12" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1315,9 +1383,15 @@
       <c r="T13" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="U13" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="U13" t="n">
+        <v>3994</v>
+      </c>
+      <c r="V13" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1462,13 @@
       <c r="T14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U14" t="inlineStr">
+      <c r="U14" t="n">
+        <v>2685</v>
+      </c>
+      <c r="V14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" t="inlineStr">
         <is>
           <t>2685</t>
         </is>
@@ -1461,9 +1541,15 @@
       <c r="T15" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>4149</t>
+      <c r="U15" t="n">
+        <v>4149</v>
+      </c>
+      <c r="V15" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W15" t="inlineStr">
+        <is>
+          <t>4336</t>
         </is>
       </c>
     </row>
@@ -1534,11 +1620,11 @@
       <c r="T16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
-      </c>
+      <c r="U16" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V16" s="3" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1607,9 +1693,15 @@
       <c r="T17" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="U17" t="inlineStr">
-        <is>
-          <t>4558</t>
+      <c r="U17" t="n">
+        <v>4558</v>
+      </c>
+      <c r="V17" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="W17" t="inlineStr">
+        <is>
+          <t>4808</t>
         </is>
       </c>
     </row>
@@ -1680,9 +1772,15 @@
       <c r="T18" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>4651</t>
+      <c r="U18" t="n">
+        <v>4651</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>4841</t>
         </is>
       </c>
     </row>
@@ -1753,9 +1851,15 @@
       <c r="T19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>5084</t>
+      <c r="U19" t="n">
+        <v>5084</v>
+      </c>
+      <c r="V19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>5299</t>
         </is>
       </c>
     </row>
@@ -1826,9 +1930,15 @@
       <c r="T20" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="U20" t="n">
+        <v>4608</v>
+      </c>
+      <c r="V20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>4768</t>
         </is>
       </c>
     </row>
@@ -1899,9 +2009,15 @@
       <c r="T21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>4881</t>
+      <c r="U21" t="n">
+        <v>4881</v>
+      </c>
+      <c r="V21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>5147</t>
         </is>
       </c>
     </row>
@@ -1972,9 +2088,15 @@
       <c r="T22" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>2830</t>
+      <c r="U22" t="n">
+        <v>2830</v>
+      </c>
+      <c r="V22" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>2982</t>
         </is>
       </c>
     </row>
@@ -2045,9 +2167,15 @@
       <c r="T23" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>3919</t>
+      <c r="U23" t="n">
+        <v>3919</v>
+      </c>
+      <c r="V23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>4259</t>
         </is>
       </c>
     </row>
@@ -2118,7 +2246,13 @@
       <c r="T24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="U24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2191,11 +2325,11 @@
       <c r="T25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>2574</t>
-        </is>
-      </c>
+      <c r="U25" t="n">
+        <v>2574</v>
+      </c>
+      <c r="V25" s="3" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2264,9 +2398,15 @@
       <c r="T26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>4665</t>
+      <c r="U26" t="n">
+        <v>4665</v>
+      </c>
+      <c r="V26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>4806</t>
         </is>
       </c>
     </row>
@@ -2337,7 +2477,13 @@
       <c r="T27" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="U27" t="n">
+        <v>3180</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="inlineStr">
         <is>
           <t>3180</t>
         </is>
@@ -2410,7 +2556,13 @@
       <c r="T28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U28" t="inlineStr">
+      <c r="U28" t="n">
+        <v>2569</v>
+      </c>
+      <c r="V28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="inlineStr">
         <is>
           <t>2569</t>
         </is>
@@ -2483,9 +2635,15 @@
       <c r="T29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>4495</t>
+      <c r="U29" t="n">
+        <v>4495</v>
+      </c>
+      <c r="V29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>4666</t>
         </is>
       </c>
     </row>
@@ -2556,7 +2714,13 @@
       <c r="T30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U30" t="inlineStr">
+      <c r="U30" t="n">
+        <v>2668</v>
+      </c>
+      <c r="V30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="inlineStr">
         <is>
           <t>2668</t>
         </is>
@@ -2629,9 +2793,15 @@
       <c r="T31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>4466</t>
+      <c r="U31" t="n">
+        <v>4466</v>
+      </c>
+      <c r="V31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>4652</t>
         </is>
       </c>
     </row>
@@ -2702,9 +2872,15 @@
       <c r="T32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>4394</t>
+      <c r="U32" t="n">
+        <v>4394</v>
+      </c>
+      <c r="V32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>4494</t>
         </is>
       </c>
     </row>
@@ -2775,11 +2951,11 @@
       <c r="T33" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U33" t="inlineStr">
-        <is>
-          <t>5084</t>
-        </is>
-      </c>
+      <c r="U33" t="n">
+        <v>5084</v>
+      </c>
+      <c r="V33" s="3" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2848,9 +3024,15 @@
       <c r="T34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U34" t="inlineStr">
-        <is>
-          <t>2734</t>
+      <c r="U34" t="n">
+        <v>2734</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -2921,9 +3103,15 @@
       <c r="T35" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="U35" t="inlineStr">
-        <is>
-          <t>4265</t>
+      <c r="U35" t="n">
+        <v>4265</v>
+      </c>
+      <c r="V35" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>4305</t>
         </is>
       </c>
     </row>
@@ -2994,9 +3182,15 @@
       <c r="T36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>3054</t>
+      <c r="U36" t="n">
+        <v>3054</v>
+      </c>
+      <c r="V36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>3191</t>
         </is>
       </c>
     </row>
@@ -3067,9 +3261,15 @@
       <c r="T37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>4888</t>
+      <c r="U37" t="n">
+        <v>4888</v>
+      </c>
+      <c r="V37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>5044</t>
         </is>
       </c>
     </row>
@@ -3140,9 +3340,15 @@
       <c r="T38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="U38" t="n">
+        <v>3988</v>
+      </c>
+      <c r="V38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -3213,9 +3419,15 @@
       <c r="T39" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>3244</t>
+      <c r="U39" t="n">
+        <v>3244</v>
+      </c>
+      <c r="V39" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>3366</t>
         </is>
       </c>
     </row>
@@ -3286,9 +3498,15 @@
       <c r="T40" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="U40" t="inlineStr">
-        <is>
-          <t>4998</t>
+      <c r="U40" t="n">
+        <v>4998</v>
+      </c>
+      <c r="V40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>5209</t>
         </is>
       </c>
     </row>
@@ -3359,9 +3577,15 @@
       <c r="T41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>4818</t>
+      <c r="U41" t="n">
+        <v>4818</v>
+      </c>
+      <c r="V41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>4995</t>
         </is>
       </c>
     </row>
@@ -3432,9 +3656,15 @@
       <c r="T42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>4437</t>
+      <c r="U42" t="n">
+        <v>4437</v>
+      </c>
+      <c r="V42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>4575</t>
         </is>
       </c>
     </row>
@@ -3505,9 +3735,15 @@
       <c r="T43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U43" t="inlineStr">
-        <is>
-          <t>4592</t>
+      <c r="U43" t="n">
+        <v>4592</v>
+      </c>
+      <c r="V43" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -3578,9 +3814,15 @@
       <c r="T44" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U44" t="inlineStr">
-        <is>
-          <t>4205</t>
+      <c r="U44" t="n">
+        <v>4205</v>
+      </c>
+      <c r="V44" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>4488</t>
         </is>
       </c>
     </row>
@@ -3651,9 +3893,15 @@
       <c r="T45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U45" t="inlineStr">
-        <is>
-          <t>4599</t>
+      <c r="U45" t="n">
+        <v>4599</v>
+      </c>
+      <c r="V45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -3724,9 +3972,15 @@
       <c r="T46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>4396</t>
+      <c r="U46" t="n">
+        <v>4396</v>
+      </c>
+      <c r="V46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>4505</t>
         </is>
       </c>
     </row>
@@ -3797,9 +4051,15 @@
       <c r="T47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>3708</t>
+      <c r="U47" t="n">
+        <v>3708</v>
+      </c>
+      <c r="V47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>4048</t>
         </is>
       </c>
     </row>
@@ -3870,9 +4130,15 @@
       <c r="T48" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="U48" t="n">
+        <v>4763</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>4739</t>
         </is>
       </c>
     </row>
@@ -3943,9 +4209,15 @@
       <c r="T49" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>4124</t>
+      <c r="U49" t="n">
+        <v>4124</v>
+      </c>
+      <c r="V49" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -3995,6 +4267,8 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" s="3" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
+      <c r="V50" s="3" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4063,9 +4337,15 @@
       <c r="T51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U51" t="inlineStr">
-        <is>
-          <t>4145</t>
+      <c r="U51" t="n">
+        <v>4145</v>
+      </c>
+      <c r="V51" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>4101</t>
         </is>
       </c>
     </row>
@@ -4136,9 +4416,15 @@
       <c r="T52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>4093</t>
+      <c r="U52" t="n">
+        <v>4093</v>
+      </c>
+      <c r="V52" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -4209,9 +4495,15 @@
       <c r="T53" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>4142</t>
+      <c r="U53" t="n">
+        <v>4142</v>
+      </c>
+      <c r="V53" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>4160</t>
         </is>
       </c>
     </row>
@@ -4282,9 +4574,15 @@
       <c r="T54" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="U54" t="inlineStr">
-        <is>
-          <t>3866</t>
+      <c r="U54" t="n">
+        <v>3866</v>
+      </c>
+      <c r="V54" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="W54" t="inlineStr">
+        <is>
+          <t>4009</t>
         </is>
       </c>
     </row>
@@ -4355,9 +4653,15 @@
       <c r="T55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="U55" t="n">
+        <v>3991</v>
+      </c>
+      <c r="V55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -4428,9 +4732,15 @@
       <c r="T56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="U56" t="n">
+        <v>3991</v>
+      </c>
+      <c r="V56" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>3999</t>
         </is>
       </c>
     </row>
@@ -4501,9 +4811,15 @@
       <c r="T57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="U57" t="n">
+        <v>4167</v>
+      </c>
+      <c r="V57" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>4182</t>
         </is>
       </c>
     </row>
@@ -4574,7 +4890,13 @@
       <c r="T58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U58" t="inlineStr">
+      <c r="U58" t="n">
+        <v>0</v>
+      </c>
+      <c r="V58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4647,9 +4969,15 @@
       <c r="T59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="U59" t="n">
+        <v>2752</v>
+      </c>
+      <c r="V59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>2766</t>
         </is>
       </c>
     </row>
@@ -4720,9 +5048,15 @@
       <c r="T60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>2470</t>
+      <c r="U60" t="n">
+        <v>2470</v>
+      </c>
+      <c r="V60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>2467</t>
         </is>
       </c>
     </row>
@@ -4793,9 +5127,15 @@
       <c r="T61" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="U61" t="inlineStr">
-        <is>
-          <t>3601</t>
+      <c r="U61" t="n">
+        <v>3601</v>
+      </c>
+      <c r="V61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>3600</t>
         </is>
       </c>
     </row>
@@ -4866,9 +5206,15 @@
       <c r="T62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>1983</t>
+      <c r="U62" t="n">
+        <v>1983</v>
+      </c>
+      <c r="V62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>1975</t>
         </is>
       </c>
     </row>
@@ -4906,6 +5252,8 @@
       <c r="S63" t="inlineStr"/>
       <c r="T63" s="3" t="inlineStr"/>
       <c r="U63" t="inlineStr"/>
+      <c r="V63" s="3" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4974,7 +5322,13 @@
       <c r="T64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U64" t="inlineStr">
+      <c r="U64" t="n">
+        <v>0</v>
+      </c>
+      <c r="V64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5034,6 +5388,8 @@
       <c r="S65" t="inlineStr"/>
       <c r="T65" s="3" t="inlineStr"/>
       <c r="U65" t="inlineStr"/>
+      <c r="V65" s="3" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5102,9 +5458,15 @@
       <c r="T66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U66" t="inlineStr">
-        <is>
-          <t>2483</t>
+      <c r="U66" t="n">
+        <v>2483</v>
+      </c>
+      <c r="V66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -5175,9 +5537,15 @@
       <c r="T67" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>4888</t>
+      <c r="U67" t="n">
+        <v>4888</v>
+      </c>
+      <c r="V67" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="W67" t="inlineStr">
+        <is>
+          <t>5041</t>
         </is>
       </c>
     </row>
@@ -5248,7 +5616,13 @@
       <c r="T68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U68" t="inlineStr">
+      <c r="U68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5321,9 +5695,15 @@
       <c r="T69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U69" t="inlineStr">
-        <is>
-          <t>2550</t>
+      <c r="U69" t="n">
+        <v>2550</v>
+      </c>
+      <c r="V69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W69" t="inlineStr">
+        <is>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -5394,7 +5774,13 @@
       <c r="T70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U70" t="inlineStr">
+      <c r="U70" t="n">
+        <v>0</v>
+      </c>
+      <c r="V70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5467,9 +5853,15 @@
       <c r="T71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U71" t="inlineStr">
-        <is>
-          <t>3438</t>
+      <c r="U71" t="n">
+        <v>3438</v>
+      </c>
+      <c r="V71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W71" t="inlineStr">
+        <is>
+          <t>3913</t>
         </is>
       </c>
     </row>
@@ -5540,9 +5932,15 @@
       <c r="T72" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U72" t="inlineStr">
-        <is>
-          <t>3215</t>
+      <c r="U72" t="n">
+        <v>3215</v>
+      </c>
+      <c r="V72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W72" t="inlineStr">
+        <is>
+          <t>3240</t>
         </is>
       </c>
     </row>
@@ -5613,7 +6011,13 @@
       <c r="T73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U73" t="inlineStr">
+      <c r="U73" t="n">
+        <v>0</v>
+      </c>
+      <c r="V73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5686,7 +6090,13 @@
       <c r="T74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U74" t="inlineStr">
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5742,6 +6152,8 @@
       <c r="S75" t="inlineStr"/>
       <c r="T75" s="3" t="inlineStr"/>
       <c r="U75" t="inlineStr"/>
+      <c r="V75" s="3" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5810,9 +6222,15 @@
       <c r="T76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>1496</t>
+      <c r="U76" t="n">
+        <v>1496</v>
+      </c>
+      <c r="V76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5883,9 +6301,15 @@
       <c r="T77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U77" t="inlineStr">
-        <is>
-          <t>2999</t>
+      <c r="U77" t="n">
+        <v>2999</v>
+      </c>
+      <c r="V77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>3024</t>
         </is>
       </c>
     </row>
@@ -5956,7 +6380,13 @@
       <c r="T78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U78" t="inlineStr">
+      <c r="U78" t="n">
+        <v>0</v>
+      </c>
+      <c r="V78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6029,7 +6459,13 @@
       <c r="T79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U79" t="inlineStr">
+      <c r="U79" t="n">
+        <v>0</v>
+      </c>
+      <c r="V79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6102,9 +6538,15 @@
       <c r="T80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U80" t="inlineStr">
-        <is>
-          <t>1450</t>
+      <c r="U80" t="n">
+        <v>1450</v>
+      </c>
+      <c r="V80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W80" t="inlineStr">
+        <is>
+          <t>1447</t>
         </is>
       </c>
     </row>
@@ -6175,7 +6617,13 @@
       <c r="T81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U81" t="inlineStr">
+      <c r="U81" t="n">
+        <v>0</v>
+      </c>
+      <c r="V81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6248,7 +6696,13 @@
       <c r="T82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U82" t="inlineStr">
+      <c r="U82" t="n">
+        <v>0</v>
+      </c>
+      <c r="V82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6321,7 +6775,13 @@
       <c r="T83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U83" t="inlineStr">
+      <c r="U83" t="n">
+        <v>0</v>
+      </c>
+      <c r="V83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6394,7 +6854,13 @@
       <c r="T84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U84" t="inlineStr">
+      <c r="U84" t="n">
+        <v>0</v>
+      </c>
+      <c r="V84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6467,7 +6933,13 @@
       <c r="T85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U85" t="inlineStr">
+      <c r="U85" t="n">
+        <v>0</v>
+      </c>
+      <c r="V85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6540,7 +7012,13 @@
       <c r="T86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U86" t="inlineStr">
+      <c r="U86" t="n">
+        <v>0</v>
+      </c>
+      <c r="V86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6613,7 +7091,13 @@
       <c r="T87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U87" t="inlineStr">
+      <c r="U87" t="n">
+        <v>0</v>
+      </c>
+      <c r="V87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6686,9 +7170,15 @@
       <c r="T88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U88" t="inlineStr">
-        <is>
-          <t>2619</t>
+      <c r="U88" t="n">
+        <v>2619</v>
+      </c>
+      <c r="V88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W88" t="inlineStr">
+        <is>
+          <t>2648</t>
         </is>
       </c>
     </row>
@@ -6759,7 +7249,13 @@
       <c r="T89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U89" t="inlineStr">
+      <c r="U89" t="n">
+        <v>0</v>
+      </c>
+      <c r="V89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6832,7 +7328,13 @@
       <c r="T90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U90" t="inlineStr">
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+      <c r="V90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6900,6 +7402,8 @@
       <c r="S91" t="inlineStr"/>
       <c r="T91" s="3" t="inlineStr"/>
       <c r="U91" t="inlineStr"/>
+      <c r="V91" s="3" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -6968,7 +7472,13 @@
       <c r="T92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7041,9 +7551,15 @@
       <c r="T93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U93" t="inlineStr">
-        <is>
-          <t>3471</t>
+      <c r="U93" t="n">
+        <v>3471</v>
+      </c>
+      <c r="V93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W93" t="inlineStr">
+        <is>
+          <t>3453</t>
         </is>
       </c>
     </row>
@@ -7114,7 +7630,13 @@
       <c r="T94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U94" t="inlineStr">
+      <c r="U94" t="n">
+        <v>0</v>
+      </c>
+      <c r="V94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7187,7 +7709,13 @@
       <c r="T95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U95" t="inlineStr">
+      <c r="U95" t="n">
+        <v>0</v>
+      </c>
+      <c r="V95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7260,7 +7788,13 @@
       <c r="T96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U96" t="inlineStr">
+      <c r="U96" t="n">
+        <v>0</v>
+      </c>
+      <c r="V96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7333,7 +7867,13 @@
       <c r="T97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U97" t="inlineStr">
+      <c r="U97" t="n">
+        <v>0</v>
+      </c>
+      <c r="V97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7406,7 +7946,13 @@
       <c r="T98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
+      <c r="U98" t="n">
+        <v>0</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7479,7 +8025,13 @@
       <c r="T99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U99" t="inlineStr">
+      <c r="U99" t="n">
+        <v>0</v>
+      </c>
+      <c r="V99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7552,7 +8104,13 @@
       <c r="T100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U100" t="inlineStr">
+      <c r="U100" t="n">
+        <v>0</v>
+      </c>
+      <c r="V100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7625,7 +8183,13 @@
       <c r="T101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U101" t="inlineStr">
+      <c r="U101" t="n">
+        <v>0</v>
+      </c>
+      <c r="V101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7698,7 +8262,13 @@
       <c r="T102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U102" t="inlineStr">
+      <c r="U102" t="n">
+        <v>0</v>
+      </c>
+      <c r="V102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7766,6 +8336,8 @@
       <c r="S103" t="inlineStr"/>
       <c r="T103" s="3" t="inlineStr"/>
       <c r="U103" t="inlineStr"/>
+      <c r="V103" s="3" t="inlineStr"/>
+      <c r="W103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -7829,6 +8401,8 @@
       <c r="S104" t="inlineStr"/>
       <c r="T104" s="3" t="inlineStr"/>
       <c r="U104" t="inlineStr"/>
+      <c r="V104" s="3" t="inlineStr"/>
+      <c r="W104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -7892,6 +8466,8 @@
       <c r="S105" t="inlineStr"/>
       <c r="T105" s="3" t="inlineStr"/>
       <c r="U105" t="inlineStr"/>
+      <c r="V105" s="3" t="inlineStr"/>
+      <c r="W105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -7955,6 +8531,8 @@
       <c r="S106" t="inlineStr"/>
       <c r="T106" s="3" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
+      <c r="V106" s="3" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8018,6 +8596,8 @@
       <c r="S107" t="inlineStr"/>
       <c r="T107" s="3" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
+      <c r="V107" s="3" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8081,6 +8661,8 @@
       <c r="S108" t="inlineStr"/>
       <c r="T108" s="3" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
+      <c r="V108" s="3" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8144,6 +8726,8 @@
       <c r="S109" t="inlineStr"/>
       <c r="T109" s="3" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
+      <c r="V109" s="3" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -8207,6 +8791,8 @@
       <c r="S110" t="inlineStr"/>
       <c r="T110" s="3" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
+      <c r="V110" s="3" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8270,6 +8856,8 @@
       <c r="S111" t="inlineStr"/>
       <c r="T111" s="3" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
+      <c r="V111" s="3" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8328,9 +8916,15 @@
       <c r="T112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U112" t="inlineStr">
-        <is>
-          <t>4342</t>
+      <c r="U112" t="n">
+        <v>4342</v>
+      </c>
+      <c r="V112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W112" t="inlineStr">
+        <is>
+          <t>4364</t>
         </is>
       </c>
     </row>
@@ -8391,9 +8985,15 @@
       <c r="T113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U113" t="inlineStr">
-        <is>
-          <t>2755</t>
+      <c r="U113" t="n">
+        <v>2755</v>
+      </c>
+      <c r="V113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W113" t="inlineStr">
+        <is>
+          <t>2776</t>
         </is>
       </c>
     </row>
@@ -8450,7 +9050,13 @@
       <c r="T114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U114" t="inlineStr">
+      <c r="U114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="V114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W114" t="inlineStr">
         <is>
           <t>1587</t>
         </is>
@@ -8509,9 +9115,15 @@
       <c r="T115" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="U115" t="inlineStr">
-        <is>
-          <t>4802</t>
+      <c r="U115" t="n">
+        <v>4802</v>
+      </c>
+      <c r="V115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>4876</t>
         </is>
       </c>
     </row>
@@ -8568,9 +9180,15 @@
       <c r="T116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="U116" t="inlineStr">
-        <is>
-          <t>3498</t>
+      <c r="U116" t="n">
+        <v>3498</v>
+      </c>
+      <c r="V116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>3591</t>
         </is>
       </c>
     </row>
@@ -8610,6 +9228,8 @@
       <c r="S117" t="inlineStr"/>
       <c r="T117" s="3" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
+      <c r="V117" s="3" t="inlineStr"/>
+      <c r="W117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8656,9 +9276,15 @@
       <c r="T118" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="U118" t="inlineStr">
-        <is>
-          <t>2693</t>
+      <c r="U118" t="n">
+        <v>2693</v>
+      </c>
+      <c r="V118" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="W118" t="inlineStr">
+        <is>
+          <t>2743</t>
         </is>
       </c>
     </row>
@@ -8698,6 +9324,8 @@
       <c r="S119" t="inlineStr"/>
       <c r="T119" s="3" t="inlineStr"/>
       <c r="U119" t="inlineStr"/>
+      <c r="V119" s="3" t="inlineStr"/>
+      <c r="W119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -8740,9 +9368,15 @@
       <c r="T120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>1468</t>
+      <c r="U120" t="n">
+        <v>1468</v>
+      </c>
+      <c r="V120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8787,7 +9421,13 @@
       <c r="T121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U121" t="inlineStr">
+      <c r="U121" t="n">
+        <v>0</v>
+      </c>
+      <c r="V121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8830,9 +9470,15 @@
       <c r="T122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="U122" t="n">
+        <v>2556</v>
+      </c>
+      <c r="V122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -8873,17 +9519,21 @@
       <c r="T123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>2538</t>
+      <c r="U123" t="n">
+        <v>2538</v>
+      </c>
+      <c r="V123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>2562</t>
         </is>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>59206405</t>
-        </is>
+      <c r="A124" t="n">
+        <v>59206405</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -8914,9 +9564,144 @@
       <c r="T124" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>1421</t>
+      <c r="U124" t="n">
+        <v>1421</v>
+      </c>
+      <c r="V124" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>1431</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>27113069</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>㊥DumbSmoky</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F125" s="3" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" s="3" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" s="3" t="inlineStr"/>
+      <c r="K125" t="inlineStr"/>
+      <c r="L125" s="3" t="inlineStr"/>
+      <c r="M125" t="inlineStr"/>
+      <c r="N125" s="3" t="inlineStr"/>
+      <c r="O125" t="inlineStr"/>
+      <c r="P125" s="3" t="inlineStr"/>
+      <c r="Q125" t="inlineStr"/>
+      <c r="R125" s="3" t="inlineStr"/>
+      <c r="S125" t="inlineStr"/>
+      <c r="T125" s="3" t="inlineStr"/>
+      <c r="U125" t="inlineStr"/>
+      <c r="V125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>2534</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>59222805</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>CAMILO</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F126" s="3" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" s="3" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" s="3" t="inlineStr"/>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" s="3" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" s="3" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" s="3" t="inlineStr"/>
+      <c r="Q126" t="inlineStr"/>
+      <c r="R126" s="3" t="inlineStr"/>
+      <c r="S126" t="inlineStr"/>
+      <c r="T126" s="3" t="inlineStr"/>
+      <c r="U126" t="inlineStr"/>
+      <c r="V126" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>1411</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>59231345</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Player-59231345</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F127" s="3" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" s="3" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" s="3" t="inlineStr"/>
+      <c r="K127" t="inlineStr"/>
+      <c r="L127" s="3" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" s="3" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" s="3" t="inlineStr"/>
+      <c r="Q127" t="inlineStr"/>
+      <c r="R127" s="3" t="inlineStr"/>
+      <c r="S127" t="inlineStr"/>
+      <c r="T127" s="3" t="inlineStr"/>
+      <c r="U127" t="inlineStr"/>
+      <c r="V127" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>1435</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-19 11:31:02
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W127"/>
+  <dimension ref="A1:Y127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -504,6 +504,16 @@
       <c r="W1" s="1" t="inlineStr">
         <is>
           <t>04-17_0</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>04-18_A</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>04-18_0</t>
         </is>
       </c>
     </row>
@@ -555,6 +565,8 @@
       <c r="U2" t="inlineStr"/>
       <c r="V2" s="3" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
+      <c r="X2" s="3" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -629,7 +641,13 @@
       <c r="V3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="W3" t="n">
+        <v>2551</v>
+      </c>
+      <c r="X3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>2551</t>
         </is>
@@ -708,7 +726,13 @@
       <c r="V4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -787,9 +811,15 @@
       <c r="V5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>4108</t>
+      <c r="W5" t="n">
+        <v>4108</v>
+      </c>
+      <c r="X5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>4166</t>
         </is>
       </c>
     </row>
@@ -866,9 +896,15 @@
       <c r="V6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="W6" t="n">
+        <v>2530</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2529</t>
         </is>
       </c>
     </row>
@@ -945,9 +981,15 @@
       <c r="V7" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>5028</t>
+      <c r="W7" t="n">
+        <v>5028</v>
+      </c>
+      <c r="X7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>5253</t>
         </is>
       </c>
     </row>
@@ -999,6 +1041,8 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" s="3" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
+      <c r="X8" s="3" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1073,9 +1117,15 @@
       <c r="V9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W9" t="inlineStr">
-        <is>
-          <t>3361</t>
+      <c r="W9" t="n">
+        <v>3361</v>
+      </c>
+      <c r="X9" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -1152,7 +1202,13 @@
       <c r="V10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W10" t="inlineStr">
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1231,7 +1287,13 @@
       <c r="V11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W11" t="inlineStr">
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1310,7 +1372,13 @@
       <c r="V12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W12" t="inlineStr">
+      <c r="W12" t="n">
+        <v>0</v>
+      </c>
+      <c r="X12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1389,9 +1457,15 @@
       <c r="V13" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="W13" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="W13" t="n">
+        <v>3989</v>
+      </c>
+      <c r="X13" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>4094</t>
         </is>
       </c>
     </row>
@@ -1468,9 +1542,15 @@
       <c r="V14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W14" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="W14" t="n">
+        <v>2685</v>
+      </c>
+      <c r="X14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>2716</t>
         </is>
       </c>
     </row>
@@ -1547,9 +1627,15 @@
       <c r="V15" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W15" t="inlineStr">
-        <is>
-          <t>4336</t>
+      <c r="W15" t="n">
+        <v>4336</v>
+      </c>
+      <c r="X15" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y15" t="inlineStr">
+        <is>
+          <t>4352</t>
         </is>
       </c>
     </row>
@@ -1625,6 +1711,8 @@
       </c>
       <c r="V16" s="3" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
+      <c r="X16" s="3" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1699,9 +1787,15 @@
       <c r="V17" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="W17" t="inlineStr">
-        <is>
-          <t>4808</t>
+      <c r="W17" t="n">
+        <v>4808</v>
+      </c>
+      <c r="X17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>4916</t>
         </is>
       </c>
     </row>
@@ -1778,9 +1872,15 @@
       <c r="V18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>4841</t>
+      <c r="W18" t="n">
+        <v>4841</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>4954</t>
         </is>
       </c>
     </row>
@@ -1857,9 +1957,15 @@
       <c r="V19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>5299</t>
+      <c r="W19" t="n">
+        <v>5299</v>
+      </c>
+      <c r="X19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>5599</t>
         </is>
       </c>
     </row>
@@ -1936,9 +2042,15 @@
       <c r="V20" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>4768</t>
+      <c r="W20" t="n">
+        <v>4768</v>
+      </c>
+      <c r="X20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>4871</t>
         </is>
       </c>
     </row>
@@ -2015,9 +2127,15 @@
       <c r="V21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>5147</t>
+      <c r="W21" t="n">
+        <v>5147</v>
+      </c>
+      <c r="X21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>5350</t>
         </is>
       </c>
     </row>
@@ -2094,9 +2212,15 @@
       <c r="V22" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>2982</t>
+      <c r="W22" t="n">
+        <v>2982</v>
+      </c>
+      <c r="X22" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>3401</t>
         </is>
       </c>
     </row>
@@ -2173,7 +2297,13 @@
       <c r="V23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W23" t="inlineStr">
+      <c r="W23" t="n">
+        <v>4259</v>
+      </c>
+      <c r="X23" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="inlineStr">
         <is>
           <t>4259</t>
         </is>
@@ -2252,7 +2382,13 @@
       <c r="V24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W24" t="inlineStr">
+      <c r="W24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2330,6 +2466,8 @@
       </c>
       <c r="V25" s="3" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
+      <c r="X25" s="3" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2404,9 +2542,15 @@
       <c r="V26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>4806</t>
+      <c r="W26" t="n">
+        <v>4806</v>
+      </c>
+      <c r="X26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -2483,9 +2627,15 @@
       <c r="V27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W27" t="inlineStr">
-        <is>
-          <t>3180</t>
+      <c r="W27" t="n">
+        <v>3180</v>
+      </c>
+      <c r="X27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>3624</t>
         </is>
       </c>
     </row>
@@ -2562,7 +2712,13 @@
       <c r="V28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W28" t="inlineStr">
+      <c r="W28" t="n">
+        <v>2569</v>
+      </c>
+      <c r="X28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y28" t="inlineStr">
         <is>
           <t>2569</t>
         </is>
@@ -2641,9 +2797,15 @@
       <c r="V29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>4666</t>
+      <c r="W29" t="n">
+        <v>4666</v>
+      </c>
+      <c r="X29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>4786</t>
         </is>
       </c>
     </row>
@@ -2720,9 +2882,15 @@
       <c r="V30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="W30" t="n">
+        <v>2668</v>
+      </c>
+      <c r="X30" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>3033</t>
         </is>
       </c>
     </row>
@@ -2799,9 +2967,15 @@
       <c r="V31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>4652</t>
+      <c r="W31" t="n">
+        <v>4652</v>
+      </c>
+      <c r="X31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>4715</t>
         </is>
       </c>
     </row>
@@ -2878,9 +3052,15 @@
       <c r="V32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>4494</t>
+      <c r="W32" t="n">
+        <v>4494</v>
+      </c>
+      <c r="X32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>4646</t>
         </is>
       </c>
     </row>
@@ -2956,6 +3136,8 @@
       </c>
       <c r="V33" s="3" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
+      <c r="X33" s="3" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3030,9 +3212,15 @@
       <c r="V34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="W34" t="n">
+        <v>2729</v>
+      </c>
+      <c r="X34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>2723</t>
         </is>
       </c>
     </row>
@@ -3109,9 +3297,15 @@
       <c r="V35" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>4305</t>
+      <c r="W35" t="n">
+        <v>4305</v>
+      </c>
+      <c r="X35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>4370</t>
         </is>
       </c>
     </row>
@@ -3188,9 +3382,15 @@
       <c r="V36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>3191</t>
+      <c r="W36" t="n">
+        <v>3191</v>
+      </c>
+      <c r="X36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>3287</t>
         </is>
       </c>
     </row>
@@ -3267,9 +3467,15 @@
       <c r="V37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>5044</t>
+      <c r="W37" t="n">
+        <v>5044</v>
+      </c>
+      <c r="X37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>5306</t>
         </is>
       </c>
     </row>
@@ -3346,9 +3552,15 @@
       <c r="V38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="W38" t="n">
+        <v>3994</v>
+      </c>
+      <c r="X38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>4123</t>
         </is>
       </c>
     </row>
@@ -3425,9 +3637,15 @@
       <c r="V39" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>3366</t>
+      <c r="W39" t="n">
+        <v>3366</v>
+      </c>
+      <c r="X39" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>3515</t>
         </is>
       </c>
     </row>
@@ -3504,9 +3722,15 @@
       <c r="V40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W40" t="inlineStr">
-        <is>
-          <t>5209</t>
+      <c r="W40" t="n">
+        <v>5209</v>
+      </c>
+      <c r="X40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>5395</t>
         </is>
       </c>
     </row>
@@ -3583,9 +3807,15 @@
       <c r="V41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>4995</t>
+      <c r="W41" t="n">
+        <v>4995</v>
+      </c>
+      <c r="X41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>5201</t>
         </is>
       </c>
     </row>
@@ -3662,9 +3892,15 @@
       <c r="V42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>4575</t>
+      <c r="W42" t="n">
+        <v>4575</v>
+      </c>
+      <c r="X42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>4789</t>
         </is>
       </c>
     </row>
@@ -3741,9 +3977,15 @@
       <c r="V43" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="W43" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="W43" t="n">
+        <v>4746</v>
+      </c>
+      <c r="X43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>4881</t>
         </is>
       </c>
     </row>
@@ -3820,9 +4062,15 @@
       <c r="V44" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>4488</t>
+      <c r="W44" t="n">
+        <v>4488</v>
+      </c>
+      <c r="X44" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>4654</t>
         </is>
       </c>
     </row>
@@ -3899,9 +4147,15 @@
       <c r="V45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="W45" t="n">
+        <v>4763</v>
+      </c>
+      <c r="X45" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>4944</t>
         </is>
       </c>
     </row>
@@ -3978,9 +4232,15 @@
       <c r="V46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>4505</t>
+      <c r="W46" t="n">
+        <v>4505</v>
+      </c>
+      <c r="X46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>4738</t>
         </is>
       </c>
     </row>
@@ -4057,9 +4317,15 @@
       <c r="V47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>4048</t>
+      <c r="W47" t="n">
+        <v>4048</v>
+      </c>
+      <c r="X47" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>4318</t>
         </is>
       </c>
     </row>
@@ -4136,9 +4402,15 @@
       <c r="V48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>4739</t>
+      <c r="W48" t="n">
+        <v>4739</v>
+      </c>
+      <c r="X48" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>5034</t>
         </is>
       </c>
     </row>
@@ -4215,9 +4487,15 @@
       <c r="V49" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>4155</t>
+      <c r="W49" t="n">
+        <v>4155</v>
+      </c>
+      <c r="X49" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>4195</t>
         </is>
       </c>
     </row>
@@ -4269,6 +4547,8 @@
       <c r="U50" t="inlineStr"/>
       <c r="V50" s="3" t="inlineStr"/>
       <c r="W50" t="inlineStr"/>
+      <c r="X50" s="3" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4343,9 +4623,15 @@
       <c r="V51" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W51" t="inlineStr">
-        <is>
-          <t>4101</t>
+      <c r="W51" t="n">
+        <v>4101</v>
+      </c>
+      <c r="X51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>4170</t>
         </is>
       </c>
     </row>
@@ -4422,9 +4708,15 @@
       <c r="V52" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="W52" t="n">
+        <v>4180</v>
+      </c>
+      <c r="X52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>4231</t>
         </is>
       </c>
     </row>
@@ -4501,9 +4793,15 @@
       <c r="V53" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>4160</t>
+      <c r="W53" t="n">
+        <v>4160</v>
+      </c>
+      <c r="X53" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>4213</t>
         </is>
       </c>
     </row>
@@ -4580,9 +4878,15 @@
       <c r="V54" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>4009</t>
+      <c r="W54" t="n">
+        <v>4009</v>
+      </c>
+      <c r="X54" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>4029</t>
         </is>
       </c>
     </row>
@@ -4659,9 +4963,15 @@
       <c r="V55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="W55" t="n">
+        <v>3988</v>
+      </c>
+      <c r="X55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -4738,9 +5048,15 @@
       <c r="V56" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>3999</t>
+      <c r="W56" t="n">
+        <v>3999</v>
+      </c>
+      <c r="X56" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>4035</t>
         </is>
       </c>
     </row>
@@ -4817,9 +5133,15 @@
       <c r="V57" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>4182</t>
+      <c r="W57" t="n">
+        <v>4182</v>
+      </c>
+      <c r="X57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>4261</t>
         </is>
       </c>
     </row>
@@ -4896,7 +5218,13 @@
       <c r="V58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W58" t="inlineStr">
+      <c r="W58" t="n">
+        <v>0</v>
+      </c>
+      <c r="X58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4975,9 +5303,15 @@
       <c r="V59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W59" t="inlineStr">
-        <is>
-          <t>2766</t>
+      <c r="W59" t="n">
+        <v>2766</v>
+      </c>
+      <c r="X59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>2777</t>
         </is>
       </c>
     </row>
@@ -5054,9 +5388,15 @@
       <c r="V60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>2467</t>
+      <c r="W60" t="n">
+        <v>2467</v>
+      </c>
+      <c r="X60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>2465</t>
         </is>
       </c>
     </row>
@@ -5133,9 +5473,15 @@
       <c r="V61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W61" t="inlineStr">
-        <is>
-          <t>3600</t>
+      <c r="W61" t="n">
+        <v>3600</v>
+      </c>
+      <c r="X61" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y61" t="inlineStr">
+        <is>
+          <t>4026</t>
         </is>
       </c>
     </row>
@@ -5212,9 +5558,15 @@
       <c r="V62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>1975</t>
+      <c r="W62" t="n">
+        <v>1975</v>
+      </c>
+      <c r="X62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>1987</t>
         </is>
       </c>
     </row>
@@ -5254,6 +5606,8 @@
       <c r="U63" t="inlineStr"/>
       <c r="V63" s="3" t="inlineStr"/>
       <c r="W63" t="inlineStr"/>
+      <c r="X63" s="3" t="inlineStr"/>
+      <c r="Y63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -5328,7 +5682,13 @@
       <c r="V64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W64" t="inlineStr">
+      <c r="W64" t="n">
+        <v>0</v>
+      </c>
+      <c r="X64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5390,6 +5750,8 @@
       <c r="U65" t="inlineStr"/>
       <c r="V65" s="3" t="inlineStr"/>
       <c r="W65" t="inlineStr"/>
+      <c r="X65" s="3" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5464,9 +5826,15 @@
       <c r="V66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W66" t="inlineStr">
-        <is>
-          <t>2480</t>
+      <c r="W66" t="n">
+        <v>2480</v>
+      </c>
+      <c r="X66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -5543,9 +5911,15 @@
       <c r="V67" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="W67" t="inlineStr">
-        <is>
-          <t>5041</t>
+      <c r="W67" t="n">
+        <v>5041</v>
+      </c>
+      <c r="X67" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y67" t="inlineStr">
+        <is>
+          <t>5173</t>
         </is>
       </c>
     </row>
@@ -5622,7 +5996,13 @@
       <c r="V68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W68" t="inlineStr">
+      <c r="W68" t="n">
+        <v>0</v>
+      </c>
+      <c r="X68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5701,9 +6081,15 @@
       <c r="V69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="W69" t="n">
+        <v>2560</v>
+      </c>
+      <c r="X69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>2618</t>
         </is>
       </c>
     </row>
@@ -5780,7 +6166,13 @@
       <c r="V70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W70" t="inlineStr">
+      <c r="W70" t="n">
+        <v>0</v>
+      </c>
+      <c r="X70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5859,9 +6251,15 @@
       <c r="V71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W71" t="inlineStr">
-        <is>
-          <t>3913</t>
+      <c r="W71" t="n">
+        <v>3913</v>
+      </c>
+      <c r="X71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y71" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -5938,9 +6336,15 @@
       <c r="V72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W72" t="inlineStr">
-        <is>
-          <t>3240</t>
+      <c r="W72" t="n">
+        <v>3240</v>
+      </c>
+      <c r="X72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="inlineStr">
+        <is>
+          <t>3234</t>
         </is>
       </c>
     </row>
@@ -6017,7 +6421,13 @@
       <c r="V73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W73" t="inlineStr">
+      <c r="W73" t="n">
+        <v>0</v>
+      </c>
+      <c r="X73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6096,7 +6506,13 @@
       <c r="V74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W74" t="inlineStr">
+      <c r="W74" t="n">
+        <v>0</v>
+      </c>
+      <c r="X74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6154,6 +6570,8 @@
       <c r="U75" t="inlineStr"/>
       <c r="V75" s="3" t="inlineStr"/>
       <c r="W75" t="inlineStr"/>
+      <c r="X75" s="3" t="inlineStr"/>
+      <c r="Y75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -6228,7 +6646,13 @@
       <c r="V76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W76" t="inlineStr">
+      <c r="W76" t="n">
+        <v>0</v>
+      </c>
+      <c r="X76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6307,9 +6731,15 @@
       <c r="V77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W77" t="inlineStr">
-        <is>
-          <t>3024</t>
+      <c r="W77" t="n">
+        <v>3024</v>
+      </c>
+      <c r="X77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>3019</t>
         </is>
       </c>
     </row>
@@ -6386,7 +6816,13 @@
       <c r="V78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W78" t="inlineStr">
+      <c r="W78" t="n">
+        <v>0</v>
+      </c>
+      <c r="X78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6465,7 +6901,13 @@
       <c r="V79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W79" t="inlineStr">
+      <c r="W79" t="n">
+        <v>0</v>
+      </c>
+      <c r="X79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6544,9 +6986,15 @@
       <c r="V80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W80" t="inlineStr">
-        <is>
-          <t>1447</t>
+      <c r="W80" t="n">
+        <v>1447</v>
+      </c>
+      <c r="X80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y80" t="inlineStr">
+        <is>
+          <t>1490</t>
         </is>
       </c>
     </row>
@@ -6623,7 +7071,13 @@
       <c r="V81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W81" t="inlineStr">
+      <c r="W81" t="n">
+        <v>0</v>
+      </c>
+      <c r="X81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6702,7 +7156,13 @@
       <c r="V82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W82" t="inlineStr">
+      <c r="W82" t="n">
+        <v>0</v>
+      </c>
+      <c r="X82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6781,7 +7241,13 @@
       <c r="V83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W83" t="inlineStr">
+      <c r="W83" t="n">
+        <v>0</v>
+      </c>
+      <c r="X83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6860,7 +7326,13 @@
       <c r="V84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W84" t="inlineStr">
+      <c r="W84" t="n">
+        <v>0</v>
+      </c>
+      <c r="X84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6939,7 +7411,13 @@
       <c r="V85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W85" t="inlineStr">
+      <c r="W85" t="n">
+        <v>0</v>
+      </c>
+      <c r="X85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7018,7 +7496,13 @@
       <c r="V86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W86" t="inlineStr">
+      <c r="W86" t="n">
+        <v>0</v>
+      </c>
+      <c r="X86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7097,7 +7581,13 @@
       <c r="V87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W87" t="inlineStr">
+      <c r="W87" t="n">
+        <v>0</v>
+      </c>
+      <c r="X87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7176,9 +7666,15 @@
       <c r="V88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W88" t="inlineStr">
-        <is>
-          <t>2648</t>
+      <c r="W88" t="n">
+        <v>2648</v>
+      </c>
+      <c r="X88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y88" t="inlineStr">
+        <is>
+          <t>2659</t>
         </is>
       </c>
     </row>
@@ -7255,7 +7751,13 @@
       <c r="V89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W89" t="inlineStr">
+      <c r="W89" t="n">
+        <v>0</v>
+      </c>
+      <c r="X89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7334,7 +7836,13 @@
       <c r="V90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W90" t="inlineStr">
+      <c r="W90" t="n">
+        <v>0</v>
+      </c>
+      <c r="X90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7404,6 +7912,8 @@
       <c r="U91" t="inlineStr"/>
       <c r="V91" s="3" t="inlineStr"/>
       <c r="W91" t="inlineStr"/>
+      <c r="X91" s="3" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -7478,7 +7988,13 @@
       <c r="V92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W92" t="inlineStr">
+      <c r="W92" t="n">
+        <v>0</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7557,9 +8073,15 @@
       <c r="V93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W93" t="inlineStr">
-        <is>
-          <t>3453</t>
+      <c r="W93" t="n">
+        <v>3453</v>
+      </c>
+      <c r="X93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y93" t="inlineStr">
+        <is>
+          <t>3438</t>
         </is>
       </c>
     </row>
@@ -7636,7 +8158,13 @@
       <c r="V94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W94" t="inlineStr">
+      <c r="W94" t="n">
+        <v>0</v>
+      </c>
+      <c r="X94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7715,7 +8243,13 @@
       <c r="V95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W95" t="inlineStr">
+      <c r="W95" t="n">
+        <v>0</v>
+      </c>
+      <c r="X95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7794,7 +8328,13 @@
       <c r="V96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W96" t="inlineStr">
+      <c r="W96" t="n">
+        <v>0</v>
+      </c>
+      <c r="X96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7873,7 +8413,13 @@
       <c r="V97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W97" t="inlineStr">
+      <c r="W97" t="n">
+        <v>0</v>
+      </c>
+      <c r="X97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7952,7 +8498,13 @@
       <c r="V98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W98" t="inlineStr">
+      <c r="W98" t="n">
+        <v>0</v>
+      </c>
+      <c r="X98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8031,7 +8583,13 @@
       <c r="V99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W99" t="inlineStr">
+      <c r="W99" t="n">
+        <v>0</v>
+      </c>
+      <c r="X99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8110,7 +8668,13 @@
       <c r="V100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W100" t="inlineStr">
+      <c r="W100" t="n">
+        <v>0</v>
+      </c>
+      <c r="X100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8189,7 +8753,13 @@
       <c r="V101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W101" t="inlineStr">
+      <c r="W101" t="n">
+        <v>0</v>
+      </c>
+      <c r="X101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8268,7 +8838,13 @@
       <c r="V102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W102" t="inlineStr">
+      <c r="W102" t="n">
+        <v>0</v>
+      </c>
+      <c r="X102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8338,6 +8914,8 @@
       <c r="U103" t="inlineStr"/>
       <c r="V103" s="3" t="inlineStr"/>
       <c r="W103" t="inlineStr"/>
+      <c r="X103" s="3" t="inlineStr"/>
+      <c r="Y103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -8403,6 +8981,8 @@
       <c r="U104" t="inlineStr"/>
       <c r="V104" s="3" t="inlineStr"/>
       <c r="W104" t="inlineStr"/>
+      <c r="X104" s="3" t="inlineStr"/>
+      <c r="Y104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -8468,6 +9048,8 @@
       <c r="U105" t="inlineStr"/>
       <c r="V105" s="3" t="inlineStr"/>
       <c r="W105" t="inlineStr"/>
+      <c r="X105" s="3" t="inlineStr"/>
+      <c r="Y105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -8533,6 +9115,8 @@
       <c r="U106" t="inlineStr"/>
       <c r="V106" s="3" t="inlineStr"/>
       <c r="W106" t="inlineStr"/>
+      <c r="X106" s="3" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8598,6 +9182,8 @@
       <c r="U107" t="inlineStr"/>
       <c r="V107" s="3" t="inlineStr"/>
       <c r="W107" t="inlineStr"/>
+      <c r="X107" s="3" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8663,6 +9249,8 @@
       <c r="U108" t="inlineStr"/>
       <c r="V108" s="3" t="inlineStr"/>
       <c r="W108" t="inlineStr"/>
+      <c r="X108" s="3" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8728,6 +9316,8 @@
       <c r="U109" t="inlineStr"/>
       <c r="V109" s="3" t="inlineStr"/>
       <c r="W109" t="inlineStr"/>
+      <c r="X109" s="3" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -8793,6 +9383,8 @@
       <c r="U110" t="inlineStr"/>
       <c r="V110" s="3" t="inlineStr"/>
       <c r="W110" t="inlineStr"/>
+      <c r="X110" s="3" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8858,6 +9450,8 @@
       <c r="U111" t="inlineStr"/>
       <c r="V111" s="3" t="inlineStr"/>
       <c r="W111" t="inlineStr"/>
+      <c r="X111" s="3" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8922,7 +9516,13 @@
       <c r="V112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W112" t="inlineStr">
+      <c r="W112" t="n">
+        <v>4364</v>
+      </c>
+      <c r="X112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y112" t="inlineStr">
         <is>
           <t>4364</t>
         </is>
@@ -8991,9 +9591,15 @@
       <c r="V113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W113" t="inlineStr">
-        <is>
-          <t>2776</t>
+      <c r="W113" t="n">
+        <v>2776</v>
+      </c>
+      <c r="X113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y113" t="inlineStr">
+        <is>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -9056,7 +9662,13 @@
       <c r="V114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W114" t="inlineStr">
+      <c r="W114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="X114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y114" t="inlineStr">
         <is>
           <t>1587</t>
         </is>
@@ -9121,9 +9733,15 @@
       <c r="V115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>4876</t>
+      <c r="W115" t="n">
+        <v>4876</v>
+      </c>
+      <c r="X115" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y115" t="inlineStr">
+        <is>
+          <t>5050</t>
         </is>
       </c>
     </row>
@@ -9186,9 +9804,15 @@
       <c r="V116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>3591</t>
+      <c r="W116" t="n">
+        <v>3591</v>
+      </c>
+      <c r="X116" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="Y116" t="inlineStr">
+        <is>
+          <t>3654</t>
         </is>
       </c>
     </row>
@@ -9230,6 +9854,8 @@
       <c r="U117" t="inlineStr"/>
       <c r="V117" s="3" t="inlineStr"/>
       <c r="W117" t="inlineStr"/>
+      <c r="X117" s="3" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -9282,9 +9908,15 @@
       <c r="V118" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="W118" t="inlineStr">
-        <is>
-          <t>2743</t>
+      <c r="W118" t="n">
+        <v>2743</v>
+      </c>
+      <c r="X118" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="Y118" t="inlineStr">
+        <is>
+          <t>2829</t>
         </is>
       </c>
     </row>
@@ -9326,6 +9958,8 @@
       <c r="U119" t="inlineStr"/>
       <c r="V119" s="3" t="inlineStr"/>
       <c r="W119" t="inlineStr"/>
+      <c r="X119" s="3" t="inlineStr"/>
+      <c r="Y119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -9374,9 +10008,15 @@
       <c r="V120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="W120" t="n">
+        <v>0</v>
+      </c>
+      <c r="X120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y120" t="inlineStr">
+        <is>
+          <t>1464</t>
         </is>
       </c>
     </row>
@@ -9427,7 +10067,13 @@
       <c r="V121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W121" t="inlineStr">
+      <c r="W121" t="n">
+        <v>0</v>
+      </c>
+      <c r="X121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9476,9 +10122,15 @@
       <c r="V122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W122" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="W122" t="n">
+        <v>2628</v>
+      </c>
+      <c r="X122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y122" t="inlineStr">
+        <is>
+          <t>2626</t>
         </is>
       </c>
     </row>
@@ -9525,9 +10177,15 @@
       <c r="V123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W123" t="inlineStr">
-        <is>
-          <t>2562</t>
+      <c r="W123" t="n">
+        <v>2562</v>
+      </c>
+      <c r="X123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y123" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -9570,17 +10228,21 @@
       <c r="V124" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>1431</t>
+      <c r="W124" t="n">
+        <v>1431</v>
+      </c>
+      <c r="X124" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y124" t="inlineStr">
+        <is>
+          <t>1441</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>27113069</t>
-        </is>
+      <c r="A125" t="n">
+        <v>27113069</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -9613,17 +10275,21 @@
       <c r="V125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W125" t="inlineStr">
+      <c r="W125" t="n">
+        <v>2534</v>
+      </c>
+      <c r="X125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y125" t="inlineStr">
         <is>
           <t>2534</t>
         </is>
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>59222805</t>
-        </is>
+      <c r="A126" t="n">
+        <v>59222805</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -9656,17 +10322,21 @@
       <c r="V126" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="W126" t="inlineStr">
-        <is>
-          <t>1411</t>
+      <c r="W126" t="n">
+        <v>1411</v>
+      </c>
+      <c r="X126" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y126" t="inlineStr">
+        <is>
+          <t>1506</t>
         </is>
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>59231345</t>
-        </is>
+      <c r="A127" t="n">
+        <v>59231345</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -9699,9 +10369,15 @@
       <c r="V127" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="W127" t="inlineStr">
-        <is>
-          <t>1435</t>
+      <c r="W127" t="n">
+        <v>1435</v>
+      </c>
+      <c r="X127" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y127" t="inlineStr">
+        <is>
+          <t>1490</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-20 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y127"/>
+  <dimension ref="A1:AA127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,6 +514,16 @@
       <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>04-18_0</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>04-19_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>04-19_0</t>
         </is>
       </c>
     </row>
@@ -567,6 +577,8 @@
       <c r="W2" t="inlineStr"/>
       <c r="X2" s="3" t="inlineStr"/>
       <c r="Y2" t="inlineStr"/>
+      <c r="Z2" s="3" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -647,7 +659,13 @@
       <c r="X3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Y3" t="n">
+        <v>2551</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>2551</t>
         </is>
@@ -732,7 +750,13 @@
       <c r="X4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -817,9 +841,15 @@
       <c r="X5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>4166</t>
+      <c r="Y5" t="n">
+        <v>4166</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>4285</t>
         </is>
       </c>
     </row>
@@ -902,9 +932,15 @@
       <c r="X6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>2529</t>
+      <c r="Y6" t="n">
+        <v>2529</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -987,9 +1023,15 @@
       <c r="X7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>5253</t>
+      <c r="Y7" t="n">
+        <v>5253</v>
+      </c>
+      <c r="Z7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>5459</t>
         </is>
       </c>
     </row>
@@ -1043,6 +1085,8 @@
       <c r="W8" t="inlineStr"/>
       <c r="X8" s="3" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
+      <c r="Z8" s="3" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1123,9 +1167,15 @@
       <c r="X9" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>3635</t>
+      <c r="Y9" t="n">
+        <v>3635</v>
+      </c>
+      <c r="Z9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>3650</t>
         </is>
       </c>
     </row>
@@ -1208,7 +1258,13 @@
       <c r="X10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y10" t="inlineStr">
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1293,7 +1349,13 @@
       <c r="X11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y11" t="inlineStr">
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1378,7 +1440,13 @@
       <c r="X12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y12" t="inlineStr">
+      <c r="Y12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1463,9 +1531,15 @@
       <c r="X13" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="Y13" t="inlineStr">
-        <is>
-          <t>4094</t>
+      <c r="Y13" t="n">
+        <v>4094</v>
+      </c>
+      <c r="Z13" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>4028</t>
         </is>
       </c>
     </row>
@@ -1548,9 +1622,15 @@
       <c r="X14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>2716</t>
+      <c r="Y14" t="n">
+        <v>2716</v>
+      </c>
+      <c r="Z14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA14" t="inlineStr">
+        <is>
+          <t>2748</t>
         </is>
       </c>
     </row>
@@ -1633,9 +1713,15 @@
       <c r="X15" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>4352</t>
+      <c r="Y15" t="n">
+        <v>4352</v>
+      </c>
+      <c r="Z15" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA15" t="inlineStr">
+        <is>
+          <t>4444</t>
         </is>
       </c>
     </row>
@@ -1713,6 +1799,8 @@
       <c r="W16" t="inlineStr"/>
       <c r="X16" s="3" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
+      <c r="Z16" s="3" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1793,9 +1881,15 @@
       <c r="X17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>4916</t>
+      <c r="Y17" t="n">
+        <v>4916</v>
+      </c>
+      <c r="Z17" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AA17" t="inlineStr">
+        <is>
+          <t>5003</t>
         </is>
       </c>
     </row>
@@ -1878,9 +1972,15 @@
       <c r="X18" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>4954</t>
+      <c r="Y18" t="n">
+        <v>4954</v>
+      </c>
+      <c r="Z18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>5118</t>
         </is>
       </c>
     </row>
@@ -1963,9 +2063,15 @@
       <c r="X19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>5599</t>
+      <c r="Y19" t="n">
+        <v>5599</v>
+      </c>
+      <c r="Z19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>5875</t>
         </is>
       </c>
     </row>
@@ -2048,9 +2154,15 @@
       <c r="X20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>4871</t>
+      <c r="Y20" t="n">
+        <v>4871</v>
+      </c>
+      <c r="Z20" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>5163</t>
         </is>
       </c>
     </row>
@@ -2133,9 +2245,15 @@
       <c r="X21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>5350</t>
+      <c r="Y21" t="n">
+        <v>5350</v>
+      </c>
+      <c r="Z21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>5604</t>
         </is>
       </c>
     </row>
@@ -2218,9 +2336,15 @@
       <c r="X22" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>3401</t>
+      <c r="Y22" t="n">
+        <v>3401</v>
+      </c>
+      <c r="Z22" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -2303,9 +2427,15 @@
       <c r="X23" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="Y23" t="n">
+        <v>4259</v>
+      </c>
+      <c r="Z23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>4589</t>
         </is>
       </c>
     </row>
@@ -2388,7 +2518,13 @@
       <c r="X24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y24" t="inlineStr">
+      <c r="Y24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2468,6 +2604,8 @@
       <c r="W25" t="inlineStr"/>
       <c r="X25" s="3" t="inlineStr"/>
       <c r="Y25" t="inlineStr"/>
+      <c r="Z25" s="3" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2548,9 +2686,15 @@
       <c r="X26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="Y26" t="n">
+        <v>4994</v>
+      </c>
+      <c r="Z26" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>5184</t>
         </is>
       </c>
     </row>
@@ -2633,9 +2777,15 @@
       <c r="X27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y27" t="inlineStr">
-        <is>
-          <t>3624</t>
+      <c r="Y27" t="n">
+        <v>3624</v>
+      </c>
+      <c r="Z27" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA27" t="inlineStr">
+        <is>
+          <t>3944</t>
         </is>
       </c>
     </row>
@@ -2718,9 +2868,15 @@
       <c r="X28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>2569</t>
+      <c r="Y28" t="n">
+        <v>2569</v>
+      </c>
+      <c r="Z28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -2803,9 +2959,15 @@
       <c r="X29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>4786</t>
+      <c r="Y29" t="n">
+        <v>4786</v>
+      </c>
+      <c r="Z29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -2888,9 +3050,15 @@
       <c r="X30" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>3033</t>
+      <c r="Y30" t="n">
+        <v>3033</v>
+      </c>
+      <c r="Z30" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>3561</t>
         </is>
       </c>
     </row>
@@ -2973,9 +3141,15 @@
       <c r="X31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>4715</t>
+      <c r="Y31" t="n">
+        <v>4715</v>
+      </c>
+      <c r="Z31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>4792</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3232,15 @@
       <c r="X32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y32" t="inlineStr">
-        <is>
-          <t>4646</t>
+      <c r="Y32" t="n">
+        <v>4646</v>
+      </c>
+      <c r="Z32" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>4636</t>
         </is>
       </c>
     </row>
@@ -3138,6 +3318,8 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" s="3" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
+      <c r="Z33" s="3" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3218,9 +3400,15 @@
       <c r="X34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>2723</t>
+      <c r="Y34" t="n">
+        <v>2723</v>
+      </c>
+      <c r="Z34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>2719</t>
         </is>
       </c>
     </row>
@@ -3303,9 +3491,15 @@
       <c r="X35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>4370</t>
+      <c r="Y35" t="n">
+        <v>4370</v>
+      </c>
+      <c r="Z35" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>4448</t>
         </is>
       </c>
     </row>
@@ -3388,9 +3582,15 @@
       <c r="X36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>3287</t>
+      <c r="Y36" t="n">
+        <v>3287</v>
+      </c>
+      <c r="Z36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>3351</t>
         </is>
       </c>
     </row>
@@ -3473,9 +3673,15 @@
       <c r="X37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>5306</t>
+      <c r="Y37" t="n">
+        <v>5306</v>
+      </c>
+      <c r="Z37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>5472</t>
         </is>
       </c>
     </row>
@@ -3558,9 +3764,15 @@
       <c r="X38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>4123</t>
+      <c r="Y38" t="n">
+        <v>4123</v>
+      </c>
+      <c r="Z38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>4062</t>
         </is>
       </c>
     </row>
@@ -3643,9 +3855,15 @@
       <c r="X39" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>3515</t>
+      <c r="Y39" t="n">
+        <v>3515</v>
+      </c>
+      <c r="Z39" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>3703</t>
         </is>
       </c>
     </row>
@@ -3728,9 +3946,15 @@
       <c r="X40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y40" t="inlineStr">
-        <is>
-          <t>5395</t>
+      <c r="Y40" t="n">
+        <v>5395</v>
+      </c>
+      <c r="Z40" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA40" t="inlineStr">
+        <is>
+          <t>5488</t>
         </is>
       </c>
     </row>
@@ -3813,9 +4037,15 @@
       <c r="X41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>5201</t>
+      <c r="Y41" t="n">
+        <v>5201</v>
+      </c>
+      <c r="Z41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>5329</t>
         </is>
       </c>
     </row>
@@ -3898,9 +4128,15 @@
       <c r="X42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y42" t="inlineStr">
-        <is>
-          <t>4789</t>
+      <c r="Y42" t="n">
+        <v>4789</v>
+      </c>
+      <c r="Z42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>4892</t>
         </is>
       </c>
     </row>
@@ -3983,9 +4219,15 @@
       <c r="X43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y43" t="inlineStr">
-        <is>
-          <t>4881</t>
+      <c r="Y43" t="n">
+        <v>4881</v>
+      </c>
+      <c r="Z43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA43" t="inlineStr">
+        <is>
+          <t>5002</t>
         </is>
       </c>
     </row>
@@ -4068,9 +4310,15 @@
       <c r="X44" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="Y44" t="inlineStr">
-        <is>
-          <t>4654</t>
+      <c r="Y44" t="n">
+        <v>4654</v>
+      </c>
+      <c r="Z44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA44" t="inlineStr">
+        <is>
+          <t>4868</t>
         </is>
       </c>
     </row>
@@ -4153,9 +4401,15 @@
       <c r="X45" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Y45" t="inlineStr">
-        <is>
-          <t>4944</t>
+      <c r="Y45" t="n">
+        <v>4944</v>
+      </c>
+      <c r="Z45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>5010</t>
         </is>
       </c>
     </row>
@@ -4238,9 +4492,15 @@
       <c r="X46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>4738</t>
+      <c r="Y46" t="n">
+        <v>4738</v>
+      </c>
+      <c r="Z46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>4861</t>
         </is>
       </c>
     </row>
@@ -4323,9 +4583,15 @@
       <c r="X47" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="Y47" t="inlineStr">
-        <is>
-          <t>4318</t>
+      <c r="Y47" t="n">
+        <v>4318</v>
+      </c>
+      <c r="Z47" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>4580</t>
         </is>
       </c>
     </row>
@@ -4408,9 +4674,15 @@
       <c r="X48" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y48" t="inlineStr">
-        <is>
-          <t>5034</t>
+      <c r="Y48" t="n">
+        <v>5034</v>
+      </c>
+      <c r="Z48" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>5262</t>
         </is>
       </c>
     </row>
@@ -4493,9 +4765,15 @@
       <c r="X49" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="Y49" t="inlineStr">
-        <is>
-          <t>4195</t>
+      <c r="Y49" t="n">
+        <v>4195</v>
+      </c>
+      <c r="Z49" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>4327</t>
         </is>
       </c>
     </row>
@@ -4549,6 +4827,8 @@
       <c r="W50" t="inlineStr"/>
       <c r="X50" s="3" t="inlineStr"/>
       <c r="Y50" t="inlineStr"/>
+      <c r="Z50" s="3" t="inlineStr"/>
+      <c r="AA50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4629,9 +4909,15 @@
       <c r="X51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y51" t="inlineStr">
-        <is>
-          <t>4170</t>
+      <c r="Y51" t="n">
+        <v>4170</v>
+      </c>
+      <c r="Z51" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>4276</t>
         </is>
       </c>
     </row>
@@ -4714,9 +5000,15 @@
       <c r="X52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>4231</t>
+      <c r="Y52" t="n">
+        <v>4231</v>
+      </c>
+      <c r="Z52" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>4310</t>
         </is>
       </c>
     </row>
@@ -4799,9 +5091,15 @@
       <c r="X53" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>4213</t>
+      <c r="Y53" t="n">
+        <v>4213</v>
+      </c>
+      <c r="Z53" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>4302</t>
         </is>
       </c>
     </row>
@@ -4884,9 +5182,15 @@
       <c r="X54" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>4029</t>
+      <c r="Y54" t="n">
+        <v>4029</v>
+      </c>
+      <c r="Z54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>4108</t>
         </is>
       </c>
     </row>
@@ -4969,9 +5273,15 @@
       <c r="X55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>3998</t>
+      <c r="Y55" t="n">
+        <v>3998</v>
+      </c>
+      <c r="Z55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>4100</t>
         </is>
       </c>
     </row>
@@ -5054,9 +5364,15 @@
       <c r="X56" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>4035</t>
+      <c r="Y56" t="n">
+        <v>4035</v>
+      </c>
+      <c r="Z56" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>4094</t>
         </is>
       </c>
     </row>
@@ -5139,9 +5455,15 @@
       <c r="X57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>4261</t>
+      <c r="Y57" t="n">
+        <v>4261</v>
+      </c>
+      <c r="Z57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>4368</t>
         </is>
       </c>
     </row>
@@ -5224,7 +5546,13 @@
       <c r="X58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y58" t="inlineStr">
+      <c r="Y58" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5309,9 +5637,15 @@
       <c r="X59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>2777</t>
+      <c r="Y59" t="n">
+        <v>2777</v>
+      </c>
+      <c r="Z59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>2851</t>
         </is>
       </c>
     </row>
@@ -5394,9 +5728,15 @@
       <c r="X60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>2465</t>
+      <c r="Y60" t="n">
+        <v>2465</v>
+      </c>
+      <c r="Z60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>2461</t>
         </is>
       </c>
     </row>
@@ -5479,9 +5819,15 @@
       <c r="X61" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Y61" t="inlineStr">
-        <is>
-          <t>4026</t>
+      <c r="Y61" t="n">
+        <v>4026</v>
+      </c>
+      <c r="Z61" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA61" t="inlineStr">
+        <is>
+          <t>4024</t>
         </is>
       </c>
     </row>
@@ -5564,9 +5910,15 @@
       <c r="X62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>1987</t>
+      <c r="Y62" t="n">
+        <v>1987</v>
+      </c>
+      <c r="Z62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>1981</t>
         </is>
       </c>
     </row>
@@ -5608,6 +5960,8 @@
       <c r="W63" t="inlineStr"/>
       <c r="X63" s="3" t="inlineStr"/>
       <c r="Y63" t="inlineStr"/>
+      <c r="Z63" s="3" t="inlineStr"/>
+      <c r="AA63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -5688,7 +6042,13 @@
       <c r="X64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y64" t="inlineStr">
+      <c r="Y64" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5752,6 +6112,8 @@
       <c r="W65" t="inlineStr"/>
       <c r="X65" s="3" t="inlineStr"/>
       <c r="Y65" t="inlineStr"/>
+      <c r="Z65" s="3" t="inlineStr"/>
+      <c r="AA65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5832,11 +6194,11 @@
       <c r="X66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y66" t="inlineStr">
-        <is>
-          <t>2524</t>
-        </is>
-      </c>
+      <c r="Y66" t="n">
+        <v>2524</v>
+      </c>
+      <c r="Z66" s="3" t="inlineStr"/>
+      <c r="AA66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -5917,9 +6279,15 @@
       <c r="X67" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y67" t="inlineStr">
-        <is>
-          <t>5173</t>
+      <c r="Y67" t="n">
+        <v>5173</v>
+      </c>
+      <c r="Z67" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA67" t="inlineStr">
+        <is>
+          <t>5295</t>
         </is>
       </c>
     </row>
@@ -6002,7 +6370,13 @@
       <c r="X68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y68" t="inlineStr">
+      <c r="Y68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6087,9 +6461,15 @@
       <c r="X69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>2618</t>
+      <c r="Y69" t="n">
+        <v>2618</v>
+      </c>
+      <c r="Z69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -6172,7 +6552,13 @@
       <c r="X70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y70" t="inlineStr">
+      <c r="Y70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6257,9 +6643,15 @@
       <c r="X71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y71" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="Y71" t="n">
+        <v>3992</v>
+      </c>
+      <c r="Z71" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA71" t="inlineStr">
+        <is>
+          <t>4347</t>
         </is>
       </c>
     </row>
@@ -6342,9 +6734,15 @@
       <c r="X72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y72" t="inlineStr">
-        <is>
-          <t>3234</t>
+      <c r="Y72" t="n">
+        <v>3234</v>
+      </c>
+      <c r="Z72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA72" t="inlineStr">
+        <is>
+          <t>3271</t>
         </is>
       </c>
     </row>
@@ -6427,7 +6825,13 @@
       <c r="X73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y73" t="inlineStr">
+      <c r="Y73" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6512,9 +6916,15 @@
       <c r="X74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y74" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Y74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA74" t="inlineStr">
+        <is>
+          <t>1229</t>
         </is>
       </c>
     </row>
@@ -6572,6 +6982,8 @@
       <c r="W75" t="inlineStr"/>
       <c r="X75" s="3" t="inlineStr"/>
       <c r="Y75" t="inlineStr"/>
+      <c r="Z75" s="3" t="inlineStr"/>
+      <c r="AA75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -6652,7 +7064,13 @@
       <c r="X76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y76" t="inlineStr">
+      <c r="Y76" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6737,9 +7155,15 @@
       <c r="X77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y77" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="Y77" t="n">
+        <v>3019</v>
+      </c>
+      <c r="Z77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>3043</t>
         </is>
       </c>
     </row>
@@ -6822,7 +7246,13 @@
       <c r="X78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y78" t="inlineStr">
+      <c r="Y78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6907,7 +7337,13 @@
       <c r="X79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y79" t="inlineStr">
+      <c r="Y79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6992,9 +7428,15 @@
       <c r="X80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y80" t="inlineStr">
-        <is>
-          <t>1490</t>
+      <c r="Y80" t="n">
+        <v>1490</v>
+      </c>
+      <c r="Z80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA80" t="inlineStr">
+        <is>
+          <t>1489</t>
         </is>
       </c>
     </row>
@@ -7077,7 +7519,13 @@
       <c r="X81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y81" t="inlineStr">
+      <c r="Y81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7162,7 +7610,13 @@
       <c r="X82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y82" t="inlineStr">
+      <c r="Y82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7247,7 +7701,13 @@
       <c r="X83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y83" t="inlineStr">
+      <c r="Y83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7332,7 +7792,13 @@
       <c r="X84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y84" t="inlineStr">
+      <c r="Y84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7417,7 +7883,13 @@
       <c r="X85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y85" t="inlineStr">
+      <c r="Y85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7502,7 +7974,13 @@
       <c r="X86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y86" t="inlineStr">
+      <c r="Y86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7587,7 +8065,13 @@
       <c r="X87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y87" t="inlineStr">
+      <c r="Y87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7672,9 +8156,15 @@
       <c r="X88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y88" t="inlineStr">
-        <is>
-          <t>2659</t>
+      <c r="Y88" t="n">
+        <v>2659</v>
+      </c>
+      <c r="Z88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA88" t="inlineStr">
+        <is>
+          <t>2746</t>
         </is>
       </c>
     </row>
@@ -7757,7 +8247,13 @@
       <c r="X89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y89" t="inlineStr">
+      <c r="Y89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7842,7 +8338,13 @@
       <c r="X90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y90" t="inlineStr">
+      <c r="Y90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7914,6 +8416,8 @@
       <c r="W91" t="inlineStr"/>
       <c r="X91" s="3" t="inlineStr"/>
       <c r="Y91" t="inlineStr"/>
+      <c r="Z91" s="3" t="inlineStr"/>
+      <c r="AA91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -7994,7 +8498,13 @@
       <c r="X92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y92" t="inlineStr">
+      <c r="Y92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8079,9 +8589,15 @@
       <c r="X93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y93" t="inlineStr">
-        <is>
-          <t>3438</t>
+      <c r="Y93" t="n">
+        <v>3438</v>
+      </c>
+      <c r="Z93" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA93" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -8164,7 +8680,13 @@
       <c r="X94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y94" t="inlineStr">
+      <c r="Y94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8249,7 +8771,13 @@
       <c r="X95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y95" t="inlineStr">
+      <c r="Y95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8334,7 +8862,13 @@
       <c r="X96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y96" t="inlineStr">
+      <c r="Y96" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8419,7 +8953,13 @@
       <c r="X97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y97" t="inlineStr">
+      <c r="Y97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8504,7 +9044,13 @@
       <c r="X98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y98" t="inlineStr">
+      <c r="Y98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8589,7 +9135,13 @@
       <c r="X99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y99" t="inlineStr">
+      <c r="Y99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8674,7 +9226,13 @@
       <c r="X100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y100" t="inlineStr">
+      <c r="Y100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8759,7 +9317,13 @@
       <c r="X101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y101" t="inlineStr">
+      <c r="Y101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8844,7 +9408,13 @@
       <c r="X102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y102" t="inlineStr">
+      <c r="Y102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8916,6 +9486,8 @@
       <c r="W103" t="inlineStr"/>
       <c r="X103" s="3" t="inlineStr"/>
       <c r="Y103" t="inlineStr"/>
+      <c r="Z103" s="3" t="inlineStr"/>
+      <c r="AA103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -8983,6 +9555,8 @@
       <c r="W104" t="inlineStr"/>
       <c r="X104" s="3" t="inlineStr"/>
       <c r="Y104" t="inlineStr"/>
+      <c r="Z104" s="3" t="inlineStr"/>
+      <c r="AA104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -9050,6 +9624,8 @@
       <c r="W105" t="inlineStr"/>
       <c r="X105" s="3" t="inlineStr"/>
       <c r="Y105" t="inlineStr"/>
+      <c r="Z105" s="3" t="inlineStr"/>
+      <c r="AA105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9117,6 +9693,8 @@
       <c r="W106" t="inlineStr"/>
       <c r="X106" s="3" t="inlineStr"/>
       <c r="Y106" t="inlineStr"/>
+      <c r="Z106" s="3" t="inlineStr"/>
+      <c r="AA106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9184,6 +9762,8 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" s="3" t="inlineStr"/>
       <c r="Y107" t="inlineStr"/>
+      <c r="Z107" s="3" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9251,6 +9831,8 @@
       <c r="W108" t="inlineStr"/>
       <c r="X108" s="3" t="inlineStr"/>
       <c r="Y108" t="inlineStr"/>
+      <c r="Z108" s="3" t="inlineStr"/>
+      <c r="AA108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9318,6 +9900,8 @@
       <c r="W109" t="inlineStr"/>
       <c r="X109" s="3" t="inlineStr"/>
       <c r="Y109" t="inlineStr"/>
+      <c r="Z109" s="3" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9385,6 +9969,8 @@
       <c r="W110" t="inlineStr"/>
       <c r="X110" s="3" t="inlineStr"/>
       <c r="Y110" t="inlineStr"/>
+      <c r="Z110" s="3" t="inlineStr"/>
+      <c r="AA110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9452,6 +10038,8 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" s="3" t="inlineStr"/>
       <c r="Y111" t="inlineStr"/>
+      <c r="Z111" s="3" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -9522,7 +10110,13 @@
       <c r="X112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y112" t="inlineStr">
+      <c r="Y112" t="n">
+        <v>4364</v>
+      </c>
+      <c r="Z112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA112" t="inlineStr">
         <is>
           <t>4364</t>
         </is>
@@ -9597,9 +10191,15 @@
       <c r="X113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y113" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="Y113" t="n">
+        <v>2819</v>
+      </c>
+      <c r="Z113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA113" t="inlineStr">
+        <is>
+          <t>2898</t>
         </is>
       </c>
     </row>
@@ -9668,7 +10268,13 @@
       <c r="X114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y114" t="inlineStr">
+      <c r="Y114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="Z114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA114" t="inlineStr">
         <is>
           <t>1587</t>
         </is>
@@ -9739,9 +10345,15 @@
       <c r="X115" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Y115" t="inlineStr">
-        <is>
-          <t>5050</t>
+      <c r="Y115" t="n">
+        <v>5050</v>
+      </c>
+      <c r="Z115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>5209</t>
         </is>
       </c>
     </row>
@@ -9810,9 +10422,15 @@
       <c r="X116" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="Y116" t="inlineStr">
-        <is>
-          <t>3654</t>
+      <c r="Y116" t="n">
+        <v>3654</v>
+      </c>
+      <c r="Z116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA116" t="inlineStr">
+        <is>
+          <t>3704</t>
         </is>
       </c>
     </row>
@@ -9856,6 +10474,8 @@
       <c r="W117" t="inlineStr"/>
       <c r="X117" s="3" t="inlineStr"/>
       <c r="Y117" t="inlineStr"/>
+      <c r="Z117" s="3" t="inlineStr"/>
+      <c r="AA117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -9914,9 +10534,15 @@
       <c r="X118" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="Y118" t="inlineStr">
-        <is>
-          <t>2829</t>
+      <c r="Y118" t="n">
+        <v>2829</v>
+      </c>
+      <c r="Z118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA118" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -9960,6 +10586,8 @@
       <c r="W119" t="inlineStr"/>
       <c r="X119" s="3" t="inlineStr"/>
       <c r="Y119" t="inlineStr"/>
+      <c r="Z119" s="3" t="inlineStr"/>
+      <c r="AA119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -10014,9 +10642,15 @@
       <c r="X120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y120" t="inlineStr">
-        <is>
-          <t>1464</t>
+      <c r="Y120" t="n">
+        <v>1464</v>
+      </c>
+      <c r="Z120" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA120" t="inlineStr">
+        <is>
+          <t>1477</t>
         </is>
       </c>
     </row>
@@ -10073,7 +10707,13 @@
       <c r="X121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y121" t="inlineStr">
+      <c r="Y121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10128,9 +10768,15 @@
       <c r="X122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y122" t="inlineStr">
-        <is>
-          <t>2626</t>
+      <c r="Y122" t="n">
+        <v>2626</v>
+      </c>
+      <c r="Z122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA122" t="inlineStr">
+        <is>
+          <t>2723</t>
         </is>
       </c>
     </row>
@@ -10183,9 +10829,15 @@
       <c r="X123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y123" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="Y123" t="n">
+        <v>2578</v>
+      </c>
+      <c r="Z123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA123" t="inlineStr">
+        <is>
+          <t>2576</t>
         </is>
       </c>
     </row>
@@ -10234,9 +10886,15 @@
       <c r="X124" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Y124" t="inlineStr">
-        <is>
-          <t>1441</t>
+      <c r="Y124" t="n">
+        <v>1441</v>
+      </c>
+      <c r="Z124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA124" t="inlineStr">
+        <is>
+          <t>1445</t>
         </is>
       </c>
     </row>
@@ -10281,9 +10939,15 @@
       <c r="X125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y125" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="Y125" t="n">
+        <v>2534</v>
+      </c>
+      <c r="Z125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA125" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -10328,9 +10992,15 @@
       <c r="X126" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="Y126" t="inlineStr">
-        <is>
-          <t>1506</t>
+      <c r="Y126" t="n">
+        <v>1506</v>
+      </c>
+      <c r="Z126" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA126" t="inlineStr">
+        <is>
+          <t>1674</t>
         </is>
       </c>
     </row>
@@ -10375,9 +11045,15 @@
       <c r="X127" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Y127" t="inlineStr">
-        <is>
-          <t>1490</t>
+      <c r="Y127" t="n">
+        <v>1490</v>
+      </c>
+      <c r="Z127" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA127" t="inlineStr">
+        <is>
+          <t>1537</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-21 11:31:15
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA127"/>
+  <dimension ref="A1:AC127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,16 @@
       <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>04-19_0</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>04-20_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>04-20_0</t>
         </is>
       </c>
     </row>
@@ -579,6 +589,8 @@
       <c r="Y2" t="inlineStr"/>
       <c r="Z2" s="3" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
+      <c r="AB2" s="3" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -665,7 +677,13 @@
       <c r="Z3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AA3" t="n">
+        <v>2551</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="inlineStr">
         <is>
           <t>2551</t>
         </is>
@@ -756,7 +774,13 @@
       <c r="Z4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -847,9 +871,15 @@
       <c r="Z5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>4285</t>
+      <c r="AA5" t="n">
+        <v>4285</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>4393</t>
         </is>
       </c>
     </row>
@@ -938,9 +968,15 @@
       <c r="Z6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="AA6" t="n">
+        <v>2522</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>2536</t>
         </is>
       </c>
     </row>
@@ -1029,9 +1065,15 @@
       <c r="Z7" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>5459</t>
+      <c r="AA7" t="n">
+        <v>5459</v>
+      </c>
+      <c r="AB7" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>5616</t>
         </is>
       </c>
     </row>
@@ -1087,6 +1129,8 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" s="3" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
+      <c r="AB8" s="3" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1173,9 +1217,15 @@
       <c r="Z9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>3650</t>
+      <c r="AA9" t="n">
+        <v>3650</v>
+      </c>
+      <c r="AB9" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>3747</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1314,13 @@
       <c r="Z10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA10" t="inlineStr">
+      <c r="AA10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1355,7 +1411,13 @@
       <c r="Z11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA11" t="inlineStr">
+      <c r="AA11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1446,7 +1508,13 @@
       <c r="Z12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA12" t="inlineStr">
+      <c r="AA12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1537,9 +1605,15 @@
       <c r="Z13" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AA13" t="inlineStr">
-        <is>
-          <t>4028</t>
+      <c r="AA13" t="n">
+        <v>4028</v>
+      </c>
+      <c r="AB13" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>4104</t>
         </is>
       </c>
     </row>
@@ -1628,9 +1702,15 @@
       <c r="Z14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>2748</t>
+      <c r="AA14" t="n">
+        <v>2748</v>
+      </c>
+      <c r="AB14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>2812</t>
         </is>
       </c>
     </row>
@@ -1719,9 +1799,15 @@
       <c r="Z15" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="AA15" t="inlineStr">
-        <is>
-          <t>4444</t>
+      <c r="AA15" t="n">
+        <v>4444</v>
+      </c>
+      <c r="AB15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>4425</t>
         </is>
       </c>
     </row>
@@ -1801,6 +1887,8 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" s="3" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
+      <c r="AB16" s="3" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1887,9 +1975,15 @@
       <c r="Z17" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AA17" t="inlineStr">
-        <is>
-          <t>5003</t>
+      <c r="AA17" t="n">
+        <v>5003</v>
+      </c>
+      <c r="AB17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>5228</t>
         </is>
       </c>
     </row>
@@ -1978,9 +2072,15 @@
       <c r="Z18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>5118</t>
+      <c r="AA18" t="n">
+        <v>5118</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>5195</t>
         </is>
       </c>
     </row>
@@ -2069,9 +2169,15 @@
       <c r="Z19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>5875</t>
+      <c r="AA19" t="n">
+        <v>5875</v>
+      </c>
+      <c r="AB19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>6064</t>
         </is>
       </c>
     </row>
@@ -2160,9 +2266,15 @@
       <c r="Z20" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>5163</t>
+      <c r="AA20" t="n">
+        <v>5163</v>
+      </c>
+      <c r="AB20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>5284</t>
         </is>
       </c>
     </row>
@@ -2251,9 +2363,15 @@
       <c r="Z21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>5604</t>
+      <c r="AA21" t="n">
+        <v>5604</v>
+      </c>
+      <c r="AB21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>5860</t>
         </is>
       </c>
     </row>
@@ -2342,9 +2460,15 @@
       <c r="Z22" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="AA22" t="n">
+        <v>3990</v>
+      </c>
+      <c r="AB22" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -2433,9 +2557,15 @@
       <c r="Z23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>4589</t>
+      <c r="AA23" t="n">
+        <v>4589</v>
+      </c>
+      <c r="AB23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>4909</t>
         </is>
       </c>
     </row>
@@ -2524,7 +2654,13 @@
       <c r="Z24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA24" t="inlineStr">
+      <c r="AA24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2606,6 +2742,8 @@
       <c r="Y25" t="inlineStr"/>
       <c r="Z25" s="3" t="inlineStr"/>
       <c r="AA25" t="inlineStr"/>
+      <c r="AB25" s="3" t="inlineStr"/>
+      <c r="AC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2692,9 +2830,15 @@
       <c r="Z26" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>5184</t>
+      <c r="AA26" t="n">
+        <v>5184</v>
+      </c>
+      <c r="AB26" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>5241</t>
         </is>
       </c>
     </row>
@@ -2783,9 +2927,15 @@
       <c r="Z27" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>3944</t>
+      <c r="AA27" t="n">
+        <v>3944</v>
+      </c>
+      <c r="AB27" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>4329</t>
         </is>
       </c>
     </row>
@@ -2874,7 +3024,13 @@
       <c r="Z28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA28" t="inlineStr">
+      <c r="AA28" t="n">
+        <v>2601</v>
+      </c>
+      <c r="AB28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC28" t="inlineStr">
         <is>
           <t>2601</t>
         </is>
@@ -2965,9 +3121,15 @@
       <c r="Z29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA29" t="inlineStr">
-        <is>
-          <t>4945</t>
+      <c r="AA29" t="n">
+        <v>4945</v>
+      </c>
+      <c r="AB29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>5072</t>
         </is>
       </c>
     </row>
@@ -3056,9 +3218,15 @@
       <c r="Z30" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>3561</t>
+      <c r="AA30" t="n">
+        <v>3561</v>
+      </c>
+      <c r="AB30" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>3924</t>
         </is>
       </c>
     </row>
@@ -3147,9 +3315,15 @@
       <c r="Z31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>4792</t>
+      <c r="AA31" t="n">
+        <v>4792</v>
+      </c>
+      <c r="AB31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>4930</t>
         </is>
       </c>
     </row>
@@ -3238,9 +3412,15 @@
       <c r="Z32" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>4636</t>
+      <c r="AA32" t="n">
+        <v>4636</v>
+      </c>
+      <c r="AB32" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>4652</t>
         </is>
       </c>
     </row>
@@ -3320,6 +3500,8 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" s="3" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
+      <c r="AB33" s="3" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3406,9 +3588,15 @@
       <c r="Z34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA34" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="AA34" t="n">
+        <v>2719</v>
+      </c>
+      <c r="AB34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>2712</t>
         </is>
       </c>
     </row>
@@ -3497,9 +3685,15 @@
       <c r="Z35" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>4448</t>
+      <c r="AA35" t="n">
+        <v>4448</v>
+      </c>
+      <c r="AB35" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -3588,9 +3782,15 @@
       <c r="Z36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>3351</t>
+      <c r="AA36" t="n">
+        <v>3351</v>
+      </c>
+      <c r="AB36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>3420</t>
         </is>
       </c>
     </row>
@@ -3679,9 +3879,15 @@
       <c r="Z37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>5472</t>
+      <c r="AA37" t="n">
+        <v>5472</v>
+      </c>
+      <c r="AB37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>5656</t>
         </is>
       </c>
     </row>
@@ -3770,9 +3976,15 @@
       <c r="Z38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>4062</t>
+      <c r="AA38" t="n">
+        <v>4062</v>
+      </c>
+      <c r="AB38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>4081</t>
         </is>
       </c>
     </row>
@@ -3861,9 +4073,15 @@
       <c r="Z39" s="4" t="n">
         <v>11</v>
       </c>
-      <c r="AA39" t="inlineStr">
-        <is>
-          <t>3703</t>
+      <c r="AA39" t="n">
+        <v>3703</v>
+      </c>
+      <c r="AB39" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>3886</t>
         </is>
       </c>
     </row>
@@ -3952,9 +4170,15 @@
       <c r="Z40" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA40" t="inlineStr">
-        <is>
-          <t>5488</t>
+      <c r="AA40" t="n">
+        <v>5488</v>
+      </c>
+      <c r="AB40" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>5704</t>
         </is>
       </c>
     </row>
@@ -4043,9 +4267,15 @@
       <c r="Z41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>5329</t>
+      <c r="AA41" t="n">
+        <v>5329</v>
+      </c>
+      <c r="AB41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>5463</t>
         </is>
       </c>
     </row>
@@ -4134,9 +4364,15 @@
       <c r="Z42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>4892</t>
+      <c r="AA42" t="n">
+        <v>4892</v>
+      </c>
+      <c r="AB42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>4996</t>
         </is>
       </c>
     </row>
@@ -4225,9 +4461,15 @@
       <c r="Z43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA43" t="inlineStr">
-        <is>
-          <t>5002</t>
+      <c r="AA43" t="n">
+        <v>5002</v>
+      </c>
+      <c r="AB43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>5182</t>
         </is>
       </c>
     </row>
@@ -4316,9 +4558,15 @@
       <c r="Z44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA44" t="inlineStr">
-        <is>
-          <t>4868</t>
+      <c r="AA44" t="n">
+        <v>4868</v>
+      </c>
+      <c r="AB44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>5019</t>
         </is>
       </c>
     </row>
@@ -4407,9 +4655,15 @@
       <c r="Z45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t>5010</t>
+      <c r="AA45" t="n">
+        <v>5010</v>
+      </c>
+      <c r="AB45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>5132</t>
         </is>
       </c>
     </row>
@@ -4498,9 +4752,15 @@
       <c r="Z46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>4861</t>
+      <c r="AA46" t="n">
+        <v>4861</v>
+      </c>
+      <c r="AB46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>4931</t>
         </is>
       </c>
     </row>
@@ -4589,9 +4849,15 @@
       <c r="Z47" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AA47" t="inlineStr">
-        <is>
-          <t>4580</t>
+      <c r="AA47" t="n">
+        <v>4580</v>
+      </c>
+      <c r="AB47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>4805</t>
         </is>
       </c>
     </row>
@@ -4680,9 +4946,15 @@
       <c r="Z48" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA48" t="inlineStr">
-        <is>
-          <t>5262</t>
+      <c r="AA48" t="n">
+        <v>5262</v>
+      </c>
+      <c r="AB48" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>5300</t>
         </is>
       </c>
     </row>
@@ -4771,9 +5043,15 @@
       <c r="Z49" s="4" t="n">
         <v>15</v>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>4327</t>
+      <c r="AA49" t="n">
+        <v>4327</v>
+      </c>
+      <c r="AB49" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>4394</t>
         </is>
       </c>
     </row>
@@ -4829,6 +5107,8 @@
       <c r="Y50" t="inlineStr"/>
       <c r="Z50" s="3" t="inlineStr"/>
       <c r="AA50" t="inlineStr"/>
+      <c r="AB50" s="3" t="inlineStr"/>
+      <c r="AC50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4915,9 +5195,15 @@
       <c r="Z51" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>4276</t>
+      <c r="AA51" t="n">
+        <v>4276</v>
+      </c>
+      <c r="AB51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>4312</t>
         </is>
       </c>
     </row>
@@ -5006,9 +5292,15 @@
       <c r="Z52" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA52" t="inlineStr">
-        <is>
-          <t>4310</t>
+      <c r="AA52" t="n">
+        <v>4310</v>
+      </c>
+      <c r="AB52" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>4344</t>
         </is>
       </c>
     </row>
@@ -5097,9 +5389,15 @@
       <c r="Z53" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA53" t="inlineStr">
-        <is>
-          <t>4302</t>
+      <c r="AA53" t="n">
+        <v>4302</v>
+      </c>
+      <c r="AB53" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>4473</t>
         </is>
       </c>
     </row>
@@ -5188,9 +5486,15 @@
       <c r="Z54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA54" t="inlineStr">
-        <is>
-          <t>4108</t>
+      <c r="AA54" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AB54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>4155</t>
         </is>
       </c>
     </row>
@@ -5279,9 +5583,15 @@
       <c r="Z55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AA55" t="inlineStr">
-        <is>
-          <t>4100</t>
+      <c r="AA55" t="n">
+        <v>4100</v>
+      </c>
+      <c r="AB55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -5370,9 +5680,15 @@
       <c r="Z56" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>4094</t>
+      <c r="AA56" t="n">
+        <v>4094</v>
+      </c>
+      <c r="AB56" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>4169</t>
         </is>
       </c>
     </row>
@@ -5461,9 +5777,15 @@
       <c r="Z57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>4368</t>
+      <c r="AA57" t="n">
+        <v>4368</v>
+      </c>
+      <c r="AB57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -5552,7 +5874,13 @@
       <c r="Z58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA58" t="inlineStr">
+      <c r="AA58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5643,9 +5971,15 @@
       <c r="Z59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA59" t="inlineStr">
-        <is>
-          <t>2851</t>
+      <c r="AA59" t="n">
+        <v>2851</v>
+      </c>
+      <c r="AB59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -5734,9 +6068,15 @@
       <c r="Z60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>2461</t>
+      <c r="AA60" t="n">
+        <v>2461</v>
+      </c>
+      <c r="AB60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>2460</t>
         </is>
       </c>
     </row>
@@ -5825,9 +6165,15 @@
       <c r="Z61" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA61" t="inlineStr">
-        <is>
-          <t>4024</t>
+      <c r="AA61" t="n">
+        <v>4024</v>
+      </c>
+      <c r="AB61" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>4354</t>
         </is>
       </c>
     </row>
@@ -5916,9 +6262,15 @@
       <c r="Z62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA62" t="inlineStr">
-        <is>
-          <t>1981</t>
+      <c r="AA62" t="n">
+        <v>1981</v>
+      </c>
+      <c r="AB62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>1975</t>
         </is>
       </c>
     </row>
@@ -5962,6 +6314,8 @@
       <c r="Y63" t="inlineStr"/>
       <c r="Z63" s="3" t="inlineStr"/>
       <c r="AA63" t="inlineStr"/>
+      <c r="AB63" s="3" t="inlineStr"/>
+      <c r="AC63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -6048,7 +6402,13 @@
       <c r="Z64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA64" t="inlineStr">
+      <c r="AA64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6114,6 +6474,8 @@
       <c r="Y65" t="inlineStr"/>
       <c r="Z65" s="3" t="inlineStr"/>
       <c r="AA65" t="inlineStr"/>
+      <c r="AB65" s="3" t="inlineStr"/>
+      <c r="AC65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6199,6 +6561,8 @@
       </c>
       <c r="Z66" s="3" t="inlineStr"/>
       <c r="AA66" t="inlineStr"/>
+      <c r="AB66" s="3" t="inlineStr"/>
+      <c r="AC66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -6285,9 +6649,15 @@
       <c r="Z67" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA67" t="inlineStr">
-        <is>
-          <t>5295</t>
+      <c r="AA67" t="n">
+        <v>5295</v>
+      </c>
+      <c r="AB67" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AC67" t="inlineStr">
+        <is>
+          <t>5448</t>
         </is>
       </c>
     </row>
@@ -6376,7 +6746,13 @@
       <c r="Z68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA68" t="inlineStr">
+      <c r="AA68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6467,9 +6843,15 @@
       <c r="Z69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="AA69" t="n">
+        <v>2660</v>
+      </c>
+      <c r="AB69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>2705</t>
         </is>
       </c>
     </row>
@@ -6558,7 +6940,13 @@
       <c r="Z70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA70" t="inlineStr">
+      <c r="AA70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6649,9 +7037,15 @@
       <c r="Z71" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA71" t="inlineStr">
-        <is>
-          <t>4347</t>
+      <c r="AA71" t="n">
+        <v>4347</v>
+      </c>
+      <c r="AB71" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC71" t="inlineStr">
+        <is>
+          <t>4537</t>
         </is>
       </c>
     </row>
@@ -6740,9 +7134,15 @@
       <c r="Z72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA72" t="inlineStr">
-        <is>
-          <t>3271</t>
+      <c r="AA72" t="n">
+        <v>3271</v>
+      </c>
+      <c r="AB72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -6831,7 +7231,13 @@
       <c r="Z73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA73" t="inlineStr">
+      <c r="AA73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6922,9 +7328,15 @@
       <c r="Z74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA74" t="inlineStr">
-        <is>
-          <t>1229</t>
+      <c r="AA74" t="n">
+        <v>1229</v>
+      </c>
+      <c r="AB74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>1227</t>
         </is>
       </c>
     </row>
@@ -6984,6 +7396,8 @@
       <c r="Y75" t="inlineStr"/>
       <c r="Z75" s="3" t="inlineStr"/>
       <c r="AA75" t="inlineStr"/>
+      <c r="AB75" s="3" t="inlineStr"/>
+      <c r="AC75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -7070,7 +7484,13 @@
       <c r="Z76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA76" t="inlineStr">
+      <c r="AA76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7161,9 +7581,15 @@
       <c r="Z77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA77" t="inlineStr">
-        <is>
-          <t>3043</t>
+      <c r="AA77" t="n">
+        <v>3043</v>
+      </c>
+      <c r="AB77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -7252,7 +7678,13 @@
       <c r="Z78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA78" t="inlineStr">
+      <c r="AA78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7343,7 +7775,13 @@
       <c r="Z79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA79" t="inlineStr">
+      <c r="AA79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7434,9 +7872,15 @@
       <c r="Z80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA80" t="inlineStr">
-        <is>
-          <t>1489</t>
+      <c r="AA80" t="n">
+        <v>1489</v>
+      </c>
+      <c r="AB80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>1486</t>
         </is>
       </c>
     </row>
@@ -7525,7 +7969,13 @@
       <c r="Z81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA81" t="inlineStr">
+      <c r="AA81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7616,7 +8066,13 @@
       <c r="Z82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA82" t="inlineStr">
+      <c r="AA82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7707,7 +8163,13 @@
       <c r="Z83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA83" t="inlineStr">
+      <c r="AA83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7798,7 +8260,13 @@
       <c r="Z84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA84" t="inlineStr">
+      <c r="AA84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7889,7 +8357,13 @@
       <c r="Z85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA85" t="inlineStr">
+      <c r="AA85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7980,7 +8454,13 @@
       <c r="Z86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA86" t="inlineStr">
+      <c r="AA86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8071,7 +8551,13 @@
       <c r="Z87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA87" t="inlineStr">
+      <c r="AA87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8162,9 +8648,15 @@
       <c r="Z88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA88" t="inlineStr">
-        <is>
-          <t>2746</t>
+      <c r="AA88" t="n">
+        <v>2746</v>
+      </c>
+      <c r="AB88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC88" t="inlineStr">
+        <is>
+          <t>2738</t>
         </is>
       </c>
     </row>
@@ -8253,7 +8745,13 @@
       <c r="Z89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA89" t="inlineStr">
+      <c r="AA89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8344,7 +8842,13 @@
       <c r="Z90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA90" t="inlineStr">
+      <c r="AA90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8418,6 +8922,8 @@
       <c r="Y91" t="inlineStr"/>
       <c r="Z91" s="3" t="inlineStr"/>
       <c r="AA91" t="inlineStr"/>
+      <c r="AB91" s="3" t="inlineStr"/>
+      <c r="AC91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -8504,7 +9010,13 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
+      <c r="AA92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8595,9 +9107,15 @@
       <c r="Z93" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AA93" t="inlineStr">
-        <is>
-          <t>3753</t>
+      <c r="AA93" t="n">
+        <v>3753</v>
+      </c>
+      <c r="AB93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC93" t="inlineStr">
+        <is>
+          <t>3736</t>
         </is>
       </c>
     </row>
@@ -8686,7 +9204,13 @@
       <c r="Z94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA94" t="inlineStr">
+      <c r="AA94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8777,7 +9301,13 @@
       <c r="Z95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA95" t="inlineStr">
+      <c r="AA95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8868,7 +9398,13 @@
       <c r="Z96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA96" t="inlineStr">
+      <c r="AA96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8959,7 +9495,13 @@
       <c r="Z97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA97" t="inlineStr">
+      <c r="AA97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9050,7 +9592,13 @@
       <c r="Z98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA98" t="inlineStr">
+      <c r="AA98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9141,7 +9689,13 @@
       <c r="Z99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA99" t="inlineStr">
+      <c r="AA99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9232,7 +9786,13 @@
       <c r="Z100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA100" t="inlineStr">
+      <c r="AA100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9323,7 +9883,13 @@
       <c r="Z101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA101" t="inlineStr">
+      <c r="AA101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9414,7 +9980,13 @@
       <c r="Z102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA102" t="inlineStr">
+      <c r="AA102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9488,6 +10060,8 @@
       <c r="Y103" t="inlineStr"/>
       <c r="Z103" s="3" t="inlineStr"/>
       <c r="AA103" t="inlineStr"/>
+      <c r="AB103" s="3" t="inlineStr"/>
+      <c r="AC103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -9557,6 +10131,8 @@
       <c r="Y104" t="inlineStr"/>
       <c r="Z104" s="3" t="inlineStr"/>
       <c r="AA104" t="inlineStr"/>
+      <c r="AB104" s="3" t="inlineStr"/>
+      <c r="AC104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -9626,6 +10202,8 @@
       <c r="Y105" t="inlineStr"/>
       <c r="Z105" s="3" t="inlineStr"/>
       <c r="AA105" t="inlineStr"/>
+      <c r="AB105" s="3" t="inlineStr"/>
+      <c r="AC105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -9695,6 +10273,8 @@
       <c r="Y106" t="inlineStr"/>
       <c r="Z106" s="3" t="inlineStr"/>
       <c r="AA106" t="inlineStr"/>
+      <c r="AB106" s="3" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9764,6 +10344,8 @@
       <c r="Y107" t="inlineStr"/>
       <c r="Z107" s="3" t="inlineStr"/>
       <c r="AA107" t="inlineStr"/>
+      <c r="AB107" s="3" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9833,6 +10415,8 @@
       <c r="Y108" t="inlineStr"/>
       <c r="Z108" s="3" t="inlineStr"/>
       <c r="AA108" t="inlineStr"/>
+      <c r="AB108" s="3" t="inlineStr"/>
+      <c r="AC108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9902,6 +10486,8 @@
       <c r="Y109" t="inlineStr"/>
       <c r="Z109" s="3" t="inlineStr"/>
       <c r="AA109" t="inlineStr"/>
+      <c r="AB109" s="3" t="inlineStr"/>
+      <c r="AC109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9971,6 +10557,8 @@
       <c r="Y110" t="inlineStr"/>
       <c r="Z110" s="3" t="inlineStr"/>
       <c r="AA110" t="inlineStr"/>
+      <c r="AB110" s="3" t="inlineStr"/>
+      <c r="AC110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10040,6 +10628,8 @@
       <c r="Y111" t="inlineStr"/>
       <c r="Z111" s="3" t="inlineStr"/>
       <c r="AA111" t="inlineStr"/>
+      <c r="AB111" s="3" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10116,7 +10706,13 @@
       <c r="Z112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA112" t="inlineStr">
+      <c r="AA112" t="n">
+        <v>4364</v>
+      </c>
+      <c r="AB112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC112" t="inlineStr">
         <is>
           <t>4364</t>
         </is>
@@ -10197,9 +10793,15 @@
       <c r="Z113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA113" t="inlineStr">
-        <is>
-          <t>2898</t>
+      <c r="AA113" t="n">
+        <v>2898</v>
+      </c>
+      <c r="AB113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC113" t="inlineStr">
+        <is>
+          <t>2925</t>
         </is>
       </c>
     </row>
@@ -10274,9 +10876,15 @@
       <c r="Z114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA114" t="inlineStr">
-        <is>
-          <t>1587</t>
+      <c r="AA114" t="n">
+        <v>1587</v>
+      </c>
+      <c r="AB114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC114" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10351,9 +10959,15 @@
       <c r="Z115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>5209</t>
+      <c r="AA115" t="n">
+        <v>5209</v>
+      </c>
+      <c r="AB115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>5483</t>
         </is>
       </c>
     </row>
@@ -10428,9 +11042,15 @@
       <c r="Z116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AA116" t="inlineStr">
-        <is>
-          <t>3704</t>
+      <c r="AA116" t="n">
+        <v>3704</v>
+      </c>
+      <c r="AB116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC116" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -10476,6 +11096,8 @@
       <c r="Y117" t="inlineStr"/>
       <c r="Z117" s="3" t="inlineStr"/>
       <c r="AA117" t="inlineStr"/>
+      <c r="AB117" s="3" t="inlineStr"/>
+      <c r="AC117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -10540,9 +11162,15 @@
       <c r="Z118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA118" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="AA118" t="n">
+        <v>2815</v>
+      </c>
+      <c r="AB118" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC118" t="inlineStr">
+        <is>
+          <t>2883</t>
         </is>
       </c>
     </row>
@@ -10588,6 +11216,8 @@
       <c r="Y119" t="inlineStr"/>
       <c r="Z119" s="3" t="inlineStr"/>
       <c r="AA119" t="inlineStr"/>
+      <c r="AB119" s="3" t="inlineStr"/>
+      <c r="AC119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -10648,9 +11278,15 @@
       <c r="Z120" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AA120" t="inlineStr">
-        <is>
-          <t>1477</t>
+      <c r="AA120" t="n">
+        <v>1477</v>
+      </c>
+      <c r="AB120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" t="inlineStr">
+        <is>
+          <t>1476</t>
         </is>
       </c>
     </row>
@@ -10713,7 +11349,13 @@
       <c r="Z121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA121" t="inlineStr">
+      <c r="AA121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10774,9 +11416,15 @@
       <c r="Z122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA122" t="inlineStr">
-        <is>
-          <t>2723</t>
+      <c r="AA122" t="n">
+        <v>2723</v>
+      </c>
+      <c r="AB122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC122" t="inlineStr">
+        <is>
+          <t>2788</t>
         </is>
       </c>
     </row>
@@ -10835,9 +11483,15 @@
       <c r="Z123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA123" t="inlineStr">
-        <is>
-          <t>2576</t>
+      <c r="AA123" t="n">
+        <v>2576</v>
+      </c>
+      <c r="AB123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC123" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -10892,9 +11546,15 @@
       <c r="Z124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA124" t="inlineStr">
-        <is>
-          <t>1445</t>
+      <c r="AA124" t="n">
+        <v>1445</v>
+      </c>
+      <c r="AB124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC124" t="inlineStr">
+        <is>
+          <t>1444</t>
         </is>
       </c>
     </row>
@@ -10945,7 +11605,13 @@
       <c r="Z125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA125" t="inlineStr">
+      <c r="AA125" t="n">
+        <v>2584</v>
+      </c>
+      <c r="AB125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC125" t="inlineStr">
         <is>
           <t>2584</t>
         </is>
@@ -10998,9 +11664,15 @@
       <c r="Z126" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="AA126" t="inlineStr">
-        <is>
-          <t>1674</t>
+      <c r="AA126" t="n">
+        <v>1674</v>
+      </c>
+      <c r="AB126" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC126" t="inlineStr">
+        <is>
+          <t>1699</t>
         </is>
       </c>
     </row>
@@ -11051,9 +11723,15 @@
       <c r="Z127" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AA127" t="inlineStr">
-        <is>
-          <t>1537</t>
+      <c r="AA127" t="n">
+        <v>1537</v>
+      </c>
+      <c r="AB127" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC127" t="inlineStr">
+        <is>
+          <t>1548</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-22 07:26:19
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC127"/>
+  <dimension ref="A1:AE127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,6 +534,16 @@
       <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>04-20_0</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>04-21_A</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>04-21_0</t>
         </is>
       </c>
     </row>
@@ -591,6 +601,8 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" s="3" t="inlineStr"/>
       <c r="AC2" t="inlineStr"/>
+      <c r="AD2" s="3" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -683,7 +695,13 @@
       <c r="AB3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AC3" t="n">
+        <v>2551</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="inlineStr">
         <is>
           <t>2551</t>
         </is>
@@ -780,7 +798,13 @@
       <c r="AB4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC4" t="inlineStr">
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -877,7 +901,13 @@
       <c r="AB5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC5" t="inlineStr">
+      <c r="AC5" t="n">
+        <v>4393</v>
+      </c>
+      <c r="AD5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="inlineStr">
         <is>
           <t>4393</t>
         </is>
@@ -974,7 +1004,13 @@
       <c r="AB6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC6" t="inlineStr">
+      <c r="AC6" t="n">
+        <v>2536</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="inlineStr">
         <is>
           <t>2536</t>
         </is>
@@ -1071,7 +1107,13 @@
       <c r="AB7" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC7" t="inlineStr">
+      <c r="AC7" t="n">
+        <v>5616</v>
+      </c>
+      <c r="AD7" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE7" t="inlineStr">
         <is>
           <t>5616</t>
         </is>
@@ -1131,6 +1173,8 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" s="3" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
+      <c r="AD8" s="3" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1223,7 +1267,13 @@
       <c r="AB9" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="AC9" t="inlineStr">
+      <c r="AC9" t="n">
+        <v>3747</v>
+      </c>
+      <c r="AD9" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE9" t="inlineStr">
         <is>
           <t>3747</t>
         </is>
@@ -1320,7 +1370,13 @@
       <c r="AB10" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC10" t="inlineStr">
+      <c r="AC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE10" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1417,7 +1473,13 @@
       <c r="AB11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC11" t="inlineStr">
+      <c r="AC11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1514,7 +1576,13 @@
       <c r="AB12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC12" t="inlineStr">
+      <c r="AC12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1611,7 +1679,13 @@
       <c r="AB13" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="AC13" t="inlineStr">
+      <c r="AC13" t="n">
+        <v>4104</v>
+      </c>
+      <c r="AD13" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AE13" t="inlineStr">
         <is>
           <t>4104</t>
         </is>
@@ -1708,7 +1782,13 @@
       <c r="AB14" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="AC14" t="inlineStr">
+      <c r="AC14" t="n">
+        <v>2812</v>
+      </c>
+      <c r="AD14" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE14" t="inlineStr">
         <is>
           <t>2812</t>
         </is>
@@ -1805,7 +1885,13 @@
       <c r="AB15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC15" t="inlineStr">
+      <c r="AC15" t="n">
+        <v>4425</v>
+      </c>
+      <c r="AD15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE15" t="inlineStr">
         <is>
           <t>4425</t>
         </is>
@@ -1889,6 +1975,8 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" s="3" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
+      <c r="AD16" s="3" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1981,7 +2069,13 @@
       <c r="AB17" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC17" t="inlineStr">
+      <c r="AC17" t="n">
+        <v>5228</v>
+      </c>
+      <c r="AD17" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE17" t="inlineStr">
         <is>
           <t>5228</t>
         </is>
@@ -2078,7 +2172,13 @@
       <c r="AB18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC18" t="inlineStr">
+      <c r="AC18" t="n">
+        <v>5195</v>
+      </c>
+      <c r="AD18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE18" t="inlineStr">
         <is>
           <t>5195</t>
         </is>
@@ -2175,7 +2275,13 @@
       <c r="AB19" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC19" t="inlineStr">
+      <c r="AC19" t="n">
+        <v>6064</v>
+      </c>
+      <c r="AD19" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE19" t="inlineStr">
         <is>
           <t>6064</t>
         </is>
@@ -2272,7 +2378,13 @@
       <c r="AB20" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC20" t="inlineStr">
+      <c r="AC20" t="n">
+        <v>5284</v>
+      </c>
+      <c r="AD20" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE20" t="inlineStr">
         <is>
           <t>5284</t>
         </is>
@@ -2369,7 +2481,13 @@
       <c r="AB21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC21" t="inlineStr">
+      <c r="AC21" t="n">
+        <v>5860</v>
+      </c>
+      <c r="AD21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE21" t="inlineStr">
         <is>
           <t>5860</t>
         </is>
@@ -2466,7 +2584,13 @@
       <c r="AB22" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="AC22" t="inlineStr">
+      <c r="AC22" t="n">
+        <v>4118</v>
+      </c>
+      <c r="AD22" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE22" t="inlineStr">
         <is>
           <t>4118</t>
         </is>
@@ -2563,7 +2687,13 @@
       <c r="AB23" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC23" t="inlineStr">
+      <c r="AC23" t="n">
+        <v>4909</v>
+      </c>
+      <c r="AD23" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE23" t="inlineStr">
         <is>
           <t>4909</t>
         </is>
@@ -2660,7 +2790,13 @@
       <c r="AB24" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC24" t="inlineStr">
+      <c r="AC24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE24" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2744,6 +2880,8 @@
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" s="3" t="inlineStr"/>
       <c r="AC25" t="inlineStr"/>
+      <c r="AD25" s="3" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2836,7 +2974,13 @@
       <c r="AB26" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC26" t="inlineStr">
+      <c r="AC26" t="n">
+        <v>5241</v>
+      </c>
+      <c r="AD26" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE26" t="inlineStr">
         <is>
           <t>5241</t>
         </is>
@@ -2933,7 +3077,13 @@
       <c r="AB27" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC27" t="inlineStr">
+      <c r="AC27" t="n">
+        <v>4329</v>
+      </c>
+      <c r="AD27" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE27" t="inlineStr">
         <is>
           <t>4329</t>
         </is>
@@ -3030,7 +3180,13 @@
       <c r="AB28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC28" t="inlineStr">
+      <c r="AC28" t="n">
+        <v>2601</v>
+      </c>
+      <c r="AD28" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE28" t="inlineStr">
         <is>
           <t>2601</t>
         </is>
@@ -3127,7 +3283,13 @@
       <c r="AB29" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC29" t="inlineStr">
+      <c r="AC29" t="n">
+        <v>5072</v>
+      </c>
+      <c r="AD29" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE29" t="inlineStr">
         <is>
           <t>5072</t>
         </is>
@@ -3224,7 +3386,13 @@
       <c r="AB30" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC30" t="inlineStr">
+      <c r="AC30" t="n">
+        <v>3924</v>
+      </c>
+      <c r="AD30" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE30" t="inlineStr">
         <is>
           <t>3924</t>
         </is>
@@ -3321,7 +3489,13 @@
       <c r="AB31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC31" t="inlineStr">
+      <c r="AC31" t="n">
+        <v>4930</v>
+      </c>
+      <c r="AD31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE31" t="inlineStr">
         <is>
           <t>4930</t>
         </is>
@@ -3418,7 +3592,13 @@
       <c r="AB32" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="AC32" t="inlineStr">
+      <c r="AC32" t="n">
+        <v>4652</v>
+      </c>
+      <c r="AD32" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE32" t="inlineStr">
         <is>
           <t>4652</t>
         </is>
@@ -3502,6 +3682,8 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" s="3" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
+      <c r="AD33" s="3" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3594,7 +3776,13 @@
       <c r="AB34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC34" t="inlineStr">
+      <c r="AC34" t="n">
+        <v>2712</v>
+      </c>
+      <c r="AD34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="inlineStr">
         <is>
           <t>2712</t>
         </is>
@@ -3691,7 +3879,13 @@
       <c r="AB35" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="AC35" t="inlineStr">
+      <c r="AC35" t="n">
+        <v>4549</v>
+      </c>
+      <c r="AD35" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AE35" t="inlineStr">
         <is>
           <t>4549</t>
         </is>
@@ -3788,7 +3982,13 @@
       <c r="AB36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC36" t="inlineStr">
+      <c r="AC36" t="n">
+        <v>3420</v>
+      </c>
+      <c r="AD36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE36" t="inlineStr">
         <is>
           <t>3420</t>
         </is>
@@ -3885,7 +4085,13 @@
       <c r="AB37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC37" t="inlineStr">
+      <c r="AC37" t="n">
+        <v>5656</v>
+      </c>
+      <c r="AD37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE37" t="inlineStr">
         <is>
           <t>5656</t>
         </is>
@@ -3982,7 +4188,13 @@
       <c r="AB38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC38" t="inlineStr">
+      <c r="AC38" t="n">
+        <v>4081</v>
+      </c>
+      <c r="AD38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE38" t="inlineStr">
         <is>
           <t>4081</t>
         </is>
@@ -4079,7 +4291,13 @@
       <c r="AB39" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AC39" t="inlineStr">
+      <c r="AC39" t="n">
+        <v>3886</v>
+      </c>
+      <c r="AD39" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE39" t="inlineStr">
         <is>
           <t>3886</t>
         </is>
@@ -4176,7 +4394,13 @@
       <c r="AB40" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AC40" t="inlineStr">
+      <c r="AC40" t="n">
+        <v>5704</v>
+      </c>
+      <c r="AD40" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE40" t="inlineStr">
         <is>
           <t>5704</t>
         </is>
@@ -4273,7 +4497,13 @@
       <c r="AB41" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC41" t="inlineStr">
+      <c r="AC41" t="n">
+        <v>5463</v>
+      </c>
+      <c r="AD41" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE41" t="inlineStr">
         <is>
           <t>5463</t>
         </is>
@@ -4370,7 +4600,13 @@
       <c r="AB42" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC42" t="inlineStr">
+      <c r="AC42" t="n">
+        <v>4996</v>
+      </c>
+      <c r="AD42" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE42" t="inlineStr">
         <is>
           <t>4996</t>
         </is>
@@ -4467,7 +4703,13 @@
       <c r="AB43" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC43" t="inlineStr">
+      <c r="AC43" t="n">
+        <v>5182</v>
+      </c>
+      <c r="AD43" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE43" t="inlineStr">
         <is>
           <t>5182</t>
         </is>
@@ -4564,7 +4806,13 @@
       <c r="AB44" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC44" t="inlineStr">
+      <c r="AC44" t="n">
+        <v>5019</v>
+      </c>
+      <c r="AD44" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE44" t="inlineStr">
         <is>
           <t>5019</t>
         </is>
@@ -4661,7 +4909,13 @@
       <c r="AB45" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC45" t="inlineStr">
+      <c r="AC45" t="n">
+        <v>5132</v>
+      </c>
+      <c r="AD45" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE45" t="inlineStr">
         <is>
           <t>5132</t>
         </is>
@@ -4758,7 +5012,13 @@
       <c r="AB46" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC46" t="inlineStr">
+      <c r="AC46" t="n">
+        <v>4931</v>
+      </c>
+      <c r="AD46" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE46" t="inlineStr">
         <is>
           <t>4931</t>
         </is>
@@ -4855,7 +5115,13 @@
       <c r="AB47" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC47" t="inlineStr">
+      <c r="AC47" t="n">
+        <v>4805</v>
+      </c>
+      <c r="AD47" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE47" t="inlineStr">
         <is>
           <t>4805</t>
         </is>
@@ -4952,7 +5218,13 @@
       <c r="AB48" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC48" t="inlineStr">
+      <c r="AC48" t="n">
+        <v>5300</v>
+      </c>
+      <c r="AD48" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE48" t="inlineStr">
         <is>
           <t>5300</t>
         </is>
@@ -5049,7 +5321,13 @@
       <c r="AB49" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AC49" t="inlineStr">
+      <c r="AC49" t="n">
+        <v>4394</v>
+      </c>
+      <c r="AD49" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE49" t="inlineStr">
         <is>
           <t>4394</t>
         </is>
@@ -5109,6 +5387,8 @@
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" s="3" t="inlineStr"/>
       <c r="AC50" t="inlineStr"/>
+      <c r="AD50" s="3" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -5201,7 +5481,13 @@
       <c r="AB51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC51" t="inlineStr">
+      <c r="AC51" t="n">
+        <v>4312</v>
+      </c>
+      <c r="AD51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE51" t="inlineStr">
         <is>
           <t>4312</t>
         </is>
@@ -5298,7 +5584,13 @@
       <c r="AB52" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC52" t="inlineStr">
+      <c r="AC52" t="n">
+        <v>4344</v>
+      </c>
+      <c r="AD52" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE52" t="inlineStr">
         <is>
           <t>4344</t>
         </is>
@@ -5395,7 +5687,13 @@
       <c r="AB53" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="AC53" t="inlineStr">
+      <c r="AC53" t="n">
+        <v>4473</v>
+      </c>
+      <c r="AD53" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE53" t="inlineStr">
         <is>
           <t>4473</t>
         </is>
@@ -5492,7 +5790,13 @@
       <c r="AB54" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC54" t="inlineStr">
+      <c r="AC54" t="n">
+        <v>4155</v>
+      </c>
+      <c r="AD54" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE54" t="inlineStr">
         <is>
           <t>4155</t>
         </is>
@@ -5589,7 +5893,13 @@
       <c r="AB55" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="AC55" t="inlineStr">
+      <c r="AC55" t="n">
+        <v>4149</v>
+      </c>
+      <c r="AD55" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE55" t="inlineStr">
         <is>
           <t>4149</t>
         </is>
@@ -5686,7 +5996,13 @@
       <c r="AB56" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="AC56" t="inlineStr">
+      <c r="AC56" t="n">
+        <v>4169</v>
+      </c>
+      <c r="AD56" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AE56" t="inlineStr">
         <is>
           <t>4169</t>
         </is>
@@ -5783,7 +6099,13 @@
       <c r="AB57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="AC57" t="inlineStr">
+      <c r="AC57" t="n">
+        <v>4397</v>
+      </c>
+      <c r="AD57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE57" t="inlineStr">
         <is>
           <t>4397</t>
         </is>
@@ -5880,7 +6202,13 @@
       <c r="AB58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC58" t="inlineStr">
+      <c r="AC58" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE58" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5977,7 +6305,13 @@
       <c r="AB59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC59" t="inlineStr">
+      <c r="AC59" t="n">
+        <v>2887</v>
+      </c>
+      <c r="AD59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE59" t="inlineStr">
         <is>
           <t>2887</t>
         </is>
@@ -6074,7 +6408,13 @@
       <c r="AB60" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC60" t="inlineStr">
+      <c r="AC60" t="n">
+        <v>2460</v>
+      </c>
+      <c r="AD60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE60" t="inlineStr">
         <is>
           <t>2460</t>
         </is>
@@ -6171,7 +6511,13 @@
       <c r="AB61" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="AC61" t="inlineStr">
+      <c r="AC61" t="n">
+        <v>4354</v>
+      </c>
+      <c r="AD61" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE61" t="inlineStr">
         <is>
           <t>4354</t>
         </is>
@@ -6268,7 +6614,13 @@
       <c r="AB62" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC62" t="inlineStr">
+      <c r="AC62" t="n">
+        <v>1975</v>
+      </c>
+      <c r="AD62" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE62" t="inlineStr">
         <is>
           <t>1975</t>
         </is>
@@ -6316,6 +6668,8 @@
       <c r="AA63" t="inlineStr"/>
       <c r="AB63" s="3" t="inlineStr"/>
       <c r="AC63" t="inlineStr"/>
+      <c r="AD63" s="3" t="inlineStr"/>
+      <c r="AE63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -6408,7 +6762,13 @@
       <c r="AB64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC64" t="inlineStr">
+      <c r="AC64" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE64" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6476,6 +6836,8 @@
       <c r="AA65" t="inlineStr"/>
       <c r="AB65" s="3" t="inlineStr"/>
       <c r="AC65" t="inlineStr"/>
+      <c r="AD65" s="3" t="inlineStr"/>
+      <c r="AE65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6563,6 +6925,8 @@
       <c r="AA66" t="inlineStr"/>
       <c r="AB66" s="3" t="inlineStr"/>
       <c r="AC66" t="inlineStr"/>
+      <c r="AD66" s="3" t="inlineStr"/>
+      <c r="AE66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -6655,7 +7019,13 @@
       <c r="AB67" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AC67" t="inlineStr">
+      <c r="AC67" t="n">
+        <v>5448</v>
+      </c>
+      <c r="AD67" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AE67" t="inlineStr">
         <is>
           <t>5448</t>
         </is>
@@ -6752,7 +7122,13 @@
       <c r="AB68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC68" t="inlineStr">
+      <c r="AC68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6849,7 +7225,13 @@
       <c r="AB69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC69" t="inlineStr">
+      <c r="AC69" t="n">
+        <v>2705</v>
+      </c>
+      <c r="AD69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE69" t="inlineStr">
         <is>
           <t>2705</t>
         </is>
@@ -6946,7 +7328,13 @@
       <c r="AB70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC70" t="inlineStr">
+      <c r="AC70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7043,7 +7431,13 @@
       <c r="AB71" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AC71" t="inlineStr">
+      <c r="AC71" t="n">
+        <v>4537</v>
+      </c>
+      <c r="AD71" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE71" t="inlineStr">
         <is>
           <t>4537</t>
         </is>
@@ -7140,7 +7534,13 @@
       <c r="AB72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC72" t="inlineStr">
+      <c r="AC72" t="n">
+        <v>3316</v>
+      </c>
+      <c r="AD72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE72" t="inlineStr">
         <is>
           <t>3316</t>
         </is>
@@ -7237,7 +7637,13 @@
       <c r="AB73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC73" t="inlineStr">
+      <c r="AC73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE73" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7334,7 +7740,13 @@
       <c r="AB74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC74" t="inlineStr">
+      <c r="AC74" t="n">
+        <v>1227</v>
+      </c>
+      <c r="AD74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE74" t="inlineStr">
         <is>
           <t>1227</t>
         </is>
@@ -7398,6 +7810,8 @@
       <c r="AA75" t="inlineStr"/>
       <c r="AB75" s="3" t="inlineStr"/>
       <c r="AC75" t="inlineStr"/>
+      <c r="AD75" s="3" t="inlineStr"/>
+      <c r="AE75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -7490,7 +7904,13 @@
       <c r="AB76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC76" t="inlineStr">
+      <c r="AC76" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE76" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7587,7 +8007,13 @@
       <c r="AB77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC77" t="inlineStr">
+      <c r="AC77" t="n">
+        <v>3067</v>
+      </c>
+      <c r="AD77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE77" t="inlineStr">
         <is>
           <t>3067</t>
         </is>
@@ -7684,7 +8110,13 @@
       <c r="AB78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC78" t="inlineStr">
+      <c r="AC78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7781,7 +8213,13 @@
       <c r="AB79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC79" t="inlineStr">
+      <c r="AC79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7878,7 +8316,13 @@
       <c r="AB80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC80" t="inlineStr">
+      <c r="AC80" t="n">
+        <v>1486</v>
+      </c>
+      <c r="AD80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE80" t="inlineStr">
         <is>
           <t>1486</t>
         </is>
@@ -7975,7 +8419,13 @@
       <c r="AB81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC81" t="inlineStr">
+      <c r="AC81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8072,7 +8522,13 @@
       <c r="AB82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC82" t="inlineStr">
+      <c r="AC82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8169,7 +8625,13 @@
       <c r="AB83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC83" t="inlineStr">
+      <c r="AC83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8266,7 +8728,13 @@
       <c r="AB84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC84" t="inlineStr">
+      <c r="AC84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8363,7 +8831,13 @@
       <c r="AB85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC85" t="inlineStr">
+      <c r="AC85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8460,7 +8934,13 @@
       <c r="AB86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC86" t="inlineStr">
+      <c r="AC86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8557,7 +9037,13 @@
       <c r="AB87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC87" t="inlineStr">
+      <c r="AC87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8654,7 +9140,13 @@
       <c r="AB88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC88" t="inlineStr">
+      <c r="AC88" t="n">
+        <v>2738</v>
+      </c>
+      <c r="AD88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE88" t="inlineStr">
         <is>
           <t>2738</t>
         </is>
@@ -8751,7 +9243,13 @@
       <c r="AB89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC89" t="inlineStr">
+      <c r="AC89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8848,7 +9346,13 @@
       <c r="AB90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC90" t="inlineStr">
+      <c r="AC90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8924,6 +9428,8 @@
       <c r="AA91" t="inlineStr"/>
       <c r="AB91" s="3" t="inlineStr"/>
       <c r="AC91" t="inlineStr"/>
+      <c r="AD91" s="3" t="inlineStr"/>
+      <c r="AE91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -9016,7 +9522,13 @@
       <c r="AB92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC92" t="inlineStr">
+      <c r="AC92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9113,7 +9625,13 @@
       <c r="AB93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC93" t="inlineStr">
+      <c r="AC93" t="n">
+        <v>3736</v>
+      </c>
+      <c r="AD93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE93" t="inlineStr">
         <is>
           <t>3736</t>
         </is>
@@ -9210,7 +9728,13 @@
       <c r="AB94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC94" t="inlineStr">
+      <c r="AC94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9307,7 +9831,13 @@
       <c r="AB95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC95" t="inlineStr">
+      <c r="AC95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9404,7 +9934,13 @@
       <c r="AB96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC96" t="inlineStr">
+      <c r="AC96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9501,7 +10037,13 @@
       <c r="AB97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC97" t="inlineStr">
+      <c r="AC97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9598,7 +10140,13 @@
       <c r="AB98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC98" t="inlineStr">
+      <c r="AC98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9695,7 +10243,13 @@
       <c r="AB99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC99" t="inlineStr">
+      <c r="AC99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9792,7 +10346,13 @@
       <c r="AB100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC100" t="inlineStr">
+      <c r="AC100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9889,7 +10449,13 @@
       <c r="AB101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC101" t="inlineStr">
+      <c r="AC101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9986,7 +10552,13 @@
       <c r="AB102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC102" t="inlineStr">
+      <c r="AC102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10062,6 +10634,8 @@
       <c r="AA103" t="inlineStr"/>
       <c r="AB103" s="3" t="inlineStr"/>
       <c r="AC103" t="inlineStr"/>
+      <c r="AD103" s="3" t="inlineStr"/>
+      <c r="AE103" t="inlineStr"/>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -10133,6 +10707,8 @@
       <c r="AA104" t="inlineStr"/>
       <c r="AB104" s="3" t="inlineStr"/>
       <c r="AC104" t="inlineStr"/>
+      <c r="AD104" s="3" t="inlineStr"/>
+      <c r="AE104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -10204,6 +10780,8 @@
       <c r="AA105" t="inlineStr"/>
       <c r="AB105" s="3" t="inlineStr"/>
       <c r="AC105" t="inlineStr"/>
+      <c r="AD105" s="3" t="inlineStr"/>
+      <c r="AE105" t="inlineStr"/>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -10275,6 +10853,8 @@
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" s="3" t="inlineStr"/>
       <c r="AC106" t="inlineStr"/>
+      <c r="AD106" s="3" t="inlineStr"/>
+      <c r="AE106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -10346,6 +10926,8 @@
       <c r="AA107" t="inlineStr"/>
       <c r="AB107" s="3" t="inlineStr"/>
       <c r="AC107" t="inlineStr"/>
+      <c r="AD107" s="3" t="inlineStr"/>
+      <c r="AE107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -10417,6 +10999,8 @@
       <c r="AA108" t="inlineStr"/>
       <c r="AB108" s="3" t="inlineStr"/>
       <c r="AC108" t="inlineStr"/>
+      <c r="AD108" s="3" t="inlineStr"/>
+      <c r="AE108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -10488,6 +11072,8 @@
       <c r="AA109" t="inlineStr"/>
       <c r="AB109" s="3" t="inlineStr"/>
       <c r="AC109" t="inlineStr"/>
+      <c r="AD109" s="3" t="inlineStr"/>
+      <c r="AE109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -10559,6 +11145,8 @@
       <c r="AA110" t="inlineStr"/>
       <c r="AB110" s="3" t="inlineStr"/>
       <c r="AC110" t="inlineStr"/>
+      <c r="AD110" s="3" t="inlineStr"/>
+      <c r="AE110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10630,6 +11218,8 @@
       <c r="AA111" t="inlineStr"/>
       <c r="AB111" s="3" t="inlineStr"/>
       <c r="AC111" t="inlineStr"/>
+      <c r="AD111" s="3" t="inlineStr"/>
+      <c r="AE111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10712,7 +11302,13 @@
       <c r="AB112" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC112" t="inlineStr">
+      <c r="AC112" t="n">
+        <v>4364</v>
+      </c>
+      <c r="AD112" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE112" t="inlineStr">
         <is>
           <t>4364</t>
         </is>
@@ -10799,7 +11395,13 @@
       <c r="AB113" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC113" t="inlineStr">
+      <c r="AC113" t="n">
+        <v>2925</v>
+      </c>
+      <c r="AD113" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE113" t="inlineStr">
         <is>
           <t>2925</t>
         </is>
@@ -10882,7 +11484,13 @@
       <c r="AB114" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC114" t="inlineStr">
+      <c r="AC114" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE114" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10965,7 +11573,13 @@
       <c r="AB115" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC115" t="inlineStr">
+      <c r="AC115" t="n">
+        <v>5483</v>
+      </c>
+      <c r="AD115" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE115" t="inlineStr">
         <is>
           <t>5483</t>
         </is>
@@ -11048,7 +11662,13 @@
       <c r="AB116" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="AC116" t="inlineStr">
+      <c r="AC116" t="n">
+        <v>3816</v>
+      </c>
+      <c r="AD116" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE116" t="inlineStr">
         <is>
           <t>3816</t>
         </is>
@@ -11098,6 +11718,8 @@
       <c r="AA117" t="inlineStr"/>
       <c r="AB117" s="3" t="inlineStr"/>
       <c r="AC117" t="inlineStr"/>
+      <c r="AD117" s="3" t="inlineStr"/>
+      <c r="AE117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -11168,7 +11790,13 @@
       <c r="AB118" s="4" t="n">
         <v>16</v>
       </c>
-      <c r="AC118" t="inlineStr">
+      <c r="AC118" t="n">
+        <v>2883</v>
+      </c>
+      <c r="AD118" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE118" t="inlineStr">
         <is>
           <t>2883</t>
         </is>
@@ -11218,6 +11846,8 @@
       <c r="AA119" t="inlineStr"/>
       <c r="AB119" s="3" t="inlineStr"/>
       <c r="AC119" t="inlineStr"/>
+      <c r="AD119" s="3" t="inlineStr"/>
+      <c r="AE119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -11284,7 +11914,13 @@
       <c r="AB120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC120" t="inlineStr">
+      <c r="AC120" t="n">
+        <v>1476</v>
+      </c>
+      <c r="AD120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE120" t="inlineStr">
         <is>
           <t>1476</t>
         </is>
@@ -11355,7 +11991,13 @@
       <c r="AB121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC121" t="inlineStr">
+      <c r="AC121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11422,7 +12064,13 @@
       <c r="AB122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC122" t="inlineStr">
+      <c r="AC122" t="n">
+        <v>2788</v>
+      </c>
+      <c r="AD122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE122" t="inlineStr">
         <is>
           <t>2788</t>
         </is>
@@ -11489,7 +12137,13 @@
       <c r="AB123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC123" t="inlineStr">
+      <c r="AC123" t="n">
+        <v>2606</v>
+      </c>
+      <c r="AD123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE123" t="inlineStr">
         <is>
           <t>2606</t>
         </is>
@@ -11552,7 +12206,13 @@
       <c r="AB124" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC124" t="inlineStr">
+      <c r="AC124" t="n">
+        <v>1444</v>
+      </c>
+      <c r="AD124" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE124" t="inlineStr">
         <is>
           <t>1444</t>
         </is>
@@ -11611,7 +12271,13 @@
       <c r="AB125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC125" t="inlineStr">
+      <c r="AC125" t="n">
+        <v>2584</v>
+      </c>
+      <c r="AD125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE125" t="inlineStr">
         <is>
           <t>2584</t>
         </is>
@@ -11670,7 +12336,13 @@
       <c r="AB126" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="AC126" t="inlineStr">
+      <c r="AC126" t="n">
+        <v>1699</v>
+      </c>
+      <c r="AD126" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE126" t="inlineStr">
         <is>
           <t>1699</t>
         </is>
@@ -11729,7 +12401,13 @@
       <c r="AB127" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="AC127" t="inlineStr">
+      <c r="AC127" t="n">
+        <v>1548</v>
+      </c>
+      <c r="AD127" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE127" t="inlineStr">
         <is>
           <t>1548</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-04-22 11:30:52
</commit_message>
<xml_diff>
--- a/Season_Attack/88.xlsx
+++ b/Season_Attack/88.xlsx
@@ -909,7 +909,7 @@
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>4393</t>
+          <t>4481</t>
         </is>
       </c>
     </row>
@@ -1012,7 +1012,7 @@
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>2536</t>
+          <t>2534</t>
         </is>
       </c>
     </row>
@@ -1110,12 +1110,12 @@
       <c r="AC7" t="n">
         <v>5616</v>
       </c>
-      <c r="AD7" s="3" t="n">
-        <v>23</v>
+      <c r="AD7" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>5616</t>
+          <t>5625</t>
         </is>
       </c>
     </row>
@@ -1271,11 +1271,11 @@
         <v>3747</v>
       </c>
       <c r="AD9" s="4" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>3747</t>
+          <t>3967</t>
         </is>
       </c>
     </row>
@@ -1683,11 +1683,11 @@
         <v>4104</v>
       </c>
       <c r="AD13" s="4" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="AE13" t="inlineStr">
         <is>
-          <t>4104</t>
+          <t>4110</t>
         </is>
       </c>
     </row>
@@ -1785,12 +1785,12 @@
       <c r="AC14" t="n">
         <v>2812</v>
       </c>
-      <c r="AD14" s="4" t="n">
-        <v>2</v>
+      <c r="AD14" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE14" t="inlineStr">
         <is>
-          <t>2812</t>
+          <t>2844</t>
         </is>
       </c>
     </row>
@@ -1888,12 +1888,12 @@
       <c r="AC15" t="n">
         <v>4425</v>
       </c>
-      <c r="AD15" s="2" t="n">
-        <v>0</v>
+      <c r="AD15" s="3" t="n">
+        <v>24</v>
       </c>
       <c r="AE15" t="inlineStr">
         <is>
-          <t>4425</t>
+          <t>4616</t>
         </is>
       </c>
     </row>
@@ -2077,7 +2077,7 @@
       </c>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>5228</t>
+          <t>5294</t>
         </is>
       </c>
     </row>
@@ -2180,7 +2180,7 @@
       </c>
       <c r="AE18" t="inlineStr">
         <is>
-          <t>5195</t>
+          <t>5365</t>
         </is>
       </c>
     </row>
@@ -2283,7 +2283,7 @@
       </c>
       <c r="AE19" t="inlineStr">
         <is>
-          <t>6064</t>
+          <t>6302</t>
         </is>
       </c>
     </row>
@@ -2382,11 +2382,11 @@
         <v>5284</v>
       </c>
       <c r="AD20" s="5" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>5284</t>
+          <t>5409</t>
         </is>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="AE21" t="inlineStr">
         <is>
-          <t>5860</t>
+          <t>6047</t>
         </is>
       </c>
     </row>
@@ -2587,12 +2587,12 @@
       <c r="AC22" t="n">
         <v>4118</v>
       </c>
-      <c r="AD22" s="4" t="n">
-        <v>8</v>
+      <c r="AD22" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>4118</t>
+          <t>4162</t>
         </is>
       </c>
     </row>
@@ -2690,8 +2690,8 @@
       <c r="AC23" t="n">
         <v>4909</v>
       </c>
-      <c r="AD23" s="3" t="n">
-        <v>20</v>
+      <c r="AD23" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
@@ -2982,7 +2982,7 @@
       </c>
       <c r="AE26" t="inlineStr">
         <is>
-          <t>5241</t>
+          <t>5398</t>
         </is>
       </c>
     </row>
@@ -3081,11 +3081,11 @@
         <v>4329</v>
       </c>
       <c r="AD27" s="3" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AE27" t="inlineStr">
         <is>
-          <t>4329</t>
+          <t>4636</t>
         </is>
       </c>
     </row>
@@ -3291,7 +3291,7 @@
       </c>
       <c r="AE29" t="inlineStr">
         <is>
-          <t>5072</t>
+          <t>5254</t>
         </is>
       </c>
     </row>
@@ -3394,7 +3394,7 @@
       </c>
       <c r="AE30" t="inlineStr">
         <is>
-          <t>3924</t>
+          <t>4304</t>
         </is>
       </c>
     </row>
@@ -3497,7 +3497,7 @@
       </c>
       <c r="AE31" t="inlineStr">
         <is>
-          <t>4930</t>
+          <t>5099</t>
         </is>
       </c>
     </row>
@@ -3600,7 +3600,7 @@
       </c>
       <c r="AE32" t="inlineStr">
         <is>
-          <t>4652</t>
+          <t>4694</t>
         </is>
       </c>
     </row>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="AE34" t="inlineStr">
         <is>
-          <t>2712</t>
+          <t>2733</t>
         </is>
       </c>
     </row>
@@ -3883,11 +3883,11 @@
         <v>4549</v>
       </c>
       <c r="AD35" s="4" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AE35" t="inlineStr">
         <is>
-          <t>4549</t>
+          <t>4576</t>
         </is>
       </c>
     </row>
@@ -3990,7 +3990,7 @@
       </c>
       <c r="AE36" t="inlineStr">
         <is>
-          <t>3420</t>
+          <t>3527</t>
         </is>
       </c>
     </row>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="AE37" t="inlineStr">
         <is>
-          <t>5656</t>
+          <t>5840</t>
         </is>
       </c>
     </row>
@@ -4196,7 +4196,7 @@
       </c>
       <c r="AE38" t="inlineStr">
         <is>
-          <t>4081</t>
+          <t>4193</t>
         </is>
       </c>
     </row>
@@ -4295,11 +4295,11 @@
         <v>3886</v>
       </c>
       <c r="AD39" s="4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AE39" t="inlineStr">
         <is>
-          <t>3886</t>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -4398,11 +4398,11 @@
         <v>5704</v>
       </c>
       <c r="AD40" s="5" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="AE40" t="inlineStr">
         <is>
-          <t>5704</t>
+          <t>5956</t>
         </is>
       </c>
     </row>
@@ -4505,7 +4505,7 @@
       </c>
       <c r="AE41" t="inlineStr">
         <is>
-          <t>5463</t>
+          <t>5651</t>
         </is>
       </c>
     </row>
@@ -4608,7 +4608,7 @@
       </c>
       <c r="AE42" t="inlineStr">
         <is>
-          <t>4996</t>
+          <t>5088</t>
         </is>
       </c>
     </row>
@@ -4711,7 +4711,7 @@
       </c>
       <c r="AE43" t="inlineStr">
         <is>
-          <t>5182</t>
+          <t>5308</t>
         </is>
       </c>
     </row>
@@ -4809,12 +4809,12 @@
       <c r="AC44" t="n">
         <v>5019</v>
       </c>
-      <c r="AD44" s="3" t="n">
-        <v>20</v>
+      <c r="AD44" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE44" t="inlineStr">
         <is>
-          <t>5019</t>
+          <t>5017</t>
         </is>
       </c>
     </row>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="AE45" t="inlineStr">
         <is>
-          <t>5132</t>
+          <t>5283</t>
         </is>
       </c>
     </row>
@@ -5020,7 +5020,7 @@
       </c>
       <c r="AE46" t="inlineStr">
         <is>
-          <t>4931</t>
+          <t>5035</t>
         </is>
       </c>
     </row>
@@ -5123,7 +5123,7 @@
       </c>
       <c r="AE47" t="inlineStr">
         <is>
-          <t>4805</t>
+          <t>4921</t>
         </is>
       </c>
     </row>
@@ -5226,7 +5226,7 @@
       </c>
       <c r="AE48" t="inlineStr">
         <is>
-          <t>5300</t>
+          <t>5512</t>
         </is>
       </c>
     </row>
@@ -5325,11 +5325,11 @@
         <v>4394</v>
       </c>
       <c r="AD49" s="4" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="AE49" t="inlineStr">
         <is>
-          <t>4394</t>
+          <t>4384</t>
         </is>
       </c>
     </row>
@@ -5484,12 +5484,12 @@
       <c r="AC51" t="n">
         <v>4312</v>
       </c>
-      <c r="AD51" s="2" t="n">
-        <v>0</v>
+      <c r="AD51" s="4" t="n">
+        <v>8</v>
       </c>
       <c r="AE51" t="inlineStr">
         <is>
-          <t>4312</t>
+          <t>4470</t>
         </is>
       </c>
     </row>
@@ -5592,7 +5592,7 @@
       </c>
       <c r="AE52" t="inlineStr">
         <is>
-          <t>4344</t>
+          <t>4448</t>
         </is>
       </c>
     </row>
@@ -5691,11 +5691,11 @@
         <v>4473</v>
       </c>
       <c r="AD53" s="3" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AE53" t="inlineStr">
         <is>
-          <t>4473</t>
+          <t>4491</t>
         </is>
       </c>
     </row>
@@ -5793,12 +5793,12 @@
       <c r="AC54" t="n">
         <v>4155</v>
       </c>
-      <c r="AD54" s="3" t="n">
-        <v>30</v>
+      <c r="AD54" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE54" t="inlineStr">
         <is>
-          <t>4155</t>
+          <t>4052</t>
         </is>
       </c>
     </row>
@@ -5901,7 +5901,7 @@
       </c>
       <c r="AE55" t="inlineStr">
         <is>
-          <t>4149</t>
+          <t>4138</t>
         </is>
       </c>
     </row>
@@ -6000,11 +6000,11 @@
         <v>4169</v>
       </c>
       <c r="AD56" s="3" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AE56" t="inlineStr">
         <is>
-          <t>4169</t>
+          <t>4192</t>
         </is>
       </c>
     </row>
@@ -6102,12 +6102,12 @@
       <c r="AC57" t="n">
         <v>4397</v>
       </c>
-      <c r="AD57" s="3" t="n">
-        <v>20</v>
+      <c r="AD57" s="4" t="n">
+        <v>8</v>
       </c>
       <c r="AE57" t="inlineStr">
         <is>
-          <t>4397</t>
+          <t>4494</t>
         </is>
       </c>
     </row>
@@ -6313,7 +6313,7 @@
       </c>
       <c r="AE59" t="inlineStr">
         <is>
-          <t>2887</t>
+          <t>2933</t>
         </is>
       </c>
     </row>
@@ -6416,7 +6416,7 @@
       </c>
       <c r="AE60" t="inlineStr">
         <is>
-          <t>2460</t>
+          <t>2490</t>
         </is>
       </c>
     </row>
@@ -6514,12 +6514,12 @@
       <c r="AC61" t="n">
         <v>4354</v>
       </c>
-      <c r="AD61" s="3" t="n">
-        <v>21</v>
+      <c r="AD61" s="4" t="n">
+        <v>2</v>
       </c>
       <c r="AE61" t="inlineStr">
         <is>
-          <t>4354</t>
+          <t>4406</t>
         </is>
       </c>
     </row>
@@ -6622,7 +6622,7 @@
       </c>
       <c r="AE62" t="inlineStr">
         <is>
-          <t>1975</t>
+          <t>1972</t>
         </is>
       </c>
     </row>
@@ -7022,12 +7022,12 @@
       <c r="AC67" t="n">
         <v>5448</v>
       </c>
-      <c r="AD67" s="5" t="n">
-        <v>32</v>
+      <c r="AD67" s="3" t="n">
+        <v>22</v>
       </c>
       <c r="AE67" t="inlineStr">
         <is>
-          <t>5448</t>
+          <t>5527</t>
         </is>
       </c>
     </row>
@@ -7434,12 +7434,12 @@
       <c r="AC71" t="n">
         <v>4537</v>
       </c>
-      <c r="AD71" s="4" t="n">
-        <v>7</v>
+      <c r="AD71" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE71" t="inlineStr">
         <is>
-          <t>4537</t>
+          <t>4602</t>
         </is>
       </c>
     </row>
@@ -7542,7 +7542,7 @@
       </c>
       <c r="AE72" t="inlineStr">
         <is>
-          <t>3316</t>
+          <t>3358</t>
         </is>
       </c>
     </row>
@@ -7748,7 +7748,7 @@
       </c>
       <c r="AE74" t="inlineStr">
         <is>
-          <t>1227</t>
+          <t>1226</t>
         </is>
       </c>
     </row>
@@ -8015,7 +8015,7 @@
       </c>
       <c r="AE77" t="inlineStr">
         <is>
-          <t>3067</t>
+          <t>3081</t>
         </is>
       </c>
     </row>
@@ -8324,7 +8324,7 @@
       </c>
       <c r="AE80" t="inlineStr">
         <is>
-          <t>1486</t>
+          <t>1497</t>
         </is>
       </c>
     </row>
@@ -9148,7 +9148,7 @@
       </c>
       <c r="AE88" t="inlineStr">
         <is>
-          <t>2738</t>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -9633,7 +9633,7 @@
       </c>
       <c r="AE93" t="inlineStr">
         <is>
-          <t>3736</t>
+          <t>3723</t>
         </is>
       </c>
     </row>
@@ -11403,7 +11403,7 @@
       </c>
       <c r="AE113" t="inlineStr">
         <is>
-          <t>2925</t>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -11581,7 +11581,7 @@
       </c>
       <c r="AE115" t="inlineStr">
         <is>
-          <t>5483</t>
+          <t>5630</t>
         </is>
       </c>
     </row>
@@ -11670,7 +11670,7 @@
       </c>
       <c r="AE116" t="inlineStr">
         <is>
-          <t>3816</t>
+          <t>3939</t>
         </is>
       </c>
     </row>
@@ -11793,12 +11793,12 @@
       <c r="AC118" t="n">
         <v>2883</v>
       </c>
-      <c r="AD118" s="4" t="n">
-        <v>16</v>
+      <c r="AD118" s="3" t="n">
+        <v>20</v>
       </c>
       <c r="AE118" t="inlineStr">
         <is>
-          <t>2883</t>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -11922,7 +11922,7 @@
       </c>
       <c r="AE120" t="inlineStr">
         <is>
-          <t>1476</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12072,7 +12072,7 @@
       </c>
       <c r="AE122" t="inlineStr">
         <is>
-          <t>2788</t>
+          <t>2849</t>
         </is>
       </c>
     </row>
@@ -12145,7 +12145,7 @@
       </c>
       <c r="AE123" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -12214,7 +12214,7 @@
       </c>
       <c r="AE124" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>1457</t>
         </is>
       </c>
     </row>
@@ -12339,12 +12339,12 @@
       <c r="AC126" t="n">
         <v>1699</v>
       </c>
-      <c r="AD126" s="4" t="n">
-        <v>1</v>
+      <c r="AD126" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AE126" t="inlineStr">
         <is>
-          <t>1699</t>
+          <t>1700</t>
         </is>
       </c>
     </row>
@@ -12405,11 +12405,11 @@
         <v>1548</v>
       </c>
       <c r="AD127" s="4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AE127" t="inlineStr">
         <is>
-          <t>1548</t>
+          <t>1602</t>
         </is>
       </c>
     </row>

</xml_diff>